<commit_message>
Updated data from update search 11/25/24
</commit_message>
<xml_diff>
--- a/data/4dsw_all_citations.xlsx
+++ b/data/4dsw_all_citations.xlsx
@@ -9980,7 +9980,7 @@
       </c>
       <c r="B993" s="0" t="inlineStr">
         <is>
-          <t> (1927). Rural School Supervision: Abstracts of Addresses Delivered at the Second Conference of Supervisors of the Southeastern States Held at Raleigh, North Carolina, December 6 and 7, 1926. Bulletin, 1927, No. 24 Bureau of Education, Department of the Interior, (), 1. </t>
+          <t>Department of the Interior Bureau of Education (1927). Rural School Supervision: Abstracts of Addresses Delivered at the Second Conference of Supervisors of the Southeastern States Held at Raleigh, North Carolina, December 6 and 7, 1926. Bulletin, 1927, No. 24 Bureau of Education, Department of the Interior, (), 1. </t>
         </is>
       </c>
     </row>
@@ -28210,7 +28210,7 @@
       </c>
       <c r="B2816" s="0" t="inlineStr">
         <is>
-          <t> (2023/09/25/). We need a four-day workweek, now – The Vermont Cynic University Wire, (), . </t>
+          <t>Martineau, Lucas (2023/09/25/). We need a four-day workweek, now – The Vermont Cynic University Wire, (), . </t>
         </is>
       </c>
     </row>
@@ -37926,3181 +37926,4261 @@
     </row>
     <row r="3788" spans="1:2">
       <c r="A3788" s="0">
-        <v>4154</v>
+        <v>4157</v>
       </c>
       <c r="B3788" s="0" t="inlineStr">
         <is>
-          <t>Nowak, Adam, Perrone, Frank, Smith, Patrick S. (2023). How Do Homeowners, Teachers, and Students Respond to a Four-Day School Week? Teachers, and Students Respond to a Four-Day School Week, (), . </t>
+          <t>Johnston, G. (2023). Slaton ISD approves 4-day school week KLBK| KAMC| EverythingLubbock. Com, (), . </t>
         </is>
       </c>
     </row>
     <row r="3789" spans="1:2">
       <c r="A3789" s="0">
-        <v>4157</v>
+        <v>4160</v>
       </c>
       <c r="B3789" s="0" t="inlineStr">
         <is>
-          <t>Johnston, G. (2023). Slaton ISD approves 4-day school week KLBK| KAMC| EverythingLubbock. Com, (), . </t>
+          <t>Bacher-Hicks, Andrew, Musaddiq, Tareena, Goodman, Joshua, Stange, Kevin (2024). The stickiness of pandemic-driven disenrollment from public schools , 100(), 102527. https://doi.org/10.1016/j.econedurev.2024.102527</t>
         </is>
       </c>
     </row>
     <row r="3790" spans="1:2">
       <c r="A3790" s="0">
-        <v>4160</v>
+        <v>4163</v>
       </c>
       <c r="B3790" s="0" t="inlineStr">
         <is>
-          <t>Bacher-Hicks, Andrew, Musaddiq, Tareena, Goodman, Joshua, Stange, Kevin (2024). The stickiness of pandemic-driven disenrollment from public schools , 100(), 102527. https://doi.org/10.1016/j.econedurev.2024.102527</t>
+          <t>Kroupova, Katerina, Havranek, Tomas, Irsova, Zuzana (2024). Student Employment and Education: A Meta-Analysis , 100(), 102539. https://doi.org/10.1016/j.econedurev.2024.102539</t>
         </is>
       </c>
     </row>
     <row r="3791" spans="1:2">
       <c r="A3791" s="0">
-        <v>4163</v>
+        <v>4164</v>
       </c>
       <c r="B3791" s="0" t="inlineStr">
         <is>
-          <t>Kroupova, Katerina, Havranek, Tomas, Irsova, Zuzana (2024). Student Employment and Education: A Meta-Analysis , 100(), 102539. https://doi.org/10.1016/j.econedurev.2024.102539</t>
+          <t> (2024). Editorial Board , 100(), 102551. https://doi.org/10.1016/S0272-7757(24)00045-1</t>
         </is>
       </c>
     </row>
     <row r="3792" spans="1:2">
       <c r="A3792" s="0">
-        <v>4164</v>
+        <v>4165</v>
       </c>
       <c r="B3792" s="0" t="inlineStr">
         <is>
-          <t> (2024). Editorial Board , 100(), 102551. https://doi.org/10.1016/S0272-7757(24)00045-1</t>
+          <t>Coelli, Michael, Foster, Gigi (2024). Unintended consequences of school accountability reforms: Public versus private schools , 99(), 102523. https://doi.org/10.1016/j.econedurev.2024.102523</t>
         </is>
       </c>
     </row>
     <row r="3793" spans="1:2">
       <c r="A3793" s="0">
-        <v>4165</v>
+        <v>4172</v>
       </c>
       <c r="B3793" s="0" t="inlineStr">
         <is>
-          <t>Coelli, Michael, Foster, Gigi (2024). Unintended consequences of school accountability reforms: Public versus private schools , 99(), 102523. https://doi.org/10.1016/j.econedurev.2024.102523</t>
+          <t>Ren, Meiqing (2024). Preschool and child health: Evidence from China's universal child care reform , 100(), 102540. https://doi.org/10.1016/j.econedurev.2024.102540</t>
         </is>
       </c>
     </row>
     <row r="3794" spans="1:2">
       <c r="A3794" s="0">
-        <v>4172</v>
+        <v>4179</v>
       </c>
       <c r="B3794" s="0" t="inlineStr">
         <is>
-          <t>Ren, Meiqing (2024). Preschool and child health: Evidence from China's universal child care reform , 100(), 102540. https://doi.org/10.1016/j.econedurev.2024.102540</t>
+          <t>Gallegos, Sebastián, García, Jorge Luis (2024). Childcare and parenting in the production of early life skills , 101(), 102557. https://doi.org/10.1016/j.econedurev.2024.102557</t>
         </is>
       </c>
     </row>
     <row r="3795" spans="1:2">
       <c r="A3795" s="0">
-        <v>4179</v>
+        <v>4181</v>
       </c>
       <c r="B3795" s="0" t="inlineStr">
         <is>
-          <t>Gallegos, Sebastián, García, Jorge Luis (2024). Childcare and parenting in the production of early life skills , 101(), 102557. https://doi.org/10.1016/j.econedurev.2024.102557</t>
+          <t>Lowry, Danielle, Page, Lindsay C., Nurshatayeva, Aizat, Iriti, Jennifer (2024). Subtraction by addition: Do private scholarship awards lead to financial aid displacement? , 99(), 102517. https://doi.org/10.1016/j.econedurev.2024.102517</t>
         </is>
       </c>
     </row>
     <row r="3796" spans="1:2">
       <c r="A3796" s="0">
-        <v>4181</v>
+        <v>4182</v>
       </c>
       <c r="B3796" s="0" t="inlineStr">
         <is>
-          <t>Lowry, Danielle, Page, Lindsay C., Nurshatayeva, Aizat, Iriti, Jennifer (2024). Subtraction by addition: Do private scholarship awards lead to financial aid displacement? , 99(), 102517. https://doi.org/10.1016/j.econedurev.2024.102517</t>
+          <t>Barrios-Fernández, Andrés, Riudavets-Barcons, Marc (2024). Teacher value-added and gender gaps in educational outcomes , 100(), 102541. https://doi.org/10.1016/j.econedurev.2024.102541</t>
         </is>
       </c>
     </row>
     <row r="3797" spans="1:2">
       <c r="A3797" s="0">
-        <v>4182</v>
+        <v>4184</v>
       </c>
       <c r="B3797" s="0" t="inlineStr">
         <is>
-          <t>Barrios-Fernández, Andrés, Riudavets-Barcons, Marc (2024). Teacher value-added and gender gaps in educational outcomes , 100(), 102541. https://doi.org/10.1016/j.econedurev.2024.102541</t>
+          <t>Drange, Nina, Sandsør, Astrid Marie Jorde (2024). The effects of a free universal after-school program on child academic outcomes , 98(), 102504. https://doi.org/10.1016/j.econedurev.2023.102504</t>
         </is>
       </c>
     </row>
     <row r="3798" spans="1:2">
       <c r="A3798" s="0">
-        <v>4184</v>
+        <v>4188</v>
       </c>
       <c r="B3798" s="0" t="inlineStr">
         <is>
-          <t>Drange, Nina, Sandsør, Astrid Marie Jorde (2024). The effects of a free universal after-school program on child academic outcomes , 98(), 102504. https://doi.org/10.1016/j.econedurev.2023.102504</t>
+          <t>Aggarwal, Khushboo, Barua, Rashmi, Vidal-Fernandez, Marian (2024). Still Waters Run Deep: Groundwater Contamination and Education Outcomes in India , 100(), 102525. https://doi.org/10.1016/j.econedurev.2024.102525</t>
         </is>
       </c>
     </row>
     <row r="3799" spans="1:2">
       <c r="A3799" s="0">
-        <v>4188</v>
+        <v>4194</v>
       </c>
       <c r="B3799" s="0" t="inlineStr">
         <is>
-          <t>Aggarwal, Khushboo, Barua, Rashmi, Vidal-Fernandez, Marian (2024). Still Waters Run Deep: Groundwater Contamination and Education Outcomes in India , 100(), 102525. https://doi.org/10.1016/j.econedurev.2024.102525</t>
+          <t>Bolhaar, Jonneke, Kuijpers, Sonny, Webbink, Dinand, Zumbuehl, Maria (2024). Does replacing grants by income-contingent loans harm enrolment? New evidence from a reform in Dutch higher education , 101(), 102546. https://doi.org/10.1016/j.econedurev.2024.102546</t>
         </is>
       </c>
     </row>
     <row r="3800" spans="1:2">
       <c r="A3800" s="0">
-        <v>4194</v>
+        <v>4195</v>
       </c>
       <c r="B3800" s="0" t="inlineStr">
         <is>
-          <t>Bolhaar, Jonneke, Kuijpers, Sonny, Webbink, Dinand, Zumbuehl, Maria (2024). Does replacing grants by income-contingent loans harm enrolment? New evidence from a reform in Dutch higher education , 101(), 102546. https://doi.org/10.1016/j.econedurev.2024.102546</t>
+          <t>de Hoyos, Rafael, Djaker, Sharnic, Ganimian, Alejandro J., Holland, Peter A. (2024). The impact of combining performance-management tools and training with diagnostic feedback in public schools: Experimental evidence from Argentina , 99(), 102518. https://doi.org/10.1016/j.econedurev.2024.102518</t>
         </is>
       </c>
     </row>
     <row r="3801" spans="1:2">
       <c r="A3801" s="0">
-        <v>4195</v>
+        <v>4196</v>
       </c>
       <c r="B3801" s="0" t="inlineStr">
         <is>
-          <t>de Hoyos, Rafael, Djaker, Sharnic, Ganimian, Alejandro J., Holland, Peter A. (2024). The impact of combining performance-management tools and training with diagnostic feedback in public schools: Experimental evidence from Argentina , 99(), 102518. https://doi.org/10.1016/j.econedurev.2024.102518</t>
+          <t>Luflade, Margaux, Zaiem, Meryam (2024). Do elite schools improve students performance? Evidence from Tunisia , 100(), 102542. https://doi.org/10.1016/j.econedurev.2024.102542</t>
         </is>
       </c>
     </row>
     <row r="3802" spans="1:2">
       <c r="A3802" s="0">
-        <v>4196</v>
+        <v>4197</v>
       </c>
       <c r="B3802" s="0" t="inlineStr">
         <is>
-          <t>Luflade, Margaux, Zaiem, Meryam (2024). Do elite schools improve students performance? Evidence from Tunisia , 100(), 102542. https://doi.org/10.1016/j.econedurev.2024.102542</t>
+          <t>Caetano, Carolina, Caetano, Gregorio, Nielsen, Eric (2024). Are children spending too much time on enrichment activities? , 98(), 102503. https://doi.org/10.1016/j.econedurev.2023.102503</t>
         </is>
       </c>
     </row>
     <row r="3803" spans="1:2">
       <c r="A3803" s="0">
-        <v>4197</v>
+        <v>4199</v>
       </c>
       <c r="B3803" s="0" t="inlineStr">
         <is>
-          <t>Caetano, Carolina, Caetano, Gregorio, Nielsen, Eric (2024). Are children spending too much time on enrichment activities? , 98(), 102503. https://doi.org/10.1016/j.econedurev.2023.102503</t>
+          <t> (2024). Editorial Board , 98(), 102514. https://doi.org/10.1016/S0272-7757(24)00008-6</t>
         </is>
       </c>
     </row>
     <row r="3804" spans="1:2">
       <c r="A3804" s="0">
-        <v>4199</v>
+        <v>4204</v>
       </c>
       <c r="B3804" s="0" t="inlineStr">
         <is>
-          <t> (2024). Editorial Board , 98(), 102514. https://doi.org/10.1016/S0272-7757(24)00008-6</t>
+          <t>Grobon, Sébastien, Wolff, François-Charles (2024). Do public scholarships crowd out parental transfers? Evidence at the intensive margin from France , 98(), 102502. https://doi.org/10.1016/j.econedurev.2023.102502</t>
         </is>
       </c>
     </row>
     <row r="3805" spans="1:2">
       <c r="A3805" s="0">
-        <v>4204</v>
+        <v>4207</v>
       </c>
       <c r="B3805" s="0" t="inlineStr">
         <is>
-          <t>Grobon, Sébastien, Wolff, François-Charles (2024). Do public scholarships crowd out parental transfers? Evidence at the intensive margin from France , 98(), 102502. https://doi.org/10.1016/j.econedurev.2023.102502</t>
+          <t>Sessou, Fidele Eric, Hidrobo, Melissa, Roy, Shalini, Huybregts, Lieven (2024). Educational impacts of an unconditional cash transfer program in Mali , 101(), 102547. https://doi.org/10.1016/j.econedurev.2024.102547</t>
         </is>
       </c>
     </row>
     <row r="3806" spans="1:2">
       <c r="A3806" s="0">
-        <v>4207</v>
+        <v>4208</v>
       </c>
       <c r="B3806" s="0" t="inlineStr">
         <is>
-          <t>Sessou, Fidele Eric, Hidrobo, Melissa, Roy, Shalini, Huybregts, Lieven (2024). Educational impacts of an unconditional cash transfer program in Mali , 101(), 102547. https://doi.org/10.1016/j.econedurev.2024.102547</t>
+          <t> (2023). Editorial Board , 95(), 102448. https://doi.org/10.1016/S0272-7757(23)00095-X</t>
         </is>
       </c>
     </row>
     <row r="3807" spans="1:2">
       <c r="A3807" s="0">
-        <v>4208</v>
+        <v>4209</v>
       </c>
       <c r="B3807" s="0" t="inlineStr">
         <is>
-          <t> (2023). Editorial Board , 95(), 102448. https://doi.org/10.1016/S0272-7757(23)00095-X</t>
+          <t>Bhardwaj, Sakshi, Shonchoy, Abu S. (2024). Social identity and learning: Adult literacy program in India , 99(), 102507. https://doi.org/10.1016/j.econedurev.2024.102507</t>
         </is>
       </c>
     </row>
     <row r="3808" spans="1:2">
       <c r="A3808" s="0">
-        <v>4209</v>
+        <v>4212</v>
       </c>
       <c r="B3808" s="0" t="inlineStr">
         <is>
-          <t>Bhardwaj, Sakshi, Shonchoy, Abu S. (2024). Social identity and learning: Adult literacy program in India , 99(), 102507. https://doi.org/10.1016/j.econedurev.2024.102507</t>
+          <t>Lopez, Jennifer, Behrman, Jere, Cueto, Santiago, Favara, Marta, Sánchez, Alan (2024). Late-childhood foundational cognitive skills predict educational outcomes through adolescence and into young adulthood: Evidence from Ethiopia and Peru , 100(), 102543. https://doi.org/10.1016/j.econedurev.2024.102543</t>
         </is>
       </c>
     </row>
     <row r="3809" spans="1:2">
       <c r="A3809" s="0">
-        <v>4212</v>
+        <v>4216</v>
       </c>
       <c r="B3809" s="0" t="inlineStr">
         <is>
-          <t>Lopez, Jennifer, Behrman, Jere, Cueto, Santiago, Favara, Marta, Sánchez, Alan (2024). Late-childhood foundational cognitive skills predict educational outcomes through adolescence and into young adulthood: Evidence from Ethiopia and Peru , 100(), 102543. https://doi.org/10.1016/j.econedurev.2024.102543</t>
+          <t>Ng, Kevin (2024). The effects of teacher tenure on productivity and selection , 101(), 102558. https://doi.org/10.1016/j.econedurev.2024.102558</t>
         </is>
       </c>
     </row>
     <row r="3810" spans="1:2">
       <c r="A3810" s="0">
-        <v>4216</v>
+        <v>4218</v>
       </c>
       <c r="B3810" s="0" t="inlineStr">
         <is>
-          <t>Ng, Kevin (2024). The effects of teacher tenure on productivity and selection , 101(), 102558. https://doi.org/10.1016/j.econedurev.2024.102558</t>
+          <t>Oliveira, Rodrigo, Santos, Alei, Severnini, Edson (2024). Bridging the gap: Mismatch effects and catch-up dynamics under a Brazilian college affirmative action program , 98(), 102501. https://doi.org/10.1016/j.econedurev.2023.102501</t>
         </is>
       </c>
     </row>
     <row r="3811" spans="1:2">
       <c r="A3811" s="0">
-        <v>4218</v>
+        <v>4221</v>
       </c>
       <c r="B3811" s="0" t="inlineStr">
         <is>
-          <t>Oliveira, Rodrigo, Santos, Alei, Severnini, Edson (2024). Bridging the gap: Mismatch effects and catch-up dynamics under a Brazilian college affirmative action program , 98(), 102501. https://doi.org/10.1016/j.econedurev.2023.102501</t>
+          <t>Tobin, Zachary (2024). How do public schools respond to competition? Evidence from a charter school expansion , 99(), 102519. https://doi.org/10.1016/j.econedurev.2024.102519</t>
         </is>
       </c>
     </row>
     <row r="3812" spans="1:2">
       <c r="A3812" s="0">
-        <v>4221</v>
+        <v>4222</v>
       </c>
       <c r="B3812" s="0" t="inlineStr">
         <is>
-          <t>Tobin, Zachary (2024). How do public schools respond to competition? Evidence from a charter school expansion , 99(), 102519. https://doi.org/10.1016/j.econedurev.2024.102519</t>
+          <t>Skinner, Benjamin T., Doyle, William R. (2024). Predicting postsecondary attendance by family income in the United States using multilevel regression with poststratification , 99(), 102508. https://doi.org/10.1016/j.econedurev.2024.102508</t>
         </is>
       </c>
     </row>
     <row r="3813" spans="1:2">
       <c r="A3813" s="0">
-        <v>4222</v>
+        <v>4223</v>
       </c>
       <c r="B3813" s="0" t="inlineStr">
         <is>
-          <t>Skinner, Benjamin T., Doyle, William R. (2024). Predicting postsecondary attendance by family income in the United States using multilevel regression with poststratification , 99(), 102508. https://doi.org/10.1016/j.econedurev.2024.102508</t>
+          <t>Hill, Andrew J., LoPalo, Melissa (2024). The effects of online vs in-class testing in moderate-stakes college environments , 98(), 102505. https://doi.org/10.1016/j.econedurev.2023.102505</t>
         </is>
       </c>
     </row>
     <row r="3814" spans="1:2">
       <c r="A3814" s="0">
-        <v>4223</v>
+        <v>4226</v>
       </c>
       <c r="B3814" s="0" t="inlineStr">
         <is>
-          <t>Hill, Andrew J., LoPalo, Melissa (2024). The effects of online vs in-class testing in moderate-stakes college environments , 98(), 102505. https://doi.org/10.1016/j.econedurev.2023.102505</t>
+          <t>Chen, Feng, Harris, Douglas N., Penn, Mary (2024). The effects of charter school entry on the supply of teachers from university-based education programs , 99(), 102520. https://doi.org/10.1016/j.econedurev.2024.102520</t>
         </is>
       </c>
     </row>
     <row r="3815" spans="1:2">
       <c r="A3815" s="0">
-        <v>4226</v>
+        <v>4228</v>
       </c>
       <c r="B3815" s="0" t="inlineStr">
         <is>
-          <t>Chen, Feng, Harris, Douglas N., Penn, Mary (2024). The effects of charter school entry on the supply of teachers from university-based education programs , 99(), 102520. https://doi.org/10.1016/j.econedurev.2024.102520</t>
+          <t>Ercolani, Marco G., Lazarova, Emiliya (2024). The UK Disability Discrimination Act 2005: Consequences for the education and employment of older children , 100(), 102544. https://doi.org/10.1016/j.econedurev.2024.102544</t>
         </is>
       </c>
     </row>
     <row r="3816" spans="1:2">
       <c r="A3816" s="0">
-        <v>4228</v>
+        <v>4234</v>
       </c>
       <c r="B3816" s="0" t="inlineStr">
         <is>
-          <t>Ercolani, Marco G., Lazarova, Emiliya (2024). The UK Disability Discrimination Act 2005: Consequences for the education and employment of older children , 100(), 102544. https://doi.org/10.1016/j.econedurev.2024.102544</t>
+          <t>Hall, Caroline, Lundin, Martin (2024). Technology in the classroom: Personal computers and learning outcomes in primary school , 100(), 102536. https://doi.org/10.1016/j.econedurev.2024.102536</t>
         </is>
       </c>
     </row>
     <row r="3817" spans="1:2">
       <c r="A3817" s="0">
-        <v>4234</v>
+        <v>4236</v>
       </c>
       <c r="B3817" s="0" t="inlineStr">
         <is>
-          <t>Hall, Caroline, Lundin, Martin (2024). Technology in the classroom: Personal computers and learning outcomes in primary school , 100(), 102536. https://doi.org/10.1016/j.econedurev.2024.102536</t>
+          <t>Najam, Rafiuddin (2024). Closing the gap: Effect of a gender quota on women’s access to education in Afghanistan , 99(), 102509. https://doi.org/10.1016/j.econedurev.2024.102509</t>
         </is>
       </c>
     </row>
     <row r="3818" spans="1:2">
       <c r="A3818" s="0">
-        <v>4236</v>
+        <v>4238</v>
       </c>
       <c r="B3818" s="0" t="inlineStr">
         <is>
-          <t>Najam, Rafiuddin (2024). Closing the gap: Effect of a gender quota on women’s access to education in Afghanistan , 99(), 102509. https://doi.org/10.1016/j.econedurev.2024.102509</t>
+          <t>Inoue, Atsushi, Tanaka, Ryuichi (2024). The rank of socioeconomic status within a class and the incidence of school bullying and school absence , 101(), 102545. https://doi.org/10.1016/j.econedurev.2024.102545</t>
         </is>
       </c>
     </row>
     <row r="3819" spans="1:2">
       <c r="A3819" s="0">
-        <v>4238</v>
+        <v>4241</v>
       </c>
       <c r="B3819" s="0" t="inlineStr">
         <is>
-          <t>Inoue, Atsushi, Tanaka, Ryuichi (2024). The rank of socioeconomic status within a class and the incidence of school bullying and school absence , 101(), 102545. https://doi.org/10.1016/j.econedurev.2024.102545</t>
+          <t>Aker, Jenny C., Sawyer, Melita, Berry, James (2024). Making sense of the shapes: What do we know about literacy learning in adulthood? , 100(), 102537. https://doi.org/10.1016/j.econedurev.2024.102537</t>
         </is>
       </c>
     </row>
     <row r="3820" spans="1:2">
       <c r="A3820" s="0">
-        <v>4241</v>
+        <v>4243</v>
       </c>
       <c r="B3820" s="0" t="inlineStr">
         <is>
-          <t>Aker, Jenny C., Sawyer, Melita, Berry, James (2024). Making sense of the shapes: What do we know about literacy learning in adulthood? , 100(), 102537. https://doi.org/10.1016/j.econedurev.2024.102537</t>
+          <t>Boring, Anne, Brown, Jennifer (2024). Gender and choices in higher education , 99(), 102521. https://doi.org/10.1016/j.econedurev.2024.102521</t>
         </is>
       </c>
     </row>
     <row r="3821" spans="1:2">
       <c r="A3821" s="0">
-        <v>4243</v>
+        <v>4246</v>
       </c>
       <c r="B3821" s="0" t="inlineStr">
         <is>
-          <t>Boring, Anne, Brown, Jennifer (2024). Gender and choices in higher education , 99(), 102521. https://doi.org/10.1016/j.econedurev.2024.102521</t>
+          <t>Schwerter, Jakob, Netz, Nicolai, Hübner, Nicolas (2024). Does instructional time at school influence study time at university? Evidence from an instructional time reform , 100(), 102526. https://doi.org/10.1016/j.econedurev.2024.102526</t>
         </is>
       </c>
     </row>
     <row r="3822" spans="1:2">
       <c r="A3822" s="0">
-        <v>4246</v>
+        <v>4250</v>
       </c>
       <c r="B3822" s="0" t="inlineStr">
         <is>
-          <t>Schwerter, Jakob, Netz, Nicolai, Hübner, Nicolas (2024). Does instructional time at school influence study time at university? Evidence from an instructional time reform , 100(), 102526. https://doi.org/10.1016/j.econedurev.2024.102526</t>
+          <t>Di Tommaso, Maria Laura, Contini, Dalit, De Rosa, Dalila, Ferrara, Francesca, Piazzalunga, Daniela, Robutti, Ornella (2024). Tackling the gender gap in mathematics with active learning methodologies , 100(), 102538. https://doi.org/10.1016/j.econedurev.2024.102538</t>
         </is>
       </c>
     </row>
     <row r="3823" spans="1:2">
       <c r="A3823" s="0">
-        <v>4250</v>
+        <v>4251</v>
       </c>
       <c r="B3823" s="0" t="inlineStr">
         <is>
-          <t>Di Tommaso, Maria Laura, Contini, Dalit, De Rosa, Dalila, Ferrara, Francesca, Piazzalunga, Daniela, Robutti, Ornella (2024). Tackling the gender gap in mathematics with active learning methodologies , 100(), 102538. https://doi.org/10.1016/j.econedurev.2024.102538</t>
+          <t>Granato, Silvia, Havari, Enkelejda, Mazzarella, Gianluca, Schnepf, Sylke V. (2024). Study abroad programmes and student outcomes: Evidence from Erasmus , 99(), 102510. https://doi.org/10.1016/j.econedurev.2024.102510</t>
         </is>
       </c>
     </row>
     <row r="3824" spans="1:2">
       <c r="A3824" s="0">
-        <v>4251</v>
+        <v>4253</v>
       </c>
       <c r="B3824" s="0" t="inlineStr">
         <is>
-          <t>Granato, Silvia, Havari, Enkelejda, Mazzarella, Gianluca, Schnepf, Sylke V. (2024). Study abroad programmes and student outcomes: Evidence from Erasmus , 99(), 102510. https://doi.org/10.1016/j.econedurev.2024.102510</t>
+          <t>Bonilla-Mejía, Leonardo, Londoño-Ortega, Erika, Henao, María Fernanda (2024). Geographic isolation and learning: Evidence from rural schools in Colombia , 99(), 102522. https://doi.org/10.1016/j.econedurev.2024.102522</t>
         </is>
       </c>
     </row>
     <row r="3825" spans="1:2">
       <c r="A3825" s="0">
-        <v>4253</v>
+        <v>4255</v>
       </c>
       <c r="B3825" s="0" t="inlineStr">
         <is>
-          <t>Bonilla-Mejía, Leonardo, Londoño-Ortega, Erika, Henao, María Fernanda (2024). Geographic isolation and learning: Evidence from rural schools in Colombia , 99(), 102522. https://doi.org/10.1016/j.econedurev.2024.102522</t>
+          <t>Zoido, Pablo, Flores-Ceceña, Iván, Székely, Miguel, Hevia, Felipe J., Castro, Eleno (2024). Remote tutoring with low-tech means to accelerate learning: Evidence for El Salvador , 98(), 102506. https://doi.org/10.1016/j.econedurev.2023.102506</t>
         </is>
       </c>
     </row>
     <row r="3826" spans="1:2">
       <c r="A3826" s="0">
-        <v>4255</v>
+        <v>4262</v>
       </c>
       <c r="B3826" s="0" t="inlineStr">
         <is>
-          <t>Zoido, Pablo, Flores-Ceceña, Iván, Székely, Miguel, Hevia, Felipe J., Castro, Eleno (2024). Remote tutoring with low-tech means to accelerate learning: Evidence for El Salvador , 98(), 102506. https://doi.org/10.1016/j.econedurev.2023.102506</t>
+          <t>Turner, Lesley J.; Gurantz, Oded (2024). Experimental Estimates of College Coaching on Postsecondary Reenrollment Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00430</t>
         </is>
       </c>
     </row>
     <row r="3827" spans="1:2">
       <c r="A3827" s="0">
-        <v>4262</v>
+        <v>4263</v>
       </c>
       <c r="B3827" s="0" t="inlineStr">
         <is>
-          <t>Turner, Lesley J.; Gurantz, Oded (2024). Experimental Estimates of College Coaching on Postsecondary Reenrollment Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00430</t>
+          <t>Grissom, Jason A. (2024). Situating Leadership at the Center of Education Finance and Policy Education Finance and Policy, 19(2), 183. 10.1162/edfp_a_00425</t>
         </is>
       </c>
     </row>
     <row r="3828" spans="1:2">
       <c r="A3828" s="0">
-        <v>4263</v>
+        <v>4266</v>
       </c>
       <c r="B3828" s="0" t="inlineStr">
         <is>
-          <t>Grissom, Jason A. (2024). Situating Leadership at the Center of Education Finance and Policy Education Finance and Policy, 19(2), 183. 10.1162/edfp_a_00425</t>
+          <t>Goss, Jacob; Mangrum, Daniel; Scally, Joelle (2024). Assessing the Relative Progressivity of the Biden Administration's Federal Student Loan Forgiveness Proposal Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00429</t>
         </is>
       </c>
     </row>
     <row r="3829" spans="1:2">
       <c r="A3829" s="0">
-        <v>4266</v>
+        <v>4267</v>
       </c>
       <c r="B3829" s="0" t="inlineStr">
         <is>
-          <t>Goss, Jacob; Mangrum, Daniel; Scally, Joelle (2024). Assessing the Relative Progressivity of the Biden Administration's Federal Student Loan Forgiveness Proposal Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00429</t>
+          <t>Chin, Mark (2024). The Impact of School Desegregation on White Individuals' Racial Attitudes and Politics in Adulthood Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00428</t>
         </is>
       </c>
     </row>
     <row r="3830" spans="1:2">
       <c r="A3830" s="0">
-        <v>4267</v>
+        <v>4271</v>
       </c>
       <c r="B3830" s="0" t="inlineStr">
         <is>
-          <t>Chin, Mark (2024). The Impact of School Desegregation on White Individuals' Racial Attitudes and Politics in Adulthood Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00428</t>
+          <t>Owen, Stephanie (2024). The Advanced Placement Program and Educational Inequality Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00424</t>
         </is>
       </c>
     </row>
     <row r="3831" spans="1:2">
       <c r="A3831" s="0">
-        <v>4271</v>
+        <v>4272</v>
       </c>
       <c r="B3831" s="0" t="inlineStr">
         <is>
-          <t>Owen, Stephanie (2024). The Advanced Placement Program and Educational Inequality Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00424</t>
+          <t>Liu, Vivian Yuen Ting; Zhou, Rachel Yang; Matsudaira, Jordan (2024). Six Years Later: Examining the Academic and Employment Outcomes of the Original and Reinstated Summer Pell Grant Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00423</t>
         </is>
       </c>
     </row>
     <row r="3832" spans="1:2">
       <c r="A3832" s="0">
-        <v>4272</v>
+        <v>4275</v>
       </c>
       <c r="B3832" s="0" t="inlineStr">
         <is>
-          <t>Liu, Vivian Yuen Ting; Zhou, Rachel Yang; Matsudaira, Jordan (2024). Six Years Later: Examining the Academic and Employment Outcomes of the Original and Reinstated Summer Pell Grant Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00423</t>
+          <t>Christian, Alvin; Jacob, Brian; Singleton, John D. (2024). Assessing School District Decision-Making: In-Person Schooling and COVID-19 Transmission Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00433</t>
         </is>
       </c>
     </row>
     <row r="3833" spans="1:2">
       <c r="A3833" s="0">
-        <v>4275</v>
+        <v>4276</v>
       </c>
       <c r="B3833" s="0" t="inlineStr">
         <is>
-          <t>Christian, Alvin; Jacob, Brian; Singleton, John D. (2024). Assessing School District Decision-Making: In-Person Schooling and COVID-19 Transmission Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00433</t>
+          <t>Atwater, Ann; Rush, Mark; Saygin, Perihan (2024). Does Online Testing Make the Grade? Evidence from a Randomized Controlled Trial Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00432</t>
         </is>
       </c>
     </row>
     <row r="3834" spans="1:2">
       <c r="A3834" s="0">
-        <v>4276</v>
+        <v>4278</v>
       </c>
       <c r="B3834" s="0" t="inlineStr">
         <is>
-          <t>Atwater, Ann; Rush, Mark; Saygin, Perihan (2024). Does Online Testing Make the Grade? Evidence from a Randomized Controlled Trial Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00432</t>
+          <t>Goldhaber, Dan; Grout, Cyrus; Wolff, Malcolm (2024). How Well Do Professional Reference Ratings Predict Teacher Performance? Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00421</t>
         </is>
       </c>
     </row>
     <row r="3835" spans="1:2">
       <c r="A3835" s="0">
-        <v>4278</v>
+        <v>4286</v>
       </c>
       <c r="B3835" s="0" t="inlineStr">
         <is>
-          <t>Goldhaber, Dan; Grout, Cyrus; Wolff, Malcolm (2024). How Well Do Professional Reference Ratings Predict Teacher Performance? Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00421</t>
+          <t>Been, Vicki; Ellen, Ingrid; Figlio, David; Nelson, Ashlyn Aiko; Ross, Stephen L.; Schwartz, Amy Ellen; Stiefel, Leanna (2024). The Effects of Housing Price Declines on Children's Educational Outcomes Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00431</t>
         </is>
       </c>
     </row>
     <row r="3836" spans="1:2">
       <c r="A3836" s="0">
-        <v>4286</v>
+        <v>4287</v>
       </c>
       <c r="B3836" s="0" t="inlineStr">
         <is>
-          <t>Been, Vicki; Ellen, Ingrid; Figlio, David; Nelson, Ashlyn Aiko; Ross, Stephen L.; Schwartz, Amy Ellen; Stiefel, Leanna (2024). The Effects of Housing Price Declines on Children's Educational Outcomes Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00431</t>
+          <t>Cordes, Lucy; McEwan, Patrick; Weerapana, Akila (2024). The External Validity of College Remediation Effects: Caveats about Compliers in Fuzzy-discontinuity Designs Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00426</t>
         </is>
       </c>
     </row>
     <row r="3837" spans="1:2">
       <c r="A3837" s="0">
-        <v>4287</v>
+        <v>4289</v>
       </c>
       <c r="B3837" s="0" t="inlineStr">
         <is>
-          <t>Cordes, Lucy; McEwan, Patrick; Weerapana, Akila (2024). The External Validity of College Remediation Effects: Caveats about Compliers in Fuzzy-discontinuity Designs Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00426</t>
+          <t>de Croes, Laurens; Cornelisz, Ilja; van Klaveren, Chris; Ruijs, Nienke (2024). The Effect of Students with Special Needs on Their Peers' Cognitive Outcomes: Results from Student-level Population Data in the Netherlands Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00422</t>
         </is>
       </c>
     </row>
     <row r="3838" spans="1:2">
       <c r="A3838" s="0">
-        <v>4289</v>
+        <v>4292</v>
       </c>
       <c r="B3838" s="0" t="inlineStr">
         <is>
-          <t>de Croes, Laurens; Cornelisz, Ilja; van Klaveren, Chris; Ruijs, Nienke (2024). The Effect of Students with Special Needs on Their Peers' Cognitive Outcomes: Results from Student-level Population Data in the Netherlands Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00422</t>
+          <t>Moschion, Julie; Polidano, Cain (2024). Finding the Right Track: Payoffs to Vocational Education Programs with Workplace Learning Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00427</t>
         </is>
       </c>
     </row>
     <row r="3839" spans="1:2">
       <c r="A3839" s="0">
-        <v>4292</v>
+        <v>4295</v>
       </c>
       <c r="B3839" s="0" t="inlineStr">
         <is>
-          <t>Moschion, Julie; Polidano, Cain (2024). Finding the Right Track: Payoffs to Vocational Education Programs with Workplace Learning Education Finance and Policy, NA(NA), 1. 10.1162/edfp_a_00427</t>
+          <t>Bahgat, Mohamed; Almasri, Zeina; Elsafty, Ashraf; Seddek, Ahmed (2024). Enhancing Team-Based Learning by Moderating FIRST-ADLX Framework inTeacher Professional Development Journal of Education and Training Studies, 12(2), 87. 10.11114/jets.v12i2.6755</t>
         </is>
       </c>
     </row>
     <row r="3840" spans="1:2">
       <c r="A3840" s="0">
-        <v>4295</v>
+        <v>4297</v>
       </c>
       <c r="B3840" s="0" t="inlineStr">
         <is>
-          <t>Bahgat, Mohamed; Almasri, Zeina; Elsafty, Ashraf; Seddek, Ahmed (2024). Enhancing Team-Based Learning by Moderating FIRST-ADLX Framework inTeacher Professional Development Journal of Education and Training Studies, 12(2), 87. 10.11114/jets.v12i2.6755</t>
+          <t>Du, Kuixi; Geiger, Jonathon; Killen, Tommie; Porta, Abril Escobal; O'Brien, Thomas (2024). The Paradigm Shift in Education in Big Data Era: Exploring the Intersection of Historical Assessment Frameworks and AI-Powered Assessment Methods in Education Journal of Education and Training Studies, 12(2), 22. 10.11114/jets.v12i2.6582</t>
         </is>
       </c>
     </row>
     <row r="3841" spans="1:2">
       <c r="A3841" s="0">
-        <v>4297</v>
+        <v>4298</v>
       </c>
       <c r="B3841" s="0" t="inlineStr">
         <is>
-          <t>Du, Kuixi; Geiger, Jonathon; Killen, Tommie; Porta, Abril Escobal; O'Brien, Thomas (2024). The Paradigm Shift in Education in Big Data Era: Exploring the Intersection of Historical Assessment Frameworks and AI-Powered Assessment Methods in Education Journal of Education and Training Studies, 12(2), 22. 10.11114/jets.v12i2.6582</t>
+          <t>Kalaitzi, Christina (2024). A Mathematics Intervention in Kindergarten Using Shel Silverstein's  "The Missing Piece Meets the Big O": Early Childhood Educators' Perceptions on a Teaching Framework Integrating Literature in Mathematics-Related Concepts Journal of Education and Training Studies, 12(2), 75. 10.11114/jets.v12i2.6744</t>
         </is>
       </c>
     </row>
     <row r="3842" spans="1:2">
       <c r="A3842" s="0">
-        <v>4298</v>
+        <v>4299</v>
       </c>
       <c r="B3842" s="0" t="inlineStr">
         <is>
-          <t>Kalaitzi, Christina (2024). A Mathematics Intervention in Kindergarten Using Shel Silverstein's  "The Missing Piece Meets the Big O": Early Childhood Educators' Perceptions on a Teaching Framework Integrating Literature in Mathematics-Related Concepts Journal of Education and Training Studies, 12(2), 75. 10.11114/jets.v12i2.6744</t>
+          <t>Shidler, Linda (2024). Retaining Teachers Through Building Confidence in Collaboration Skills: Promoting 21st-Century Teaching Skills in Teacher Education Journal of Education and Training Studies, 12(2), 1. 10.11114/jets.v12i2.6649</t>
         </is>
       </c>
     </row>
     <row r="3843" spans="1:2">
       <c r="A3843" s="0">
-        <v>4299</v>
+        <v>4300</v>
       </c>
       <c r="B3843" s="0" t="inlineStr">
         <is>
-          <t>Shidler, Linda (2024). Retaining Teachers Through Building Confidence in Collaboration Skills: Promoting 21st-Century Teaching Skills in Teacher Education Journal of Education and Training Studies, 12(2), 1. 10.11114/jets.v12i2.6649</t>
+          <t>Xu, Yonghong Jade; Yang, Mei; Zhang, Shaoan; Muthukumar, Venkatesan (2024). How Constructivist Learning Impacts Secondary Girls' STEM Career Interests Journal of Education and Training Studies, 12(2), 62. 10.11114/jets.v12i2.6793</t>
         </is>
       </c>
     </row>
     <row r="3844" spans="1:2">
       <c r="A3844" s="0">
-        <v>4300</v>
+        <v>4301</v>
       </c>
       <c r="B3844" s="0" t="inlineStr">
         <is>
-          <t>Xu, Yonghong Jade; Yang, Mei; Zhang, Shaoan; Muthukumar, Venkatesan (2024). How Constructivist Learning Impacts Secondary Girls' STEM Career Interests Journal of Education and Training Studies, 12(2), 62. 10.11114/jets.v12i2.6793</t>
+          <t>Cao, Yilin; Li, Shangrong; Shen, Beifei (2024). An Analysis of Holistic Education Models in Mainland China's Higher Education Institutions: A Case Study of College English Curriculum Journal of Education and Training Studies, 12(3), 49. 10.11114/jets.v12i3.6773</t>
         </is>
       </c>
     </row>
     <row r="3845" spans="1:2">
       <c r="A3845" s="0">
-        <v>4301</v>
+        <v>4302</v>
       </c>
       <c r="B3845" s="0" t="inlineStr">
         <is>
-          <t>Cao, Yilin; Li, Shangrong; Shen, Beifei (2024). An Analysis of Holistic Education Models in Mainland China's Higher Education Institutions: A Case Study of College English Curriculum Journal of Education and Training Studies, 12(3), 49. 10.11114/jets.v12i3.6773</t>
+          <t>Choi, Youngae; Hatcher, Wilson J.; Spinrad, Mark (2024). Preschool and Kindergarten Teachers' Self-Reported Phonological Awareness Strategies and Challenges in Teaching English Learners Journal of Education and Training Studies, 12(3), 36. 10.11114/jets.v12i3.6900</t>
         </is>
       </c>
     </row>
     <row r="3846" spans="1:2">
       <c r="A3846" s="0">
-        <v>4302</v>
+        <v>4303</v>
       </c>
       <c r="B3846" s="0" t="inlineStr">
         <is>
-          <t>Choi, Youngae; Hatcher, Wilson J.; Spinrad, Mark (2024). Preschool and Kindergarten Teachers' Self-Reported Phonological Awareness Strategies and Challenges in Teaching English Learners Journal of Education and Training Studies, 12(3), 36. 10.11114/jets.v12i3.6900</t>
+          <t>Cardoso, Fabrício; Braga, Lucianara; Loureiro, Vitor; Bonone, Filipe; Souza, Samuel; Sholl-Franco, Alfred (2024). Neuropsychopedagogical Motor Intervention Program Strengthening Inhibitory Control, Working Memory, and Language Abilities in Post-COVID-19 School Returnees Journal of Education and Training Studies, 12(3), 1. 10.11114/jets.v12i3.6789</t>
         </is>
       </c>
     </row>
     <row r="3847" spans="1:2">
       <c r="A3847" s="0">
-        <v>4303</v>
+        <v>4304</v>
       </c>
       <c r="B3847" s="0" t="inlineStr">
         <is>
-          <t>Cardoso, Fabrício; Braga, Lucianara; Loureiro, Vitor; Bonone, Filipe; Souza, Samuel; Sholl-Franco, Alfred (2024). Neuropsychopedagogical Motor Intervention Program Strengthening Inhibitory Control, Working Memory, and Language Abilities in Post-COVID-19 School Returnees Journal of Education and Training Studies, 12(3), 1. 10.11114/jets.v12i3.6789</t>
+          <t>Huang, Jing; Zhang, Yong (2024). On the Implementation Difficulties of Assessing Course Objective Attainment based on Outcome-Based Education Journal of Education and Training Studies, 12(3), 12. 10.11114/jets.v12i3.6738</t>
         </is>
       </c>
     </row>
     <row r="3848" spans="1:2">
       <c r="A3848" s="0">
-        <v>4304</v>
+        <v>4305</v>
       </c>
       <c r="B3848" s="0" t="inlineStr">
         <is>
-          <t>Huang, Jing; Zhang, Yong (2024). On the Implementation Difficulties of Assessing Course Objective Attainment based on Outcome-Based Education Journal of Education and Training Studies, 12(3), 12. 10.11114/jets.v12i3.6738</t>
+          <t>Zayed, Amal Mohamed (2024). Digital Resilience, Digital Stress, and Social Support as Predictors of Academic Well-Being among University Students Journal of Education and Training Studies, 12(3), 60. 10.11114/jets.v12i3.6894</t>
         </is>
       </c>
     </row>
     <row r="3849" spans="1:2">
       <c r="A3849" s="0">
-        <v>4305</v>
+        <v>4306</v>
       </c>
       <c r="B3849" s="0" t="inlineStr">
         <is>
-          <t>Zayed, Amal Mohamed (2024). Digital Resilience, Digital Stress, and Social Support as Predictors of Academic Well-Being among University Students Journal of Education and Training Studies, 12(3), 60. 10.11114/jets.v12i3.6894</t>
+          <t>Barnes, Jonathan; Ntung, Alex (2023). A School for Humanity: Confronting Division and Trauma Through Lived Values in Burundi Journal of Education and Training Studies, 12(1), 81. 10.11114/jets.v12i1.6424</t>
         </is>
       </c>
     </row>
     <row r="3850" spans="1:2">
       <c r="A3850" s="0">
-        <v>4306</v>
+        <v>4307</v>
       </c>
       <c r="B3850" s="0" t="inlineStr">
         <is>
-          <t>Barnes, Jonathan; Ntung, Alex (2023). A School for Humanity: Confronting Division and Trauma Through Lived Values in Burundi Journal of Education and Training Studies, 12(1), 81. 10.11114/jets.v12i1.6424</t>
+          <t>Mammadov, Maarif; Babayev, Anar; Mukhtarov, Mirsadig (2024). Examining the Psychometric Properties of the Adolescent Students' Basic Psychological Needs at School Scale for the Azerbaijani Sample Journal of Education and Training Studies, 12(2), 114. 10.11114/jets.v12i2.6545</t>
         </is>
       </c>
     </row>
     <row r="3851" spans="1:2">
       <c r="A3851" s="0">
-        <v>4307</v>
+        <v>4308</v>
       </c>
       <c r="B3851" s="0" t="inlineStr">
         <is>
-          <t>Mammadov, Maarif; Babayev, Anar; Mukhtarov, Mirsadig (2024). Examining the Psychometric Properties of the Adolescent Students' Basic Psychological Needs at School Scale for the Azerbaijani Sample Journal of Education and Training Studies, 12(2), 114. 10.11114/jets.v12i2.6545</t>
+          <t>Brown, Emily C.; Edwin, Mary (2024). The Influence of a Culturally Informed Suicide Prevention Training on School Mental Health Professionals' Beliefs Journal of Education and Training Studies, 12(2), 11. 10.11114/jets.v12i2.6571</t>
         </is>
       </c>
     </row>
     <row r="3852" spans="1:2">
       <c r="A3852" s="0">
-        <v>4308</v>
+        <v>4309</v>
       </c>
       <c r="B3852" s="0" t="inlineStr">
         <is>
-          <t>Brown, Emily C.; Edwin, Mary (2024). The Influence of a Culturally Informed Suicide Prevention Training on School Mental Health Professionals' Beliefs Journal of Education and Training Studies, 12(2), 11. 10.11114/jets.v12i2.6571</t>
+          <t>Rowley, Micheal P; Wilkins, Elizabeth M (2024). Weaving Pathways: The Role of High School Family and Consumer Sciences Courses in Cultivating a Teacher Pipeline Across the Midwest Journal of Education and Training Studies, 12(2), 31. 10.11114/jets.v12i2.6589</t>
         </is>
       </c>
     </row>
     <row r="3853" spans="1:2">
       <c r="A3853" s="0">
-        <v>4309</v>
+        <v>4310</v>
       </c>
       <c r="B3853" s="0" t="inlineStr">
         <is>
-          <t>Rowley, Micheal P; Wilkins, Elizabeth M (2024). Weaving Pathways: The Role of High School Family and Consumer Sciences Courses in Cultivating a Teacher Pipeline Across the Midwest Journal of Education and Training Studies, 12(2), 31. 10.11114/jets.v12i2.6589</t>
+          <t>Kumar, Aakash; Rupley, William H.; Paige, David; McKeown, Debra (2024). Writing Woes of ESL Learners: Can Dynamic Assessment Be the Solution? Journal of Education and Training Studies, 12(2), 48. 10.11114/jets.v12i2.6785</t>
         </is>
       </c>
     </row>
     <row r="3854" spans="1:2">
       <c r="A3854" s="0">
-        <v>4310</v>
+        <v>4311</v>
       </c>
       <c r="B3854" s="0" t="inlineStr">
         <is>
-          <t>Kumar, Aakash; Rupley, William H.; Paige, David; McKeown, Debra (2024). Writing Woes of ESL Learners: Can Dynamic Assessment Be the Solution? Journal of Education and Training Studies, 12(2), 48. 10.11114/jets.v12i2.6785</t>
+          <t>Smith, Robert (2023). Reviewer Acknowledgements for Journal of Education and Training Studies, Vol. 12, No. 1 Journal of Education and Training Studies, 12(1), 99. 10.11114/jets.v12i1.6655</t>
         </is>
       </c>
     </row>
     <row r="3855" spans="1:2">
       <c r="A3855" s="0">
-        <v>4311</v>
+        <v>4312</v>
       </c>
       <c r="B3855" s="0" t="inlineStr">
         <is>
-          <t>Smith, Robert (2023). Reviewer Acknowledgements for Journal of Education and Training Studies, Vol. 12, No. 1 Journal of Education and Training Studies, 12(1), 99. 10.11114/jets.v12i1.6655</t>
+          <t>Wang, Shijie (2024). Challenges and Strategies of Higher Vocational Education in China with the New Demographics-Based on the Data Analysis of China's Seventh National Census Journal of Education and Training Studies, 12(3), 18. 10.11114/jets.v12i3.6889</t>
         </is>
       </c>
     </row>
     <row r="3856" spans="1:2">
       <c r="A3856" s="0">
-        <v>4312</v>
+        <v>4313</v>
       </c>
       <c r="B3856" s="0" t="inlineStr">
         <is>
-          <t>Wang, Shijie (2024). Challenges and Strategies of Higher Vocational Education in China with the New Demographics-Based on the Data Analysis of China's Seventh National Census Journal of Education and Training Studies, 12(3), 18. 10.11114/jets.v12i3.6889</t>
+          <t>Smith, Robert (2024). Reviewer Acknowledgements for Journal of Education and Training Studies, Vol. 12, No. 2 Journal of Education and Training Studies, 12(2), 124. 10.11114/jets.v12i2.6840</t>
         </is>
       </c>
     </row>
     <row r="3857" spans="1:2">
       <c r="A3857" s="0">
-        <v>4313</v>
+        <v>4314</v>
       </c>
       <c r="B3857" s="0" t="inlineStr">
         <is>
-          <t>Smith, Robert (2024). Reviewer Acknowledgements for Journal of Education and Training Studies, Vol. 12, No. 2 Journal of Education and Training Studies, 12(2), 124. 10.11114/jets.v12i2.6840</t>
+          <t>Bowman, Richard F. (2024). Preparing Students to Move into Societal Roles as Leaders Journal of Education and Training Studies, 12(2), 41. 10.11114/jets.v12i2.6761</t>
         </is>
       </c>
     </row>
     <row r="3858" spans="1:2">
       <c r="A3858" s="0">
-        <v>4314</v>
+        <v>4315</v>
       </c>
       <c r="B3858" s="0" t="inlineStr">
         <is>
-          <t>Bowman, Richard F. (2024). Preparing Students to Move into Societal Roles as Leaders Journal of Education and Training Studies, 12(2), 41. 10.11114/jets.v12i2.6761</t>
+          <t>Pierce, Hannah; Kermack, Alex; Foley, Vikki (2024). What Training Do Foundation Doctors Feel They Require to Develop as Clinical Teachers? Journal of Education and Training Studies, 12(2), 106. 10.11114/jets.v12i2.6714</t>
         </is>
       </c>
     </row>
     <row r="3859" spans="1:2">
       <c r="A3859" s="0">
-        <v>4315</v>
+        <v>4317</v>
       </c>
       <c r="B3859" s="0" t="inlineStr">
         <is>
-          <t>Pierce, Hannah; Kermack, Alex; Foley, Vikki (2024). What Training Do Foundation Doctors Feel They Require to Develop as Clinical Teachers? Journal of Education and Training Studies, 12(2), 106. 10.11114/jets.v12i2.6714</t>
+          <t>, (2023). Issue Information Journal of School Health, 94(1), 1. 10.1111/josh.13204</t>
         </is>
       </c>
     </row>
     <row r="3860" spans="1:2">
       <c r="A3860" s="0">
-        <v>4317</v>
+        <v>4318</v>
       </c>
       <c r="B3860" s="0" t="inlineStr">
         <is>
-          <t>, (2023). Issue Information Journal of School Health, 94(1), 1. 10.1111/josh.13204</t>
+          <t>Langner, Jonathan; Langston, Krista; Mrachek, Ally; Faitak, Bonnie; Martin, Pamela; Cueto, Alexa; Clampitt, Jennifer L; Long, Christopher R; Bartow, Amy; Bodey, Susan; McElfish, Pearl A (2024). Creating Healthy Environments for Schools: A Comprehensive Approach to Improving Nutrition in Arkansas Public Schools. The Journal of school health, NA(NA), NA. 10.1111/josh.13437</t>
         </is>
       </c>
     </row>
     <row r="3861" spans="1:2">
       <c r="A3861" s="0">
-        <v>4318</v>
+        <v>4319</v>
       </c>
       <c r="B3861" s="0" t="inlineStr">
         <is>
-          <t>Langner, Jonathan; Langston, Krista; Mrachek, Ally; Faitak, Bonnie; Martin, Pamela; Cueto, Alexa; Clampitt, Jennifer L; Long, Christopher R; Bartow, Amy; Bodey, Susan; McElfish, Pearl A (2024). Creating Healthy Environments for Schools: A Comprehensive Approach to Improving Nutrition in Arkansas Public Schools. The Journal of school health, NA(NA), NA. 10.1111/josh.13437</t>
+          <t>Murdock, Abigail R; Rogers, Michelle L; Jackson, Tracy L; Monteiro, Karine; Chambers, Laura C (2023). Mental Health Status of Rhode Island Middle School and High School Students Before Versus During the COVID-19 Pandemic. The Journal of school health, 94(6), 489. 10.1111/josh.13424</t>
         </is>
       </c>
     </row>
     <row r="3862" spans="1:2">
       <c r="A3862" s="0">
-        <v>4319</v>
+        <v>4320</v>
       </c>
       <c r="B3862" s="0" t="inlineStr">
         <is>
-          <t>Murdock, Abigail R; Rogers, Michelle L; Jackson, Tracy L; Monteiro, Karine; Chambers, Laura C (2023). Mental Health Status of Rhode Island Middle School and High School Students Before Versus During the COVID-19 Pandemic. The Journal of school health, 94(6), 489. 10.1111/josh.13424</t>
+          <t>Archuleta, Shannon; Allison-Burbank, Joshuaa D.; Ingalls, Allison; Begay, Renae; Grass, Ryan; Larzelere, Francene; Begaye, Vanessa; Howe, LD; Tsosie, Alicia; Keryte, Angelina Phoebe; Haroz, Emily E. (2024). Withdrawal: Baseline Sociodemographic Characteristics and Mental Health Status of Primary Caregivers and Children Attending Schools on the Navajo Nation and White Mountain Apache Tribe During COVID-19. The Journal of school health, 94(5), 481. 10.1111/josh.13419</t>
         </is>
       </c>
     </row>
     <row r="3863" spans="1:2">
       <c r="A3863" s="0">
-        <v>4320</v>
+        <v>4321</v>
       </c>
       <c r="B3863" s="0" t="inlineStr">
         <is>
-          <t>Archuleta, Shannon; Allison-Burbank, Joshuaa D.; Ingalls, Allison; Begay, Renae; Grass, Ryan; Larzelere, Francene; Begaye, Vanessa; Howe, LD; Tsosie, Alicia; Keryte, Angelina Phoebe; Haroz, Emily E. (2024). Withdrawal: Baseline Sociodemographic Characteristics and Mental Health Status of Primary Caregivers and Children Attending Schools on the Navajo Nation and White Mountain Apache Tribe During COVID-19. The Journal of school health, 94(5), 481. 10.1111/josh.13419</t>
+          <t>Patte, Karen A; Gohari, Mahmood R; Faulkner, Guy; Bélanger, Richard E; Leatherdale, Scott T (2024). Inequitable Changes in School Connectedness During the Ongoing COVID-19 Pandemic in a Cohort of Canadian Adolescents. The Journal of school health, 94(6), 509. 10.1111/josh.13443</t>
         </is>
       </c>
     </row>
     <row r="3864" spans="1:2">
       <c r="A3864" s="0">
-        <v>4321</v>
+        <v>4322</v>
       </c>
       <c r="B3864" s="0" t="inlineStr">
         <is>
-          <t>Patte, Karen A; Gohari, Mahmood R; Faulkner, Guy; Bélanger, Richard E; Leatherdale, Scott T (2024). Inequitable Changes in School Connectedness During the Ongoing COVID-19 Pandemic in a Cohort of Canadian Adolescents. The Journal of school health, 94(6), 509. 10.1111/josh.13443</t>
+          <t>Banas, Jennifer R; Valley, Julia A; Chaudhri, Amina; Gershon, Sarah (2024). The Psychosocial Benefits of Biblioguidance Book Clubs. The Journal of school health, NA(NA), NA. 10.1111/josh.13428</t>
         </is>
       </c>
     </row>
     <row r="3865" spans="1:2">
       <c r="A3865" s="0">
-        <v>4322</v>
+        <v>4323</v>
       </c>
       <c r="B3865" s="0" t="inlineStr">
         <is>
-          <t>Banas, Jennifer R; Valley, Julia A; Chaudhri, Amina; Gershon, Sarah (2024). The Psychosocial Benefits of Biblioguidance Book Clubs. The Journal of school health, NA(NA), NA. 10.1111/josh.13428</t>
+          <t>Shepherd, Heather A; Heming, Emily; Reed, Nick; Caron, Jeffrey G; Yeates, Keith O; Emery, Carolyn A (2024). Describing High School Stakeholders' Preferences for a Return-to-School Framework Following Concussion. The Journal of school health, NA(NA), NA. 10.1111/josh.13434</t>
         </is>
       </c>
     </row>
     <row r="3866" spans="1:2">
       <c r="A3866" s="0">
-        <v>4323</v>
+        <v>4324</v>
       </c>
       <c r="B3866" s="0" t="inlineStr">
         <is>
-          <t>Shepherd, Heather A; Heming, Emily; Reed, Nick; Caron, Jeffrey G; Yeates, Keith O; Emery, Carolyn A (2024). Describing High School Stakeholders' Preferences for a Return-to-School Framework Following Concussion. The Journal of school health, NA(NA), NA. 10.1111/josh.13434</t>
+          <t>Frye, William S; Swan, Kimberly; Gardner, Lauren M (2023). Utilization of an Educational Liaison for Coordinated Care Between the Medical Home and School-Based Professionals for Students with Chronic Pain. The Journal of school health, 94(3), 273. 10.1111/josh.13423</t>
         </is>
       </c>
     </row>
     <row r="3867" spans="1:2">
       <c r="A3867" s="0">
-        <v>4324</v>
+        <v>4325</v>
       </c>
       <c r="B3867" s="0" t="inlineStr">
         <is>
-          <t>Frye, William S; Swan, Kimberly; Gardner, Lauren M (2023). Utilization of an Educational Liaison for Coordinated Care Between the Medical Home and School-Based Professionals for Students with Chronic Pain. The Journal of school health, 94(3), 273. 10.1111/josh.13423</t>
+          <t>Thurstone, Christian; Loh, Ryan; O'Leary, Sonja; Bruce, Sophia; Ladegard, Kristie (2023). School-Based Services May Eliminate Substance Treatment Disparities: Results From a Nonrandomized Program Evaluation. The Journal of school health, 94(3), 267. 10.1111/josh.13413</t>
         </is>
       </c>
     </row>
     <row r="3868" spans="1:2">
       <c r="A3868" s="0">
-        <v>4325</v>
+        <v>4326</v>
       </c>
       <c r="B3868" s="0" t="inlineStr">
         <is>
-          <t>Thurstone, Christian; Loh, Ryan; O'Leary, Sonja; Bruce, Sophia; Ladegard, Kristie (2023). School-Based Services May Eliminate Substance Treatment Disparities: Results From a Nonrandomized Program Evaluation. The Journal of school health, 94(3), 267. 10.1111/josh.13413</t>
+          <t>Kolbe, Lloyd J (2024). The Future of School Health Education in the United States: An Ontology. The Journal of school health, NA(NA), NA. 10.1111/josh.13436</t>
         </is>
       </c>
     </row>
     <row r="3869" spans="1:2">
       <c r="A3869" s="0">
-        <v>4326</v>
+        <v>4327</v>
       </c>
       <c r="B3869" s="0" t="inlineStr">
         <is>
-          <t>Kolbe, Lloyd J (2024). The Future of School Health Education in the United States: An Ontology. The Journal of school health, NA(NA), NA. 10.1111/josh.13436</t>
+          <t>, (2024). Issue Information Journal of School Health, 94(4), 285. 10.1111/josh.13207</t>
         </is>
       </c>
     </row>
     <row r="3870" spans="1:2">
       <c r="A3870" s="0">
-        <v>4327</v>
+        <v>4328</v>
       </c>
       <c r="B3870" s="0" t="inlineStr">
         <is>
-          <t>, (2024). Issue Information Journal of School Health, 94(4), 285. 10.1111/josh.13207</t>
+          <t>Burkholder, Kara; Bennett, Brooke L; McKee, Sarah L; Cohen, Juliana F W; Xu, Ran; Schwartz, Marlene B (2024). Participation in the US Department of Agriculture's Summer Meal Programs: 2019-2021. The Journal of school health, NA(NA), NA. 10.1111/josh.13438</t>
         </is>
       </c>
     </row>
     <row r="3871" spans="1:2">
       <c r="A3871" s="0">
-        <v>4328</v>
+        <v>4329</v>
       </c>
       <c r="B3871" s="0" t="inlineStr">
         <is>
-          <t>Burkholder, Kara; Bennett, Brooke L; McKee, Sarah L; Cohen, Juliana F W; Xu, Ran; Schwartz, Marlene B (2024). Participation in the US Department of Agriculture's Summer Meal Programs: 2019-2021. The Journal of school health, NA(NA), NA. 10.1111/josh.13438</t>
+          <t>Burnett, Honora Quinn; Boral, Alyssa; Schaap, Samantha; Haas-Howard, Christy; O'Leary, Sonja (2023). Implementing a School-Based Health Center Virtual Care Program: A Qualitative Exploration of the School Nurse Perspective. The Journal of school health, NA(NA), NA. 10.1111/josh.13415</t>
         </is>
       </c>
     </row>
     <row r="3872" spans="1:2">
       <c r="A3872" s="0">
-        <v>4329</v>
+        <v>4331</v>
       </c>
       <c r="B3872" s="0" t="inlineStr">
         <is>
-          <t>Burnett, Honora Quinn; Boral, Alyssa; Schaap, Samantha; Haas-Howard, Christy; O'Leary, Sonja (2023). Implementing a School-Based Health Center Virtual Care Program: A Qualitative Exploration of the School Nurse Perspective. The Journal of school health, NA(NA), NA. 10.1111/josh.13415</t>
+          <t>Arnold, Jim P; Farello, Anna; Özkoca, Nazlı; Ozenbaugh, Isabella; Braxling, Cole; Massey, William V (2024). Improving Recess through Collaboration: Exploring the Facilitators and Barriers to Sustaining Positive Playground Behavior. The Journal of school health, NA(NA), NA. 10.1111/josh.13461</t>
         </is>
       </c>
     </row>
     <row r="3873" spans="1:2">
       <c r="A3873" s="0">
-        <v>4331</v>
+        <v>4332</v>
       </c>
       <c r="B3873" s="0" t="inlineStr">
         <is>
-          <t>Arnold, Jim P; Farello, Anna; Özkoca, Nazlı; Ozenbaugh, Isabella; Braxling, Cole; Massey, William V (2024). Improving Recess through Collaboration: Exploring the Facilitators and Barriers to Sustaining Positive Playground Behavior. The Journal of school health, NA(NA), NA. 10.1111/josh.13461</t>
+          <t>, (2024). NA Journal of School Health, 94(4), NA. 10.1111/josh.v94.4</t>
         </is>
       </c>
     </row>
     <row r="3874" spans="1:2">
       <c r="A3874" s="0">
-        <v>4332</v>
+        <v>4334</v>
       </c>
       <c r="B3874" s="0" t="inlineStr">
         <is>
-          <t>, (2024). NA Journal of School Health, 94(4), NA. 10.1111/josh.v94.4</t>
+          <t>Wordley, Valerie; Vasthare, Ramprasad; Lee, Hyewon (2024). Oral Health for all Schools: A Call to Integrate Oral Health in School Systems. The Journal of school health, NA(NA), NA. 10.1111/josh.13450</t>
         </is>
       </c>
     </row>
     <row r="3875" spans="1:2">
       <c r="A3875" s="0">
-        <v>4334</v>
+        <v>4335</v>
       </c>
       <c r="B3875" s="0" t="inlineStr">
         <is>
-          <t>Wordley, Valerie; Vasthare, Ramprasad; Lee, Hyewon (2024). Oral Health for all Schools: A Call to Integrate Oral Health in School Systems. The Journal of school health, NA(NA), NA. 10.1111/josh.13450</t>
+          <t>Chau, Kénora; Chau, Nearkasen (2024). Untreated Allergy Among Middle School Students: Associations with Socioeconomic Adversities and Academic, Behavior, and Health Difficulties. The Journal of school health, NA(NA), NA. 10.1111/josh.13447</t>
         </is>
       </c>
     </row>
     <row r="3876" spans="1:2">
       <c r="A3876" s="0">
-        <v>4335</v>
+        <v>4336</v>
       </c>
       <c r="B3876" s="0" t="inlineStr">
         <is>
-          <t>Chau, Kénora; Chau, Nearkasen (2024). Untreated Allergy Among Middle School Students: Associations with Socioeconomic Adversities and Academic, Behavior, and Health Difficulties. The Journal of school health, NA(NA), NA. 10.1111/josh.13447</t>
+          <t>Fisher, Sycarah; Benner, Kalea; Huang, Hannah; Day, Elizabeth (2024). Substance Use Screening, Brief Intervention, and Referral to Treatment in Urban Settings: Barriers and Facilitators to Implementation With Minoritized Youth. The Journal of school health, 94(4), 299. 10.1111/josh.13430</t>
         </is>
       </c>
     </row>
     <row r="3877" spans="1:2">
       <c r="A3877" s="0">
-        <v>4336</v>
+        <v>4337</v>
       </c>
       <c r="B3877" s="0" t="inlineStr">
         <is>
-          <t>Fisher, Sycarah; Benner, Kalea; Huang, Hannah; Day, Elizabeth (2024). Substance Use Screening, Brief Intervention, and Referral to Treatment in Urban Settings: Barriers and Facilitators to Implementation With Minoritized Youth. The Journal of school health, 94(4), 299. 10.1111/josh.13430</t>
+          <t>Sowa, Nathaniel A; Gaffney, Katie; Sanders, Amanda; Murrell, Caroline (2024). School-Based Tele-Behavioral Health: A Scoping Review of the Literature. The Journal of school health, 94(6), 571. 10.1111/josh.13435</t>
         </is>
       </c>
     </row>
     <row r="3878" spans="1:2">
       <c r="A3878" s="0">
-        <v>4337</v>
+        <v>4338</v>
       </c>
       <c r="B3878" s="0" t="inlineStr">
         <is>
-          <t>Sowa, Nathaniel A; Gaffney, Katie; Sanders, Amanda; Murrell, Caroline (2024). School-Based Tele-Behavioral Health: A Scoping Review of the Literature. The Journal of school health, 94(6), 571. 10.1111/josh.13435</t>
+          <t>Price, Myeshia N; Lee, Wilson Y; Hobbs, J N; DeChants, Jonah P; Davis, Carrie K (2024). Middle and High School LGBTQ Students Report What Makes School LGBTQ-Affirming Across Race/Ethnicity and Gender Identity, a Topic Modeling Method. The Journal of school health, NA(NA), NA. 10.1111/josh.13460</t>
         </is>
       </c>
     </row>
     <row r="3879" spans="1:2">
       <c r="A3879" s="0">
-        <v>4338</v>
+        <v>4339</v>
       </c>
       <c r="B3879" s="0" t="inlineStr">
         <is>
-          <t>Price, Myeshia N; Lee, Wilson Y; Hobbs, J N; DeChants, Jonah P; Davis, Carrie K (2024). Middle and High School LGBTQ Students Report What Makes School LGBTQ-Affirming Across Race/Ethnicity and Gender Identity, a Topic Modeling Method. The Journal of school health, NA(NA), NA. 10.1111/josh.13460</t>
+          <t>Moore, Mikaela; Balascio, Phoebe; Bonner-Johnson, Tausha; Garth, José; Brinkman, Britney; Hill, Ashley V (2024). Implementing Comprehensive Sex and Sexuality Education in Kindergarten-Grade 12 Schools: Guiding Practices and Examples. The Journal of school health, 94(4), 374. 10.1111/josh.13431</t>
         </is>
       </c>
     </row>
     <row r="3880" spans="1:2">
       <c r="A3880" s="0">
-        <v>4339</v>
+        <v>4340</v>
       </c>
       <c r="B3880" s="0" t="inlineStr">
         <is>
-          <t>Moore, Mikaela; Balascio, Phoebe; Bonner-Johnson, Tausha; Garth, José; Brinkman, Britney; Hill, Ashley V (2024). Implementing Comprehensive Sex and Sexuality Education in Kindergarten-Grade 12 Schools: Guiding Practices and Examples. The Journal of school health, 94(4), 374. 10.1111/josh.13431</t>
+          <t>, (2024). NA Journal of School Health, 94(5), NA. 10.1111/josh.v94.5</t>
         </is>
       </c>
     </row>
     <row r="3881" spans="1:2">
       <c r="A3881" s="0">
-        <v>4340</v>
+        <v>4341</v>
       </c>
       <c r="B3881" s="0" t="inlineStr">
         <is>
-          <t>, (2024). NA Journal of School Health, 94(5), NA. 10.1111/josh.v94.5</t>
+          <t>Hullenaar, Keith L; Hicks, Chelsea D; Stubblefield, Marcus W; Herndon Flip, Lester; Seabrooks, Susan K; Vavilala, Monica S; Laing, Sharon S (2024). Insights from Developing and Implementing a Novel School Community Collaborative Model to Promote School Safety. The Journal of school health, NA(NA), NA. 10.1111/josh.13451</t>
         </is>
       </c>
     </row>
     <row r="3882" spans="1:2">
       <c r="A3882" s="0">
-        <v>4341</v>
+        <v>4342</v>
       </c>
       <c r="B3882" s="0" t="inlineStr">
         <is>
-          <t>Hullenaar, Keith L; Hicks, Chelsea D; Stubblefield, Marcus W; Herndon Flip, Lester; Seabrooks, Susan K; Vavilala, Monica S; Laing, Sharon S (2024). Insights from Developing and Implementing a Novel School Community Collaborative Model to Promote School Safety. The Journal of school health, NA(NA), NA. 10.1111/josh.13451</t>
+          <t>, (2023). NA Journal of School Health, 93(11), NA. 10.1111/josh.v93.11</t>
         </is>
       </c>
     </row>
     <row r="3883" spans="1:2">
       <c r="A3883" s="0">
-        <v>4342</v>
+        <v>4343</v>
       </c>
       <c r="B3883" s="0" t="inlineStr">
         <is>
-          <t>, (2023). NA Journal of School Health, 93(11), NA. 10.1111/josh.v93.11</t>
+          <t>Jayawardene, Wasantha; Lohrmann, David; Agley, Jon; Jun, Mikyoung; Gassman, Ruth (2024). Adverse Childhood Experience-Related Conditions and Substance Use in Adolescents: A Secondary Analysis of Cross-Sectional Survey Data. The Journal of school health, 94(5), 385. 10.1111/josh.13429</t>
         </is>
       </c>
     </row>
     <row r="3884" spans="1:2">
       <c r="A3884" s="0">
-        <v>4343</v>
+        <v>4344</v>
       </c>
       <c r="B3884" s="0" t="inlineStr">
         <is>
-          <t>Jayawardene, Wasantha; Lohrmann, David; Agley, Jon; Jun, Mikyoung; Gassman, Ruth (2024). Adverse Childhood Experience-Related Conditions and Substance Use in Adolescents: A Secondary Analysis of Cross-Sectional Survey Data. The Journal of school health, 94(5), 385. 10.1111/josh.13429</t>
+          <t>Perniciaro, Kelly; Moore, Michele J; Zeglin, Robert J; Terrell, Kassie R (2024). Body Dissatisfaction and Health Risk Behaviors Among Middle School Girls. The Journal of school health, 94(5), 453. 10.1111/josh.13440</t>
         </is>
       </c>
     </row>
     <row r="3885" spans="1:2">
       <c r="A3885" s="0">
-        <v>4344</v>
+        <v>4345</v>
       </c>
       <c r="B3885" s="0" t="inlineStr">
         <is>
-          <t>Perniciaro, Kelly; Moore, Michele J; Zeglin, Robert J; Terrell, Kassie R (2024). Body Dissatisfaction and Health Risk Behaviors Among Middle School Girls. The Journal of school health, 94(5), 453. 10.1111/josh.13440</t>
+          <t>, (2024). NA Journal of School Health, 94(1), NA. 10.1111/josh.v94.1</t>
         </is>
       </c>
     </row>
     <row r="3886" spans="1:2">
       <c r="A3886" s="0">
-        <v>4345</v>
+        <v>4346</v>
       </c>
       <c r="B3886" s="0" t="inlineStr">
         <is>
-          <t>, (2024). NA Journal of School Health, 94(1), NA. 10.1111/josh.v94.1</t>
+          <t>Keeton, Victoria F; Soleimanpour, Samira; Geierstanger, Sara; Schapiro, Naomi A (2024). Case Management for Social Needs of Youth and Families in School-Based Health Centers. The Journal of school health, 94(5), 462. 10.1111/josh.13432</t>
         </is>
       </c>
     </row>
     <row r="3887" spans="1:2">
       <c r="A3887" s="0">
-        <v>4346</v>
+        <v>4347</v>
       </c>
       <c r="B3887" s="0" t="inlineStr">
         <is>
-          <t>Keeton, Victoria F; Soleimanpour, Samira; Geierstanger, Sara; Schapiro, Naomi A (2024). Case Management for Social Needs of Youth and Families in School-Based Health Centers. The Journal of school health, 94(5), 462. 10.1111/josh.13432</t>
+          <t>, (2024). Issue Information Journal of School Health, 94(2), 101. 10.1111/josh.13205</t>
         </is>
       </c>
     </row>
     <row r="3888" spans="1:2">
       <c r="A3888" s="0">
-        <v>4347</v>
+        <v>4348</v>
       </c>
       <c r="B3888" s="0" t="inlineStr">
         <is>
-          <t>, (2024). Issue Information Journal of School Health, 94(2), 101. 10.1111/josh.13205</t>
+          <t>LoPresto, Lynnea M; Cassady, Diana L; Dove, Melanie S (2023). Evaluation of School Wellness Policies in Low-Income California Districts After the 2016 USDA Final Rule. The Journal of school health, 94(4), 327. 10.1111/josh.13422</t>
         </is>
       </c>
     </row>
     <row r="3889" spans="1:2">
       <c r="A3889" s="0">
-        <v>4348</v>
+        <v>4349</v>
       </c>
       <c r="B3889" s="0" t="inlineStr">
         <is>
-          <t>LoPresto, Lynnea M; Cassady, Diana L; Dove, Melanie S (2023). Evaluation of School Wellness Policies in Low-Income California Districts After the 2016 USDA Final Rule. The Journal of school health, 94(4), 327. 10.1111/josh.13422</t>
+          <t>, (2024). Issue Information Journal of School Health, 94(3), 205. 10.1111/josh.13206</t>
         </is>
       </c>
     </row>
     <row r="3890" spans="1:2">
       <c r="A3890" s="0">
-        <v>4349</v>
+        <v>4350</v>
       </c>
       <c r="B3890" s="0" t="inlineStr">
         <is>
-          <t>, (2024). Issue Information Journal of School Health, 94(3), 205. 10.1111/josh.13206</t>
+          <t>Kan, Kristin; Enaholo, Ososese; Kanaley, Madeleine; Holtzman, Gwen; Ibrahim, Khalid; Morales, Lu; Lombard, Lisa; Gupta, Ruchi (2023). Well-Being of Children and Families in COVID-19 Hotspots in Chicago. The Journal of school health, 94(3), 219. 10.1111/josh.13416</t>
         </is>
       </c>
     </row>
     <row r="3891" spans="1:2">
       <c r="A3891" s="0">
-        <v>4350</v>
+        <v>4352</v>
       </c>
       <c r="B3891" s="0" t="inlineStr">
         <is>
-          <t>Kan, Kristin; Enaholo, Ososese; Kanaley, Madeleine; Holtzman, Gwen; Ibrahim, Khalid; Morales, Lu; Lombard, Lisa; Gupta, Ruchi (2023). Well-Being of Children and Families in COVID-19 Hotspots in Chicago. The Journal of school health, 94(3), 219. 10.1111/josh.13416</t>
+          <t>Mellon, Pamela; Montemurro, Genevieve; Sulz, Lauren; Torrance, Brian; Storey, Kate (2024). "Your Kid Has Potential, But They Need Sleep": Teacher Perspectives on School-Based Sleep Promotion in Alberta, Canada. The Journal of school health, 94(4), 357. 10.1111/josh.13439</t>
         </is>
       </c>
     </row>
     <row r="3892" spans="1:2">
       <c r="A3892" s="0">
-        <v>4352</v>
+        <v>4353</v>
       </c>
       <c r="B3892" s="0" t="inlineStr">
         <is>
-          <t>Mellon, Pamela; Montemurro, Genevieve; Sulz, Lauren; Torrance, Brian; Storey, Kate (2024). "Your Kid Has Potential, But They Need Sleep": Teacher Perspectives on School-Based Sleep Promotion in Alberta, Canada. The Journal of school health, 94(4), 357. 10.1111/josh.13439</t>
+          <t>Yeargin, Susan; Hirschhorn, Rebecca M; Adams, William M; Scarneo-Miller, Samantha E (2024). Secondary School State Athletic Association Health and Safety Policy Development Processes. The Journal of school health, NA(NA), NA. 10.1111/josh.13454</t>
         </is>
       </c>
     </row>
     <row r="3893" spans="1:2">
       <c r="A3893" s="0">
-        <v>4353</v>
+        <v>4354</v>
       </c>
       <c r="B3893" s="0" t="inlineStr">
         <is>
-          <t>Yeargin, Susan; Hirschhorn, Rebecca M; Adams, William M; Scarneo-Miller, Samantha E (2024). Secondary School State Athletic Association Health and Safety Policy Development Processes. The Journal of school health, NA(NA), NA. 10.1111/josh.13454</t>
+          <t>Dunfee, Madeline N; Bush, Heather; Leger, Kate A; Hilbert, Timothy J; Brancato, Candace; Haynes, Erin N (2024). Characteristics of K-12 Teachers Considering Leaving Due to COVID-19 and for Other Reasons. The Journal of school health, 94(6), 519. 10.1111/josh.13452</t>
         </is>
       </c>
     </row>
     <row r="3894" spans="1:2">
       <c r="A3894" s="0">
-        <v>4354</v>
+        <v>4356</v>
       </c>
       <c r="B3894" s="0" t="inlineStr">
         <is>
-          <t>Dunfee, Madeline N; Bush, Heather; Leger, Kate A; Hilbert, Timothy J; Brancato, Candace; Haynes, Erin N (2024). Characteristics of K-12 Teachers Considering Leaving Due to COVID-19 and for Other Reasons. The Journal of school health, 94(6), 519. 10.1111/josh.13452</t>
+          <t>Venkatapuram, Pranaya; Angulo-Lozano, Juan C; Spinzi, Stav; Brown-Johnson, Cati; Phord-Toy, Ashley; Kan, Kathleen M (2024). Parental Knowledge, Beliefs, Practices, and Barriers Related to Children's Bladder Health in the School Environment. The Journal of school health, NA(NA), NA. 10.1111/josh.13456</t>
         </is>
       </c>
     </row>
     <row r="3895" spans="1:2">
       <c r="A3895" s="0">
-        <v>4356</v>
+        <v>4357</v>
       </c>
       <c r="B3895" s="0" t="inlineStr">
         <is>
-          <t>Venkatapuram, Pranaya; Angulo-Lozano, Juan C; Spinzi, Stav; Brown-Johnson, Cati; Phord-Toy, Ashley; Kan, Kathleen M (2024). Parental Knowledge, Beliefs, Practices, and Barriers Related to Children's Bladder Health in the School Environment. The Journal of school health, NA(NA), NA. 10.1111/josh.13456</t>
+          <t>Abu Khudair, Sara; Khader, Yousef; Al Nsour, Mohannad; Tanaka, Eizaburo (2024). The Provision of Psychosocial Support to Students in Jordan: Teachers' Knowledge, Attitudes, Skills, Practices, and Perceived Barriers. The Journal of school health, NA(NA), NA. 10.1111/josh.13459</t>
         </is>
       </c>
     </row>
     <row r="3896" spans="1:2">
       <c r="A3896" s="0">
-        <v>4357</v>
+        <v>4358</v>
       </c>
       <c r="B3896" s="0" t="inlineStr">
         <is>
-          <t>Abu Khudair, Sara; Khader, Yousef; Al Nsour, Mohannad; Tanaka, Eizaburo (2024). The Provision of Psychosocial Support to Students in Jordan: Teachers' Knowledge, Attitudes, Skills, Practices, and Perceived Barriers. The Journal of school health, NA(NA), NA. 10.1111/josh.13459</t>
+          <t>Ruff, Ryan R; Barry Godín, Tamarinda J; Whittemore, Rachel; Murray Small, Topaz; Santiago-Galvin, Nydia; Sharma, Priyanka (2024). Unmet Dental Needs in Children Following Suspension of School-Based Oral Health Services Due to COVID-19. The Journal of school health, 94(5), 427. 10.1111/josh.13433</t>
         </is>
       </c>
     </row>
     <row r="3897" spans="1:2">
       <c r="A3897" s="0">
-        <v>4358</v>
+        <v>4359</v>
       </c>
       <c r="B3897" s="0" t="inlineStr">
         <is>
-          <t>Ruff, Ryan R; Barry Godín, Tamarinda J; Whittemore, Rachel; Murray Small, Topaz; Santiago-Galvin, Nydia; Sharma, Priyanka (2024). Unmet Dental Needs in Children Following Suspension of School-Based Oral Health Services Due to COVID-19. The Journal of school health, 94(5), 427. 10.1111/josh.13433</t>
+          <t>, (2024). Issue Information Journal of School Health, 94(5), 381. 10.1111/josh.13208</t>
         </is>
       </c>
     </row>
     <row r="3898" spans="1:2">
       <c r="A3898" s="0">
-        <v>4359</v>
+        <v>4360</v>
       </c>
       <c r="B3898" s="0" t="inlineStr">
         <is>
-          <t>, (2024). Issue Information Journal of School Health, 94(5), 381. 10.1111/josh.13208</t>
+          <t>Martinez, Laurie A; Opalinski, Andra S; Herbert, Linda (2023). The Lived Experiences of Students With Food Allergies During a Usual Weekday. The Journal of school health, NA(NA), NA. 10.1111/josh.13420</t>
         </is>
       </c>
     </row>
     <row r="3899" spans="1:2">
       <c r="A3899" s="0">
-        <v>4360</v>
+        <v>4361</v>
       </c>
       <c r="B3899" s="0" t="inlineStr">
         <is>
-          <t>Martinez, Laurie A; Opalinski, Andra S; Herbert, Linda (2023). The Lived Experiences of Students With Food Allergies During a Usual Weekday. The Journal of school health, NA(NA), NA. 10.1111/josh.13420</t>
+          <t>Gaal, Susanne R; Fuller, Matthew B (2024). School Safety and Mental Health Awareness: Recommendations from K-12 Texas Public School Teachers. The Journal of school health, 94(4), 308. 10.1111/josh.13425</t>
         </is>
       </c>
     </row>
     <row r="3900" spans="1:2">
       <c r="A3900" s="0">
-        <v>4361</v>
+        <v>4362</v>
       </c>
       <c r="B3900" s="0" t="inlineStr">
         <is>
-          <t>Gaal, Susanne R; Fuller, Matthew B (2024). School Safety and Mental Health Awareness: Recommendations from K-12 Texas Public School Teachers. The Journal of school health, 94(4), 308. 10.1111/josh.13425</t>
+          <t>Fraley, Hannah E; Capp, Gordon (2024). Past School Discipline Experiences: Perspectives of Disabled Adults. The Journal of school health, NA(NA), NA. 10.1111/josh.13462</t>
         </is>
       </c>
     </row>
     <row r="3901" spans="1:2">
       <c r="A3901" s="0">
-        <v>4362</v>
+        <v>4363</v>
       </c>
       <c r="B3901" s="0" t="inlineStr">
         <is>
-          <t>Fraley, Hannah E; Capp, Gordon (2024). Past School Discipline Experiences: Perspectives of Disabled Adults. The Journal of school health, NA(NA), NA. 10.1111/josh.13462</t>
+          <t>Dougherty, Michelle; Plenn, Eion R; Corey, Stephanie L; Onufer, Lindsay; Coulter, Robert W S; NA, NA (2023). Going the Extra Mile: How High School Staff Use Informal Strategies to Support, Protect, and Care for LGBTQ+ Students. The Journal of school health, 94(4), 289. 10.1111/josh.13417</t>
         </is>
       </c>
     </row>
     <row r="3902" spans="1:2">
       <c r="A3902" s="0">
-        <v>4363</v>
+        <v>4364</v>
       </c>
       <c r="B3902" s="0" t="inlineStr">
         <is>
-          <t>Dougherty, Michelle; Plenn, Eion R; Corey, Stephanie L; Onufer, Lindsay; Coulter, Robert W S; NA, NA (2023). Going the Extra Mile: How High School Staff Use Informal Strategies to Support, Protect, and Care for LGBTQ+ Students. The Journal of school health, 94(4), 289. 10.1111/josh.13417</t>
+          <t>Lindstrom Johnson, Sarah; Kulkarni, Nita; Rodríguez De Jesús, Sue A; Cottam, Stephanie; Fillhouer, Marianne; Guevara, Ana M M (2024). School-Family Partnerships to Support Attendance: Advancing an Equity-Centered Theoretical Framework. The Journal of school health, NA(NA), NA. 10.1111/josh.13457</t>
         </is>
       </c>
     </row>
     <row r="3903" spans="1:2">
       <c r="A3903" s="0">
-        <v>4364</v>
+        <v>4365</v>
       </c>
       <c r="B3903" s="0" t="inlineStr">
         <is>
-          <t>Lindstrom Johnson, Sarah; Kulkarni, Nita; Rodríguez De Jesús, Sue A; Cottam, Stephanie; Fillhouer, Marianne; Guevara, Ana M M (2024). School-Family Partnerships to Support Attendance: Advancing an Equity-Centered Theoretical Framework. The Journal of school health, NA(NA), NA. 10.1111/josh.13457</t>
+          <t>, (2024). NA Journal of School Health, 94(3), NA. 10.1111/josh.v94.3</t>
         </is>
       </c>
     </row>
     <row r="3904" spans="1:2">
       <c r="A3904" s="0">
-        <v>4365</v>
+        <v>4366</v>
       </c>
       <c r="B3904" s="0" t="inlineStr">
         <is>
-          <t>, (2024). NA Journal of School Health, 94(3), NA. 10.1111/josh.v94.3</t>
+          <t>Lawson, Gwendolyn M; Azad, Gazi (2024). School-Based Mental Health Interventions: Recommendations for Selecting and Reporting Implementation Strategies. The Journal of school health, 94(6), 581. 10.1111/josh.13458</t>
         </is>
       </c>
     </row>
     <row r="3905" spans="1:2">
       <c r="A3905" s="0">
-        <v>4366</v>
+        <v>4367</v>
       </c>
       <c r="B3905" s="0" t="inlineStr">
         <is>
-          <t>Lawson, Gwendolyn M; Azad, Gazi (2024). School-Based Mental Health Interventions: Recommendations for Selecting and Reporting Implementation Strategies. The Journal of school health, 94(6), 581. 10.1111/josh.13458</t>
+          <t>Jones, Sherry Everett; Brener, Nancy D; Queen, Barbara; Hershey-Arista, Molly; Harris, William; Underwood, J Michael (2024). Reliability of the 2020 School Health Profiles Principal and Lead Health Education Teacher Questionnaires. The Journal of school health, 94(5), 395. 10.1111/josh.13426</t>
         </is>
       </c>
     </row>
     <row r="3906" spans="1:2">
       <c r="A3906" s="0">
-        <v>4367</v>
+        <v>4368</v>
       </c>
       <c r="B3906" s="0" t="inlineStr">
         <is>
-          <t>Jones, Sherry Everett; Brener, Nancy D; Queen, Barbara; Hershey-Arista, Molly; Harris, William; Underwood, J Michael (2024). Reliability of the 2020 School Health Profiles Principal and Lead Health Education Teacher Questionnaires. The Journal of school health, 94(5), 395. 10.1111/josh.13426</t>
+          <t>, (2023). NA Journal of School Health, 93(12), NA. 10.1111/josh.v93.12</t>
         </is>
       </c>
     </row>
     <row r="3907" spans="1:2">
       <c r="A3907" s="0">
-        <v>4368</v>
+        <v>4369</v>
       </c>
       <c r="B3907" s="0" t="inlineStr">
         <is>
-          <t>, (2023). NA Journal of School Health, 93(12), NA. 10.1111/josh.v93.12</t>
+          <t>Shamblen, Stephen R; Ashley, Olivia; Gluck, Andrew; Wood, Catherine (2024). A Group Randomized Controlled Trial of Relationships Under Construction Sexual Risk Avoidance Education. The Journal of school health, NA(NA), NA. 10.1111/josh.13441</t>
         </is>
       </c>
     </row>
     <row r="3908" spans="1:2">
       <c r="A3908" s="0">
-        <v>4369</v>
+        <v>4371</v>
       </c>
       <c r="B3908" s="0" t="inlineStr">
         <is>
-          <t>Shamblen, Stephen R; Ashley, Olivia; Gluck, Andrew; Wood, Catherine (2024). A Group Randomized Controlled Trial of Relationships Under Construction Sexual Risk Avoidance Education. The Journal of school health, NA(NA), NA. 10.1111/josh.13441</t>
+          <t>, (2024). Issue Information Journal of School Health, 94(6), 485. 10.1111/josh.13209</t>
         </is>
       </c>
     </row>
     <row r="3909" spans="1:2">
       <c r="A3909" s="0">
-        <v>4371</v>
+        <v>4372</v>
       </c>
       <c r="B3909" s="0" t="inlineStr">
         <is>
-          <t>, (2024). Issue Information Journal of School Health, 94(6), 485. 10.1111/josh.13209</t>
+          <t>Bates, Samantha; Harrell, Danielle R (2023). COVID-19 School Closures: Disruptions in School-Based Support Services and Socioemotional Loss Among Middle School Students. The Journal of school health, 94(3), 209. 10.1111/josh.13421</t>
         </is>
       </c>
     </row>
     <row r="3910" spans="1:2">
       <c r="A3910" s="0">
-        <v>4372</v>
+        <v>4373</v>
       </c>
       <c r="B3910" s="0" t="inlineStr">
         <is>
-          <t>Bates, Samantha; Harrell, Danielle R (2023). COVID-19 School Closures: Disruptions in School-Based Support Services and Socioemotional Loss Among Middle School Students. The Journal of school health, 94(3), 209. 10.1111/josh.13421</t>
+          <t>Welty, Cody W; Bingham, Lindsay; Morales, Mario; Gerald, Lynn B; Ellingson, Katherine D; Haynes, Patricia L (2024). School Connectedness and Suicide Among High School Youth: A Systematic Review. The Journal of school health, 94(5), 469. 10.1111/josh.13445</t>
         </is>
       </c>
     </row>
     <row r="3911" spans="1:2">
       <c r="A3911" s="0">
-        <v>4373</v>
+        <v>4374</v>
       </c>
       <c r="B3911" s="0" t="inlineStr">
         <is>
-          <t>Welty, Cody W; Bingham, Lindsay; Morales, Mario; Gerald, Lynn B; Ellingson, Katherine D; Haynes, Patricia L (2024). School Connectedness and Suicide Among High School Youth: A Systematic Review. The Journal of school health, 94(5), 469. 10.1111/josh.13445</t>
+          <t>, (2024). NA Journal of School Health, 94(2), NA. 10.1111/josh.v94.2</t>
         </is>
       </c>
     </row>
     <row r="3912" spans="1:2">
       <c r="A3912" s="0">
-        <v>4374</v>
+        <v>4375</v>
       </c>
       <c r="B3912" s="0" t="inlineStr">
         <is>
-          <t>, (2024). NA Journal of School Health, 94(2), NA. 10.1111/josh.v94.2</t>
+          <t>Davis, Charles R; Eraca, Jennifer; Davis, Patti A (2024). Improving Students Access to Primary Health Care Through School-Based Health Centers. The Journal of school health, NA(NA), NA. 10.1111/josh.13455</t>
         </is>
       </c>
     </row>
     <row r="3913" spans="1:2">
       <c r="A3913" s="0">
-        <v>4375</v>
+        <v>4376</v>
       </c>
       <c r="B3913" s="0" t="inlineStr">
         <is>
-          <t>Davis, Charles R; Eraca, Jennifer; Davis, Patti A (2024). Improving Students Access to Primary Health Care Through School-Based Health Centers. The Journal of school health, NA(NA), NA. 10.1111/josh.13455</t>
+          <t>Lo Moro, Giuseppina; Scaioli, Giacomo; Conrado, Francesco; Lusiani, Luca; Pinto, Sonia; Rolfini, Edoardo; Bert, Fabrizio; Siliquini, Roberta (2024). Parental Perception of Children's Mental Health During the Pandemic: Insights From an Italian Cross-Sectional Study. The Journal of school health, 94(6), 539. 10.1111/josh.13449</t>
         </is>
       </c>
     </row>
     <row r="3914" spans="1:2">
       <c r="A3914" s="0">
-        <v>4376</v>
+        <v>4377</v>
       </c>
       <c r="B3914" s="0" t="inlineStr">
         <is>
-          <t>Lo Moro, Giuseppina; Scaioli, Giacomo; Conrado, Francesco; Lusiani, Luca; Pinto, Sonia; Rolfini, Edoardo; Bert, Fabrizio; Siliquini, Roberta (2024). Parental Perception of Children's Mental Health During the Pandemic: Insights From an Italian Cross-Sectional Study. The Journal of school health, 94(6), 539. 10.1111/josh.13449</t>
+          <t>Ambrosino, Christina; Beharry, Kelly; Kallem, Medha; Johnson, Sara B; Connor, Katherine A; Collins, Megan E (2024). Maryland School Health partners' Perspectives on the Impact of COVID-19 on School Health Services for Grades K-12. The Journal of school health, 94(6), 529. 10.1111/josh.13453</t>
         </is>
       </c>
     </row>
     <row r="3915" spans="1:2">
       <c r="A3915" s="0">
-        <v>4377</v>
+        <v>4378</v>
       </c>
       <c r="B3915" s="0" t="inlineStr">
         <is>
-          <t>Ambrosino, Christina; Beharry, Kelly; Kallem, Medha; Johnson, Sara B; Connor, Katherine A; Collins, Megan E (2024). Maryland School Health partners' Perspectives on the Impact of COVID-19 on School Health Services for Grades K-12. The Journal of school health, 94(6), 529. 10.1111/josh.13453</t>
+          <t>Orenstein, Shawn; Yarnell, Jordy; Connors, Elizabeth; Bohnenkamp, Jill; Hoover, Sharon; Lever, Nancy (2024). The State School Mental Health Profile: Findings from 25 States. The Journal of school health, 94(5), 443. 10.1111/josh.13442</t>
         </is>
       </c>
     </row>
     <row r="3916" spans="1:2">
       <c r="A3916" s="0">
-        <v>4378</v>
+        <v>4379</v>
       </c>
       <c r="B3916" s="0" t="inlineStr">
         <is>
-          <t>Orenstein, Shawn; Yarnell, Jordy; Connors, Elizabeth; Bohnenkamp, Jill; Hoover, Sharon; Lever, Nancy (2024). The State School Mental Health Profile: Findings from 25 States. The Journal of school health, 94(5), 443. 10.1111/josh.13442</t>
+          <t>Ilakkuvan, Vinu; De Biasi, Anne (2024). Delivering Medicaid Mental Health Services and Supports in Schools: Current Landscape and Opportunities to Expand. The Journal of school health, 94(6), 562. 10.1111/josh.13427</t>
         </is>
       </c>
     </row>
     <row r="3917" spans="1:2">
       <c r="A3917" s="0">
-        <v>4379</v>
+        <v>4380</v>
       </c>
       <c r="B3917" s="0" t="inlineStr">
         <is>
-          <t>Ilakkuvan, Vinu; De Biasi, Anne (2024). Delivering Medicaid Mental Health Services and Supports in Schools: Current Landscape and Opportunities to Expand. The Journal of school health, 94(6), 562. 10.1111/josh.13427</t>
+          <t>Treviño-Peña, Roberto; Romero, Zasha; Fuentes, Jesús C; Cortez, Karla E; Alanis, Elizabeth; Alvarenga, Juan C L (2024). A Coordinated School Health Program Effect on Cardiorespiratory Fitness of South Texas Preschool Children: A Cluster Randomized Trial. The Journal of school health, 94(4), 336. 10.1111/josh.13414</t>
         </is>
       </c>
     </row>
     <row r="3918" spans="1:2">
       <c r="A3918" s="0">
-        <v>4380</v>
+        <v>4381</v>
       </c>
       <c r="B3918" s="0" t="inlineStr">
         <is>
-          <t>Treviño-Peña, Roberto; Romero, Zasha; Fuentes, Jesús C; Cortez, Karla E; Alanis, Elizabeth; Alvarenga, Juan C L (2024). A Coordinated School Health Program Effect on Cardiorespiratory Fitness of South Texas Preschool Children: A Cluster Randomized Trial. The Journal of school health, 94(4), 336. 10.1111/josh.13414</t>
+          <t>, (2024). NA Journal of School Health, 94(6), NA. 10.1111/josh.v94.6</t>
         </is>
       </c>
     </row>
     <row r="3919" spans="1:2">
       <c r="A3919" s="0">
-        <v>4381</v>
+        <v>4383</v>
       </c>
       <c r="B3919" s="0" t="inlineStr">
         <is>
-          <t>, (2024). NA Journal of School Health, 94(6), NA. 10.1111/josh.v94.6</t>
+          <t>Armstrong-Carter, Emma; Osborn, Steve; Smith, Olivia; Siskowski, Connie; Olson, Elizabeth (2024). "I Missed School to Take Care of Someone Else": Middle and High School Students' Caregiving Responsibilities as a Reason for Absenteeism. The Journal of school health, NA(NA), NA. 10.1111/josh.13446</t>
         </is>
       </c>
     </row>
     <row r="3920" spans="1:2">
       <c r="A3920" s="0">
-        <v>4383</v>
+        <v>4384</v>
       </c>
       <c r="B3920" s="0" t="inlineStr">
         <is>
-          <t>Armstrong-Carter, Emma; Osborn, Steve; Smith, Olivia; Siskowski, Connie; Olson, Elizabeth (2024). "I Missed School to Take Care of Someone Else": Middle and High School Students' Caregiving Responsibilities as a Reason for Absenteeism. The Journal of school health, NA(NA), NA. 10.1111/josh.13446</t>
+          <t>Chaffee, Benjamin W; Cheng, Jing; Couch, Elizabeth T; Halpern-Felsher, Bonnie (2023). Engagement, Mental Health, and Substance Use Under In-Person or Remote School Instruction During the COVID-19 Pandemic. The Journal of school health, 94(6), 501. 10.1111/josh.13418</t>
         </is>
       </c>
     </row>
     <row r="3921" spans="1:2">
       <c r="A3921" s="0">
-        <v>4384</v>
+        <v>4385</v>
       </c>
       <c r="B3921" s="0" t="inlineStr">
         <is>
-          <t>Chaffee, Benjamin W; Cheng, Jing; Couch, Elizabeth T; Halpern-Felsher, Bonnie (2023). Engagement, Mental Health, and Substance Use Under In-Person or Remote School Instruction During the COVID-19 Pandemic. The Journal of school health, 94(6), 501. 10.1111/josh.13418</t>
+          <t>Walsh, Tyler J; Kalb, Luther G; Gemmell, Michael; Liu, Jingxia; Caburnay, Charlene A; Gurnett, Christina A; Newland, Jason G; NA, NA (2024). Assessment of COVID-19 Messaging Strategies to Increase Testing for Students With Intellectual and Developmental Disabilities. The Journal of school health, 94(6), 551. 10.1111/josh.13448</t>
         </is>
       </c>
     </row>
     <row r="3922" spans="1:2">
       <c r="A3922" s="0">
-        <v>4385</v>
+        <v>4386</v>
       </c>
       <c r="B3922" s="0" t="inlineStr">
         <is>
-          <t>Walsh, Tyler J; Kalb, Luther G; Gemmell, Michael; Liu, Jingxia; Caburnay, Charlene A; Gurnett, Christina A; Newland, Jason G; NA, NA (2024). Assessment of COVID-19 Messaging Strategies to Increase Testing for Students With Intellectual and Developmental Disabilities. The Journal of school health, 94(6), 551. 10.1111/josh.13448</t>
+          <t>Partin, Jeana M., Hayes, Sonya D. (2024). Learning From Each Other: Experiences of Rural Principals in a Networked Learning Community , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3923" spans="1:2">
       <c r="A3923" s="0">
-        <v>4386</v>
+        <v>4387</v>
       </c>
       <c r="B3923" s="0" t="inlineStr">
         <is>
-          <t>Partin, Jeana M., Hayes, Sonya D. (2024). Learning From Each Other: Experiences of Rural Principals in a Networked Learning Community , 45(), . </t>
+          <t>Simeonoff, Speridon Sr, Simeonoff, Judy, Simeonoff, Teacon, Simeonoff, Speridon Jr, Haakanson, Sven Jr, Simeonoff, Cheri, Haakanson, Balika, Sabzalian, Leilani (2024). Healing and Connectedness at Akhiok Kids Camp , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3924" spans="1:2">
       <c r="A3924" s="0">
-        <v>4387</v>
+        <v>4388</v>
       </c>
       <c r="B3924" s="0" t="inlineStr">
         <is>
-          <t>Simeonoff, Speridon Sr, Simeonoff, Judy, Simeonoff, Teacon, Simeonoff, Speridon Jr, Haakanson, Sven Jr, Simeonoff, Cheri, Haakanson, Balika, Sabzalian, Leilani (2024). Healing and Connectedness at Akhiok Kids Camp , 45(), . </t>
+          <t>LeClair-Diaz, Amanda, Stanton, Christine (2024). “It Ain’t Gonna be MY History”: Collaborative Meaning-Making to Advance Curricular Sovereignty With(in) Rural, Indigenous-Serving Schools , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3925" spans="1:2">
       <c r="A3925" s="0">
-        <v>4388</v>
+        <v>4389</v>
       </c>
       <c r="B3925" s="0" t="inlineStr">
         <is>
-          <t>LeClair-Diaz, Amanda, Stanton, Christine (2024). “It Ain’t Gonna be MY History”: Collaborative Meaning-Making to Advance Curricular Sovereignty With(in) Rural, Indigenous-Serving Schools , 45(), . </t>
+          <t>Youngbull, Natalie R., Sanders, David (2024). Tribal College and University (TCU) Leadership, Faculty, and Staff Perspectives on Student Success , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3926" spans="1:2">
       <c r="A3926" s="0">
-        <v>4389</v>
+        <v>4390</v>
       </c>
       <c r="B3926" s="0" t="inlineStr">
         <is>
-          <t>Youngbull, Natalie R., Sanders, David (2024). Tribal College and University (TCU) Leadership, Faculty, and Staff Perspectives on Student Success , 45(), . </t>
+          <t>Belansky, Elaine S., Diaz Solodukhin, Liliana, Edelman, Anna, Hobbs, Savannah, Hazel, Cynthia, Cutforth, Nicholas (2024). Strategies to Recruit and Retain the Rural School Mental Health Workforce , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3927" spans="1:2">
       <c r="A3927" s="0">
-        <v>4390</v>
+        <v>4391</v>
       </c>
       <c r="B3927" s="0" t="inlineStr">
         <is>
-          <t>Belansky, Elaine S., Diaz Solodukhin, Liliana, Edelman, Anna, Hobbs, Savannah, Hazel, Cynthia, Cutforth, Nicholas (2024). Strategies to Recruit and Retain the Rural School Mental Health Workforce , 45(), . </t>
+          <t>Cutler White, Carol, Chapman, Diane D. (2024). Rural Parent Viewpoints of What Makes College Possible: A Q Methodology Study , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3928" spans="1:2">
       <c r="A3928" s="0">
-        <v>4391</v>
+        <v>4392</v>
       </c>
       <c r="B3928" s="0" t="inlineStr">
         <is>
-          <t>Cutler White, Carol, Chapman, Diane D. (2024). Rural Parent Viewpoints of What Makes College Possible: A Q Methodology Study , 45(), . </t>
+          <t>Boulden, Rawn, Schimmel, Christine (2024). Addressing the Rural Youth Mental Health Crisis Through Youth Mental Health First Aid , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3929" spans="1:2">
       <c r="A3929" s="0">
-        <v>4392</v>
+        <v>4393</v>
       </c>
       <c r="B3929" s="0" t="inlineStr">
         <is>
-          <t>Boulden, Rawn, Schimmel, Christine (2024). Addressing the Rural Youth Mental Health Crisis Through Youth Mental Health First Aid , 45(), . </t>
+          <t>McNamee, Ty C., Ardoin, Sonja, Willis, Jenay F. E. (2024). Rural, Poor and Working-Class Student Postsecondary Experiences During the COVID-19 Pandemic: Policy Lessons Learned for Supporting Future College Success , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3930" spans="1:2">
       <c r="A3930" s="0">
-        <v>4393</v>
+        <v>4394</v>
       </c>
       <c r="B3930" s="0" t="inlineStr">
         <is>
-          <t>McNamee, Ty C., Ardoin, Sonja, Willis, Jenay F. E. (2024). Rural, Poor and Working-Class Student Postsecondary Experiences During the COVID-19 Pandemic: Policy Lessons Learned for Supporting Future College Success , 45(), . </t>
+          <t>O'Brien, Dani, Montgomery, Josh, Hunter, Bezhigogaabawiikwe, Howes, Niizhoobinesiikwe, Gonzalez, Waasegiizhigookwe Rosie, Makwe Ikwe, Manidoo, Zak, Kevin (2024). Seasons of Learning: Rural Indigenous Teacher Preparation , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3931" spans="1:2">
       <c r="A3931" s="0">
-        <v>4394</v>
+        <v>4395</v>
       </c>
       <c r="B3931" s="0" t="inlineStr">
         <is>
-          <t>O'Brien, Dani, Montgomery, Josh, Hunter, Bezhigogaabawiikwe, Howes, Niizhoobinesiikwe, Gonzalez, Waasegiizhigookwe Rosie, Makwe Ikwe, Manidoo, Zak, Kevin (2024). Seasons of Learning: Rural Indigenous Teacher Preparation , 45(), . </t>
+          <t>Whitlow, Carrie F. (2024). From Theory to Practice: How the Cheyenne and Arapaho Department of Education (Re)Centered Indian Education in Western Rural Oklahoma , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3932" spans="1:2">
       <c r="A3932" s="0">
-        <v>4395</v>
+        <v>4396</v>
       </c>
       <c r="B3932" s="0" t="inlineStr">
         <is>
-          <t>Whitlow, Carrie F. (2024). From Theory to Practice: How the Cheyenne and Arapaho Department of Education (Re)Centered Indian Education in Western Rural Oklahoma , 45(), . </t>
+          <t>RedCorn, Alex, Sutherland, Daniella, Lees, Anna, Chesley-Park, Mandy, Redeagle, Braxton (2024). Introduction to Joint Special Issue Between The Rural Educator and Journal of American Indian Education Collaboration: Issue 1 , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3933" spans="1:2">
       <c r="A3933" s="0">
-        <v>4396</v>
+        <v>4397</v>
       </c>
       <c r="B3933" s="0" t="inlineStr">
         <is>
-          <t>RedCorn, Alex, Sutherland, Daniella, Lees, Anna, Chesley-Park, Mandy, Redeagle, Braxton (2024). Introduction to Joint Special Issue Between The Rural Educator and Journal of American Indian Education Collaboration: Issue 1 , 45(), . </t>
+          <t>Stone, Jana, Ferguson, Carinna, Boulden, Rawn (2024). Culturally Conflicted: Women in Rural Appalachian School Leadership , 45(), . </t>
         </is>
       </c>
     </row>
     <row r="3934" spans="1:2">
       <c r="A3934" s="0">
-        <v>4397</v>
+        <v>4398</v>
       </c>
       <c r="B3934" s="0" t="inlineStr">
         <is>
-          <t>Stone, Jana, Ferguson, Carinna, Boulden, Rawn (2024). Culturally Conflicted: Women in Rural Appalachian School Leadership , 45(), . </t>
+          <t>Wenze, Susan J, Charles, Thalia K (2024/07//). Earlier Start Time for an Undergraduate Introductory Psychology Course is Associated with Worse Academic and Sleep-Related Outcomes Teaching of Psychology, 51(3), 277. https://doi.org/10.1177/00986283221103473</t>
         </is>
       </c>
     </row>
     <row r="3935" spans="1:2">
       <c r="A3935" s="0">
-        <v>4398</v>
+        <v>4399</v>
       </c>
       <c r="B3935" s="0" t="inlineStr">
         <is>
-          <t>Wenze, Susan J, Charles, Thalia K (2024/07//). Earlier Start Time for an Undergraduate Introductory Psychology Course is Associated with Worse Academic and Sleep-Related Outcomes Teaching of Psychology, 51(3), 277. https://doi.org/10.1177/00986283221103473</t>
+          <t> (2024/06/17/). OU Norman campus to cancel class, operations on first football game day University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3936" spans="1:2">
       <c r="A3936" s="0">
-        <v>4399</v>
+        <v>4400</v>
       </c>
       <c r="B3936" s="0" t="inlineStr">
         <is>
-          <t> (2024/06/17/). OU Norman campus to cancel class, operations on first football game day University Wire, (), . </t>
+          <t>Gómez, Jessie, Carrera, Catherine (2024/06/07/). Chalkbeat: Newark Teachers Union ratifies new contract with 4.5% average annual raises, extended workday Chalkbeat, (), . </t>
         </is>
       </c>
     </row>
     <row r="3937" spans="1:2">
       <c r="A3937" s="0">
-        <v>4400</v>
+        <v>4401</v>
       </c>
       <c r="B3937" s="0" t="inlineStr">
         <is>
-          <t>Gómez, Jessie, Carrera, Catherine (2024/06/07/). Chalkbeat: Newark Teachers Union ratifies new contract with 4.5% average annual raises, extended workday Chalkbeat, (), . </t>
+          <t>Naysmith, Emma (2024/06/05/). Must-have apps for success as a Penn State student University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3938" spans="1:2">
       <c r="A3938" s="0">
-        <v>4401</v>
+        <v>4402</v>
       </c>
       <c r="B3938" s="0" t="inlineStr">
         <is>
-          <t>Naysmith, Emma (2024/06/05/). Must-have apps for success as a Penn State student University Wire, (), . </t>
+          <t>Anonymous (2024/06//). READER REPLY School Administrator, 81(6), 4. </t>
         </is>
       </c>
     </row>
     <row r="3939" spans="1:2">
       <c r="A3939" s="0">
-        <v>4402</v>
+        <v>4403</v>
       </c>
       <c r="B3939" s="0" t="inlineStr">
         <is>
-          <t>Anonymous (2024/06//). READER REPLY School Administrator, 81(6), 4. </t>
+          <t>Messner, Kate (2024/06//). An Epic Collaboration: How To Create An 18-Book Series With 16 Authors School Library Journal, 70(6), 16. </t>
         </is>
       </c>
     </row>
     <row r="3940" spans="1:2">
       <c r="A3940" s="0">
-        <v>4403</v>
+        <v>4404</v>
       </c>
       <c r="B3940" s="0" t="inlineStr">
         <is>
-          <t>Messner, Kate (2024/06//). An Epic Collaboration: How To Create An 18-Book Series With 16 Authors School Library Journal, 70(6), 16. </t>
+          <t>Basil, Madelon, Hammer, Katherine (2024///Jun/Jul). 5 SUMMER LOVE RULES TO LIVE BY Girls' Life, 30(6), 44. </t>
         </is>
       </c>
     </row>
     <row r="3941" spans="1:2">
       <c r="A3941" s="0">
-        <v>4404</v>
+        <v>4405</v>
       </c>
       <c r="B3941" s="0" t="inlineStr">
         <is>
-          <t>Basil, Madelon, Hammer, Katherine (2024///Jun/Jul). 5 SUMMER LOVE RULES TO LIVE BY Girls' Life, 30(6), 44. </t>
+          <t>Zimmer, Amy (2024/05/28/). Chalkbeat: NYC schools have a 1-day week before winter break. This student is trying to change that. Chalkbeat, (), . </t>
         </is>
       </c>
     </row>
     <row r="3942" spans="1:2">
       <c r="A3942" s="0">
-        <v>4405</v>
+        <v>4406</v>
       </c>
       <c r="B3942" s="0" t="inlineStr">
         <is>
-          <t>Zimmer, Amy (2024/05/28/). Chalkbeat: NYC schools have a 1-day week before winter break. This student is trying to change that. Chalkbeat, (), . </t>
+          <t>Moyse, Eli (2024/05/16/). Moyse: President Beilock’s Optics Obsession - The Dartmouth University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3943" spans="1:2">
       <c r="A3943" s="0">
-        <v>4406</v>
+        <v>4407</v>
       </c>
       <c r="B3943" s="0" t="inlineStr">
         <is>
-          <t>Moyse, Eli (2024/05/16/). Moyse: President Beilock’s Optics Obsession - The Dartmouth University Wire, (), . </t>
+          <t> (2024/05/14/). NPS Board of Education discusses Norman North football stadium updates, revises 2024-25 calendar University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3944" spans="1:2">
       <c r="A3944" s="0">
-        <v>4407</v>
+        <v>4408</v>
       </c>
       <c r="B3944" s="0" t="inlineStr">
         <is>
-          <t> (2024/05/14/). NPS Board of Education discusses Norman North football stadium updates, revises 2024-25 calendar University Wire, (), . </t>
+          <t>Bogat, G Anne, McCartney, Kathleen, Repetti, Rena (2024/05/10/). You Don’t Have to Mull the Retirement Question Alone: Three professors share lessons learned from joining a support group to “workshop” the decision on when to retire. Pat Kinsella for The Chronicle The Chronicle of Higher Education, (), . </t>
         </is>
       </c>
     </row>
     <row r="3945" spans="1:2">
       <c r="A3945" s="0">
-        <v>4408</v>
+        <v>4409</v>
       </c>
       <c r="B3945" s="0" t="inlineStr">
         <is>
-          <t>Bogat, G Anne, McCartney, Kathleen, Repetti, Rena (2024/05/10/). You Don’t Have to Mull the Retirement Question Alone: Three professors share lessons learned from joining a support group to “workshop” the decision on when to retire. Pat Kinsella for The Chronicle The Chronicle of Higher Education, (), . </t>
+          <t> (2024/05/07/). Class of 2024 appreciates graduation experience - The Daily Iowan University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3946" spans="1:2">
       <c r="A3946" s="0">
-        <v>4409</v>
+        <v>4410</v>
       </c>
       <c r="B3946" s="0" t="inlineStr">
         <is>
-          <t> (2024/05/07/). Class of 2024 appreciates graduation experience - The Daily Iowan University Wire, (), . </t>
+          <t> (2024/05/06/). Graduating students face apartment move-out challenges University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3947" spans="1:2">
       <c r="A3947" s="0">
-        <v>4410</v>
+        <v>4411</v>
       </c>
       <c r="B3947" s="0" t="inlineStr">
         <is>
-          <t> (2024/05/06/). Graduating students face apartment move-out challenges University Wire, (), . </t>
+          <t> (2024/05/06/). Student moms work to balance school, parenting - KentWired University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3948" spans="1:2">
       <c r="A3948" s="0">
-        <v>4411</v>
+        <v>4412</v>
       </c>
       <c r="B3948" s="0" t="inlineStr">
         <is>
-          <t> (2024/05/06/). Student moms work to balance school, parenting - KentWired University Wire, (), . </t>
+          <t>Barry, Liv (2024/05/02/). Cancellation of reading day points to lack of attention to student interest University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3949" spans="1:2">
       <c r="A3949" s="0">
-        <v>4412</v>
+        <v>4413</v>
       </c>
       <c r="B3949" s="0" t="inlineStr">
         <is>
-          <t>Barry, Liv (2024/05/02/). Cancellation of reading day points to lack of attention to student interest University Wire, (), . </t>
+          <t>Barry, Liv (2024/05/02/). Reading days swapped for national holidays University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3950" spans="1:2">
       <c r="A3950" s="0">
-        <v>4413</v>
+        <v>4414</v>
       </c>
       <c r="B3950" s="0" t="inlineStr">
         <is>
-          <t>Barry, Liv (2024/05/02/). Reading days swapped for national holidays University Wire, (), . </t>
+          <t>Anonymous (2024/05//). BITS &amp; PIECES School Administrator, 81(5), 50. </t>
         </is>
       </c>
     </row>
     <row r="3951" spans="1:2">
       <c r="A3951" s="0">
-        <v>4414</v>
+        <v>4415</v>
       </c>
       <c r="B3951" s="0" t="inlineStr">
         <is>
-          <t>Anonymous (2024/05//). BITS &amp; PIECES School Administrator, 81(5), 50. </t>
+          <t>Kirschner, Paul A (2024/05/01/). 3-Star Learning Experiences - Automattic Inc.: 4 X 1,25 ≠ 5 3-Star Learning Experiences [Blog], (), . </t>
         </is>
       </c>
     </row>
     <row r="3952" spans="1:2">
       <c r="A3952" s="0">
-        <v>4415</v>
+        <v>4416</v>
       </c>
       <c r="B3952" s="0" t="inlineStr">
         <is>
-          <t>Kirschner, Paul A (2024/05/01/). 3-Star Learning Experiences - Automattic Inc.: 4 X 1,25 ≠ 5 3-Star Learning Experiences [Blog], (), . </t>
+          <t> (2024/04/30/). Iowa track and field's Lizzy Korczak embarks on a journey with the javelin - The Daily Iowan University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3953" spans="1:2">
       <c r="A3953" s="0">
-        <v>4416</v>
+        <v>4417</v>
       </c>
       <c r="B3953" s="0" t="inlineStr">
         <is>
-          <t> (2024/04/30/). Iowa track and field's Lizzy Korczak embarks on a journey with the javelin - The Daily Iowan University Wire, (), . </t>
+          <t>Sugarman, Sierra (2024/04/30/). Candidates reflect on DSG election and campaign process - The Dartmouth University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3954" spans="1:2">
       <c r="A3954" s="0">
-        <v>4417</v>
+        <v>4418</v>
       </c>
       <c r="B3954" s="0" t="inlineStr">
         <is>
-          <t>Sugarman, Sierra (2024/04/30/). Candidates reflect on DSG election and campaign process - The Dartmouth University Wire, (), . </t>
+          <t>Petraske, Michael (2024/04/25/). Women's track earn top three finish at Holy Cross University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3955" spans="1:2">
       <c r="A3955" s="0">
-        <v>4418</v>
+        <v>4419</v>
       </c>
       <c r="B3955" s="0" t="inlineStr">
         <is>
-          <t>Petraske, Michael (2024/04/25/). Women's track earn top three finish at Holy Cross University Wire, (), . </t>
+          <t>Shillue, Tom, Timpf, Kat, Tyrus, Benson, Guy (2024/04/24/). George Washington's 250-Year-Old Cherries Found Buried At Mount Vernon; Nine-Year-Old 'Seagull Boy' Takes Top Spot In European Screeching Contest; Millennials Are Ready For A Four-Day Week; Cocaine Inside Louisiana Kindergartener's School Cubby Leads To Metairic Mom's Arrest; Trump Defends White-Nationalist Protesters: 'Some Very Fine People On Both Sides'; College Students Attending Southern Schools In Larger Numbers; Protests At College Campuses In U.S. Over Israel-Hamas War Draw Controversy; Ohio Company Creates Flame-Throwing Robotic Dog; Transportation Department Announces New Rule Forcing Airlines To Automatically Give Refunds For Delayed Or Canceled Flights The Greg Gutfeld Show, (), . </t>
         </is>
       </c>
     </row>
     <row r="3956" spans="1:2">
       <c r="A3956" s="0">
-        <v>4419</v>
+        <v>4420</v>
       </c>
       <c r="B3956" s="0" t="inlineStr">
         <is>
-          <t>Shillue, Tom, Timpf, Kat, Tyrus, Benson, Guy (2024/04/24/). George Washington's 250-Year-Old Cherries Found Buried At Mount Vernon; Nine-Year-Old 'Seagull Boy' Takes Top Spot In European Screeching Contest; Millennials Are Ready For A Four-Day Week; Cocaine Inside Louisiana Kindergartener's School Cubby Leads To Metairic Mom's Arrest; Trump Defends White-Nationalist Protesters: 'Some Very Fine People On Both Sides'; College Students Attending Southern Schools In Larger Numbers; Protests At College Campuses In U.S. Over Israel-Hamas War Draw Controversy; Ohio Company Creates Flame-Throwing Robotic Dog; Transportation Department Announces New Rule Forcing Airlines To Automatically Give Refunds For Delayed Or Canceled Flights The Greg Gutfeld Show, (), . </t>
+          <t>Repkin, Jacob (2024/04/24/). It’s time to close the social distance in higher education – The Mesa Press University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3957" spans="1:2">
       <c r="A3957" s="0">
-        <v>4420</v>
+        <v>4421</v>
       </c>
       <c r="B3957" s="0" t="inlineStr">
         <is>
-          <t>Repkin, Jacob (2024/04/24/). It’s time to close the social distance in higher education – The Mesa Press University Wire, (), . </t>
+          <t>Smith, Rebecca (2024/04/22/). Stanford in Style: Spring has sprung Login or create an account University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3958" spans="1:2">
       <c r="A3958" s="0">
-        <v>4421</v>
+        <v>4422</v>
       </c>
       <c r="B3958" s="0" t="inlineStr">
         <is>
-          <t>Smith, Rebecca (2024/04/22/). Stanford in Style: Spring has sprung Login or create an account University Wire, (), . </t>
+          <t> (2024/04/19/). No days off: Study day goes missing from academic calendar – THE CHANTICLEER University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3959" spans="1:2">
       <c r="A3959" s="0">
-        <v>4422</v>
+        <v>4423</v>
       </c>
       <c r="B3959" s="0" t="inlineStr">
         <is>
-          <t> (2024/04/19/). No days off: Study day goes missing from academic calendar – THE CHANTICLEER University Wire, (), . </t>
+          <t>Davies, Victoria (2024/04/17/). Extended passing times follow changes to finals period and Dean's Date University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3960" spans="1:2">
       <c r="A3960" s="0">
-        <v>4423</v>
+        <v>4424</v>
       </c>
       <c r="B3960" s="0" t="inlineStr">
         <is>
-          <t>Davies, Victoria (2024/04/17/). Extended passing times follow changes to finals period and Dean's Date University Wire, (), . </t>
+          <t>Christina Zhang Alexis Spector (2024/04/15/). A day in the life of a Law School student University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3961" spans="1:2">
       <c r="A3961" s="0">
-        <v>4424</v>
+        <v>4425</v>
       </c>
       <c r="B3961" s="0" t="inlineStr">
         <is>
-          <t>Christina Zhang Alexis Spector (2024/04/15/). A day in the life of a Law School student University Wire, (), . </t>
+          <t>Asmar, Melanie (2024/04/12/). Chalkbeat: School lunch time is too short. Colorado lawmakers solution? A task force to make recommendations. Chalkbeat, (), . </t>
         </is>
       </c>
     </row>
     <row r="3962" spans="1:2">
       <c r="A3962" s="0">
-        <v>4425</v>
+        <v>4426</v>
       </c>
       <c r="B3962" s="0" t="inlineStr">
         <is>
-          <t>Asmar, Melanie (2024/04/12/). Chalkbeat: School lunch time is too short. Colorado lawmakers solution? A task force to make recommendations. Chalkbeat, (), . </t>
+          <t> (2024/04/12/). Zaki announces timing changes to new student orientation schedule University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3963" spans="1:2">
       <c r="A3963" s="0">
-        <v>4426</v>
+        <v>4427</v>
       </c>
       <c r="B3963" s="0" t="inlineStr">
         <is>
-          <t> (2024/04/12/). Zaki announces timing changes to new student orientation schedule University Wire, (), . </t>
+          <t> (2024/04/10/). Strides have been made since Cesar Chavez, but there is more to be done University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3964" spans="1:2">
       <c r="A3964" s="0">
-        <v>4427</v>
+        <v>4428</v>
       </c>
       <c r="B3964" s="0" t="inlineStr">
         <is>
-          <t> (2024/04/10/). Strides have been made since Cesar Chavez, but there is more to be done University Wire, (), . </t>
+          <t> (2024/04/10/). Meet the new 24-25 SGA ticket  University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3965" spans="1:2">
       <c r="A3965" s="0">
-        <v>4428</v>
+        <v>4429</v>
       </c>
       <c r="B3965" s="0" t="inlineStr">
         <is>
-          <t> (2024/04/10/). Meet the new 24-25 SGA ticket  University Wire, (), . </t>
+          <t> (2024/04/09/). Spring plant sale rewards season of student efforts University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3966" spans="1:2">
       <c r="A3966" s="0">
-        <v>4429</v>
+        <v>4430</v>
       </c>
       <c r="B3966" s="0" t="inlineStr">
         <is>
-          <t> (2024/04/09/). Spring plant sale rewards season of student efforts University Wire, (), . </t>
+          <t> (2024/04/05/). North Westwood Neighborhood Council recap - April 3 University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3967" spans="1:2">
       <c r="A3967" s="0">
-        <v>4430</v>
+        <v>4431</v>
       </c>
       <c r="B3967" s="0" t="inlineStr">
         <is>
-          <t> (2024/04/05/). North Westwood Neighborhood Council recap - April 3 University Wire, (), . </t>
+          <t> (2024/04/05/). Faculty assembly discusses calendar changes, campus renovations - The Pitt News University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3968" spans="1:2">
       <c r="A3968" s="0">
-        <v>4431</v>
+        <v>4432</v>
       </c>
       <c r="B3968" s="0" t="inlineStr">
         <is>
-          <t> (2024/04/05/). Faculty assembly discusses calendar changes, campus renovations - The Pitt News University Wire, (), . </t>
+          <t>Sones, Lily (2024/04/04/). Barnard Seniors Demand Recognition of "Palestinian Genocide" &amp; Divestment From President Rosenbury - Barnard Bulletin University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3969" spans="1:2">
       <c r="A3969" s="0">
-        <v>4432</v>
+        <v>4433</v>
       </c>
       <c r="B3969" s="0" t="inlineStr">
         <is>
-          <t>Sones, Lily (2024/04/04/). Barnard Seniors Demand Recognition of "Palestinian Genocide" &amp; Divestment From President Rosenbury - Barnard Bulletin University Wire, (), . </t>
+          <t>Botkin, Rachel (2024/04/04/). ODEI Leadership Fellowship Program to launch in fall 2024 University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3970" spans="1:2">
       <c r="A3970" s="0">
-        <v>4433</v>
+        <v>4434</v>
       </c>
       <c r="B3970" s="0" t="inlineStr">
         <is>
-          <t>Botkin, Rachel (2024/04/04/). ODEI Leadership Fellowship Program to launch in fall 2024 University Wire, (), . </t>
+          <t>Haslun, John (2024/04/03/). UConn COP29 applications for 2024 open after last year’s cancellation  | The Daily Campus University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3971" spans="1:2">
       <c r="A3971" s="0">
-        <v>4434</v>
+        <v>4435</v>
       </c>
       <c r="B3971" s="0" t="inlineStr">
         <is>
-          <t>Haslun, John (2024/04/03/). UConn COP29 applications for 2024 open after last year’s cancellation  | The Daily Campus University Wire, (), . </t>
+          <t>Stubbs, Anna (2024/04/02/). Massoni, Rost-Nasshan take the stage for Grand Marshal runoff University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3972" spans="1:2">
       <c r="A3972" s="0">
-        <v>4435</v>
+        <v>4436</v>
       </c>
       <c r="B3972" s="0" t="inlineStr">
         <is>
-          <t>Stubbs, Anna (2024/04/02/). Massoni, Rost-Nasshan take the stage for Grand Marshal runoff University Wire, (), . </t>
+          <t> (2024/04/01/). The highs and lows of being a residential assistant University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3973" spans="1:2">
       <c r="A3973" s="0">
-        <v>4436</v>
+        <v>4437</v>
       </c>
       <c r="B3973" s="0" t="inlineStr">
         <is>
-          <t> (2024/04/01/). The highs and lows of being a residential assistant University Wire, (), . </t>
+          <t> (2024/04//). Poll Points: Public perceptions of teacher working conditions Phi Delta Kappan, 105(7), 72. https://doi.org/10.1177/00317217241244915</t>
         </is>
       </c>
     </row>
     <row r="3974" spans="1:2">
       <c r="A3974" s="0">
-        <v>4437</v>
+        <v>4438</v>
       </c>
       <c r="B3974" s="0" t="inlineStr">
         <is>
-          <t> (2024/04//). Poll Points: Public perceptions of teacher working conditions Phi Delta Kappan, 105(7), 72. https://doi.org/10.1177/00317217241244915</t>
+          <t>Goode, Elizabeth, Syme, Suzi, Nieuwoudt, Johanna E (2024/04//). The impact of immersive scheduling on student learning and success in an Australian pathways program: Journal of the Association for Programmed Learning Innovations in Education and Teaching International, 61(2), 263. https://doi.org/10.1080/14703297.2022.2157304</t>
         </is>
       </c>
     </row>
     <row r="3975" spans="1:2">
       <c r="A3975" s="0">
-        <v>4438</v>
+        <v>4439</v>
       </c>
       <c r="B3975" s="0" t="inlineStr">
         <is>
-          <t>Goode, Elizabeth, Syme, Suzi, Nieuwoudt, Johanna E (2024/04//). The impact of immersive scheduling on student learning and success in an Australian pathways program: Journal of the Association for Programmed Learning Innovations in Education and Teaching International, 61(2), 263. https://doi.org/10.1080/14703297.2022.2157304</t>
+          <t> (2024/03/31/). The real reason Chico State parties on Chavez – The Orion University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3976" spans="1:2">
       <c r="A3976" s="0">
-        <v>4439</v>
+        <v>4440</v>
       </c>
       <c r="B3976" s="0" t="inlineStr">
         <is>
-          <t> (2024/03/31/). The real reason Chico State parties on Chavez – The Orion University Wire, (), . </t>
+          <t> (2024/03/29/). Plarn: A Service-Learning Project Helps the Homeless - Eagle Media University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3977" spans="1:2">
       <c r="A3977" s="0">
-        <v>4440</v>
+        <v>4441</v>
       </c>
       <c r="B3977" s="0" t="inlineStr">
         <is>
-          <t> (2024/03/29/). Plarn: A Service-Learning Project Helps the Homeless - Eagle Media University Wire, (), . </t>
+          <t> (2024/03/28/). Toto, we're not in Miami anymore. We're in misery. University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3978" spans="1:2">
       <c r="A3978" s="0">
-        <v>4441</v>
+        <v>4442</v>
       </c>
       <c r="B3978" s="0" t="inlineStr">
         <is>
-          <t> (2024/03/28/). Toto, we're not in Miami anymore. We're in misery. University Wire, (), . </t>
+          <t> (2024/03/28/). Faculty Senate strikes down wellness days University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3979" spans="1:2">
       <c r="A3979" s="0">
-        <v>4442</v>
+        <v>4443</v>
       </c>
       <c r="B3979" s="0" t="inlineStr">
         <is>
-          <t> (2024/03/28/). Faculty Senate strikes down wellness days University Wire, (), . </t>
+          <t>Lee, Ethan (2024/03/28/). Play(er) of the Week: James Marsden ’26 Talks Early Baseball Memories, Spring Hot Streak, and the Cardinals’ Winning Mentality University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3980" spans="1:2">
       <c r="A3980" s="0">
-        <v>4443</v>
+        <v>4444</v>
       </c>
       <c r="B3980" s="0" t="inlineStr">
         <is>
-          <t>Lee, Ethan (2024/03/28/). Play(er) of the Week: James Marsden ’26 Talks Early Baseball Memories, Spring Hot Streak, and the Cardinals’ Winning Mentality University Wire, (), . </t>
+          <t>Show-Me Institute, Missouri (2024/03/27/). How Will the Four-day School Week Progress in Light of SB 727? CE Think Tank Newswire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3981" spans="1:2">
       <c r="A3981" s="0">
-        <v>4444</v>
+        <v>4445</v>
       </c>
       <c r="B3981" s="0" t="inlineStr">
         <is>
-          <t>Show-Me Institute, Missouri (2024/03/27/). How Will the Four-day School Week Progress in Light of SB 727? CE Think Tank Newswire, (), . </t>
+          <t>Rhodes, Shanley (2024/03/25/). Chalkbeat: I turned my kitchen table into a classroom. Then I took the idea schoolwide. Chalkbeat, (), . </t>
         </is>
       </c>
     </row>
     <row r="3982" spans="1:2">
       <c r="A3982" s="0">
-        <v>4445</v>
+        <v>4446</v>
       </c>
       <c r="B3982" s="0" t="inlineStr">
         <is>
-          <t>Rhodes, Shanley (2024/03/25/). Chalkbeat: I turned my kitchen table into a classroom. Then I took the idea schoolwide. Chalkbeat, (), . </t>
+          <t>Robles, Yesenia (2024/03/23/). Chalkbeat: Colorado will allow some of this years new migrant students to skip state tests Chalkbeat, (), . </t>
         </is>
       </c>
     </row>
     <row r="3983" spans="1:2">
       <c r="A3983" s="0">
-        <v>4446</v>
+        <v>4447</v>
       </c>
       <c r="B3983" s="0" t="inlineStr">
         <is>
-          <t>Robles, Yesenia (2024/03/23/). Chalkbeat: Colorado will allow some of this years new migrant students to skip state tests Chalkbeat, (), . </t>
+          <t>Probert, Katie (2024/03/22/). ‘You’re a derby girl now:’ student finds community through roller derby University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3984" spans="1:2">
       <c r="A3984" s="0">
-        <v>4447</v>
+        <v>4448</v>
       </c>
       <c r="B3984" s="0" t="inlineStr">
         <is>
-          <t>Probert, Katie (2024/03/22/). ‘You’re a derby girl now:’ student finds community through roller derby University Wire, (), . </t>
+          <t>Zetzer, Rian (2024/03/22/). Students express mixed feelings about removal of Fall break University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3985" spans="1:2">
       <c r="A3985" s="0">
-        <v>4448</v>
+        <v>4449</v>
       </c>
       <c r="B3985" s="0" t="inlineStr">
         <is>
-          <t>Zetzer, Rian (2024/03/22/). Students express mixed feelings about removal of Fall break University Wire, (), . </t>
+          <t>Gamble, Nicole (2024/03/22/). Seniors: Plan to graduate with honors? University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3986" spans="1:2">
       <c r="A3986" s="0">
-        <v>4449</v>
+        <v>4450</v>
       </c>
       <c r="B3986" s="0" t="inlineStr">
         <is>
-          <t>Gamble, Nicole (2024/03/22/). Seniors: Plan to graduate with honors? University Wire, (), . </t>
+          <t>Mondeaux, Cami (2024/03/22/). Westminster is returning to campus in the fall — but it won’t look the same University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3987" spans="1:2">
       <c r="A3987" s="0">
-        <v>4450</v>
+        <v>4451</v>
       </c>
       <c r="B3987" s="0" t="inlineStr">
         <is>
-          <t>Mondeaux, Cami (2024/03/22/). Westminster is returning to campus in the fall — but it won’t look the same University Wire, (), . </t>
+          <t>Cushing, Maddie (2024/03/22/). Lucy Wilks shares dog training tips and experiences University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3988" spans="1:2">
       <c r="A3988" s="0">
-        <v>4451</v>
+        <v>4452</v>
       </c>
       <c r="B3988" s="0" t="inlineStr">
         <is>
-          <t>Cushing, Maddie (2024/03/22/). Lucy Wilks shares dog training tips and experiences University Wire, (), . </t>
+          <t>Daly, Jaclyn (2024/03/22/). How to ease the transition to online classes University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3989" spans="1:2">
       <c r="A3989" s="0">
-        <v>4452</v>
+        <v>4453</v>
       </c>
       <c r="B3989" s="0" t="inlineStr">
         <is>
-          <t>Daly, Jaclyn (2024/03/22/). How to ease the transition to online classes University Wire, (), . </t>
+          <t>Mangum, Abby (2024/03/22/). OPINION: Unpaid internships need to take a back seat University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3990" spans="1:2">
       <c r="A3990" s="0">
-        <v>4453</v>
+        <v>4454</v>
       </c>
       <c r="B3990" s="0" t="inlineStr">
         <is>
-          <t>Mangum, Abby (2024/03/22/). OPINION: Unpaid internships need to take a back seat University Wire, (), . </t>
+          <t> (2024/03/22/). ASW creates religious and cultural holiday observance policy University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3991" spans="1:2">
       <c r="A3991" s="0">
-        <v>4454</v>
+        <v>4455</v>
       </c>
       <c r="B3991" s="0" t="inlineStr">
         <is>
-          <t> (2024/03/22/). ASW creates religious and cultural holiday observance policy University Wire, (), . </t>
+          <t> (2024/03/22/). Griffin Editorial 3/22 University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3992" spans="1:2">
       <c r="A3992" s="0">
-        <v>4455</v>
+        <v>4456</v>
       </c>
       <c r="B3992" s="0" t="inlineStr">
         <is>
-          <t> (2024/03/22/). Griffin Editorial 3/22 University Wire, (), . </t>
+          <t>Green, Ava C (2024/03/22/). Ask Ava! University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3993" spans="1:2">
       <c r="A3993" s="0">
-        <v>4456</v>
+        <v>4457</v>
       </c>
       <c r="B3993" s="0" t="inlineStr">
         <is>
-          <t>Green, Ava C (2024/03/22/). Ask Ava! University Wire, (), . </t>
+          <t>Piteo, Colin (2024/03/21/). Looking to reschedule a final? Here’s how   | The Daily Campus University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3994" spans="1:2">
       <c r="A3994" s="0">
-        <v>4457</v>
+        <v>4458</v>
       </c>
       <c r="B3994" s="0" t="inlineStr">
         <is>
-          <t>Piteo, Colin (2024/03/21/). Looking to reschedule a final? Here’s how   | The Daily Campus University Wire, (), . </t>
+          <t>Rutherford, Piper (2024/03/19/). Beyond the egg hunts: Spiritual Life staff reflect on meaning of Easter University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3995" spans="1:2">
       <c r="A3995" s="0">
-        <v>4458</v>
+        <v>4459</v>
       </c>
       <c r="B3995" s="0" t="inlineStr">
         <is>
-          <t>Rutherford, Piper (2024/03/19/). Beyond the egg hunts: Spiritual Life staff reflect on meaning of Easter University Wire, (), . </t>
+          <t>Pastor, Manuela (2024/03/15/). Study abroad to inspire your education University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3996" spans="1:2">
       <c r="A3996" s="0">
-        <v>4459</v>
+        <v>4460</v>
       </c>
       <c r="B3996" s="0" t="inlineStr">
         <is>
-          <t>Pastor, Manuela (2024/03/15/). Study abroad to inspire your education University Wire, (), . </t>
+          <t> (2024/03/14/). Total Solar Eclipse: The Celestial challenges - BG Falcon Media University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3997" spans="1:2">
       <c r="A3997" s="0">
-        <v>4460</v>
+        <v>4461</v>
       </c>
       <c r="B3997" s="0" t="inlineStr">
         <is>
-          <t> (2024/03/14/). Total Solar Eclipse: The Celestial challenges - BG Falcon Media University Wire, (), . </t>
+          <t>Beekman, Madison (2024/03/13/). Euforia Italiana University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3998" spans="1:2">
       <c r="A3998" s="0">
-        <v>4461</v>
+        <v>4462</v>
       </c>
       <c r="B3998" s="0" t="inlineStr">
         <is>
-          <t>Beekman, Madison (2024/03/13/). Euforia Italiana University Wire, (), . </t>
+          <t>Chipperfield, Eden (2024/03/12/). Council Chats: motion for SFSS petition for fall reading break passes University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="3999" spans="1:2">
       <c r="A3999" s="0">
-        <v>4462</v>
+        <v>4463</v>
       </c>
       <c r="B3999" s="0" t="inlineStr">
         <is>
-          <t>Chipperfield, Eden (2024/03/12/). Council Chats: motion for SFSS petition for fall reading break passes University Wire, (), . </t>
+          <t>Fandino, Sophia (2024/03/06/). Student Center gets steamy for RAH’s ‘Night of Sex’ University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4000" spans="1:2">
       <c r="A4000" s="0">
-        <v>4463</v>
+        <v>4464</v>
       </c>
       <c r="B4000" s="0" t="inlineStr">
         <is>
-          <t>Fandino, Sophia (2024/03/06/). Student Center gets steamy for RAH’s ‘Night of Sex’ University Wire, (), . </t>
+          <t>Carranza, Ashley (2024/03/05/). Hunting for housing University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4001" spans="1:2">
       <c r="A4001" s="0">
-        <v>4464</v>
+        <v>4465</v>
       </c>
       <c r="B4001" s="0" t="inlineStr">
         <is>
-          <t>Carranza, Ashley (2024/03/05/). Hunting for housing University Wire, (), . </t>
+          <t>Bomeny, Carolina (2024/03/03/). Old legacies, new approaches: Reworked diversity requirement to take effect next year University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4002" spans="1:2">
       <c r="A4002" s="0">
-        <v>4465</v>
+        <v>4467</v>
       </c>
       <c r="B4002" s="0" t="inlineStr">
         <is>
-          <t>Bomeny, Carolina (2024/03/03/). Old legacies, new approaches: Reworked diversity requirement to take effect next year University Wire, (), . </t>
+          <t>Network, digitalLEARNING (2024/03//). UGC chairman announces increasing university enrollment in CUET UG for admissions Digital Learning, (), . </t>
         </is>
       </c>
     </row>
     <row r="4003" spans="1:2">
       <c r="A4003" s="0">
-        <v>4467</v>
+        <v>4468</v>
       </c>
       <c r="B4003" s="0" t="inlineStr">
         <is>
-          <t>Network, digitalLEARNING (2024/03//). UGC chairman announces increasing university enrollment in CUET UG for admissions Digital Learning, (), . </t>
+          <t>Hall, Sarah Lindenfeld (2024/03//). Embracing the Four-Day School Week School Administrator, 81(3), 16. </t>
         </is>
       </c>
     </row>
     <row r="4004" spans="1:2">
       <c r="A4004" s="0">
-        <v>4468</v>
+        <v>4469</v>
       </c>
       <c r="B4004" s="0" t="inlineStr">
         <is>
-          <t>Hall, Sarah Lindenfeld (2024/03//). Embracing the Four-Day School Week School Administrator, 81(3), 16. </t>
+          <t>Patterson, Paula (2024/03//). Why We Transitioned to a Four-Day Week School Administrator, 81(3), 19. </t>
         </is>
       </c>
     </row>
     <row r="4005" spans="1:2">
       <c r="A4005" s="0">
-        <v>4469</v>
+        <v>4470</v>
       </c>
       <c r="B4005" s="0" t="inlineStr">
         <is>
-          <t>Patterson, Paula (2024/03//). Why We Transitioned to a Four-Day Week School Administrator, 81(3), 19. </t>
+          <t>Hall, Sarah (2024/03//). What to Consider About Moving to a Four-Day Week School Administrator, 81(3), 20. </t>
         </is>
       </c>
     </row>
     <row r="4006" spans="1:2">
       <c r="A4006" s="0">
-        <v>4470</v>
+        <v>4471</v>
       </c>
       <c r="B4006" s="0" t="inlineStr">
         <is>
-          <t>Hall, Sarah (2024/03//). What to Consider About Moving to a Four-Day Week School Administrator, 81(3), 20. </t>
+          <t>O’Malley, Meagan D., Greene, Jeremy D., Chima, Gurminder, Martinez, Celeste A., Arciga, Mariana Vargas, Yates, Heather (2024/03//). Our COVID Stories: Adolescents Drawing Meaning from a Public Health Crisis Through a Youth Voice Intervention Contemporary School Psychology, 28(1), 97. https://doi.org/10.1007/s40688-023-00477-1</t>
         </is>
       </c>
     </row>
     <row r="4007" spans="1:2">
       <c r="A4007" s="0">
-        <v>4471</v>
+        <v>4472</v>
       </c>
       <c r="B4007" s="0" t="inlineStr">
         <is>
-          <t>O’Malley, Meagan D., Greene, Jeremy D., Chima, Gurminder, Martinez, Celeste A., Arciga, Mariana Vargas, Yates, Heather (2024/03//). Our COVID Stories: Adolescents Drawing Meaning from a Public Health Crisis Through a Youth Voice Intervention Contemporary School Psychology, 28(1), 97. https://doi.org/10.1007/s40688-023-00477-1</t>
+          <t>Nathan, Linda F, Cochrane, Lydia, Hoda Ayesha (2024/03//). Big problems require big solutions Phi Delta Kappan, 105(6), 26. https://doi.org/10.1177/00317217241238104</t>
         </is>
       </c>
     </row>
     <row r="4008" spans="1:2">
       <c r="A4008" s="0">
-        <v>4472</v>
+        <v>4473</v>
       </c>
       <c r="B4008" s="0" t="inlineStr">
         <is>
-          <t>Nathan, Linda F, Cochrane, Lydia, Hoda Ayesha (2024/03//). Big problems require big solutions Phi Delta Kappan, 105(6), 26. https://doi.org/10.1177/00317217241238104</t>
+          <t>y Langer Research Associates for PDK International (2024/03//). Poll Points: What does the public think about expanding time in school? Phi Delta Kappan, 105(6), 72. https://doi.org/10.1177/00317217241238119</t>
         </is>
       </c>
     </row>
     <row r="4009" spans="1:2">
       <c r="A4009" s="0">
-        <v>4473</v>
+        <v>4474</v>
       </c>
       <c r="B4009" s="0" t="inlineStr">
         <is>
-          <t> (2024/03//). Poll Points: What does the public think about expanding time in school? Phi Delta Kappan, 105(6), 72. https://doi.org/10.1177/00317217241238119</t>
+          <t>Pelletier, Caroline (2024/03//). Against Personalised Learning International Journal of Artificial Intelligence in Education, 34(1), 111. https://doi.org/10.1007/s40593-023-00348-z</t>
         </is>
       </c>
     </row>
     <row r="4010" spans="1:2">
       <c r="A4010" s="0">
-        <v>4474</v>
+        <v>4475</v>
       </c>
       <c r="B4010" s="0" t="inlineStr">
         <is>
-          <t>Pelletier, Caroline (2024/03//). Against Personalised Learning International Journal of Artificial Intelligence in Education, 34(1), 111. https://doi.org/10.1007/s40593-023-00348-z</t>
+          <t> (2024/02/29/). Ticket troubles, schedule dilemmas: Students give take on getting in Foster Pavilion University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4011" spans="1:2">
       <c r="A4011" s="0">
-        <v>4475</v>
+        <v>4476</v>
       </c>
       <c r="B4011" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/29/). Ticket troubles, schedule dilemmas: Students give take on getting in Foster Pavilion University Wire, (), . </t>
+          <t> (2024/02/29/). Students informed of Wellness Weekend cancellation thanks to resolution by Student Association – The Racquet Press University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4012" spans="1:2">
       <c r="A4012" s="0">
-        <v>4476</v>
+        <v>4477</v>
       </c>
       <c r="B4012" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/29/). Students informed of Wellness Weekend cancellation thanks to resolution by Student Association – The Racquet Press University Wire, (), . </t>
+          <t>Donahue, Grace (2024/02/29/). Is there ‘too much’ time in the day? | Is It Just Me Or? University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4013" spans="1:2">
       <c r="A4013" s="0">
-        <v>4477</v>
+        <v>4478</v>
       </c>
       <c r="B4013" s="0" t="inlineStr">
         <is>
-          <t>Donahue, Grace (2024/02/29/). Is there ‘too much’ time in the day? | Is It Just Me Or? University Wire, (), . </t>
+          <t> (2024/02/29/). Youth sports of Pullman - The Daily Evergreen University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4014" spans="1:2">
       <c r="A4014" s="0">
-        <v>4478</v>
+        <v>4479</v>
       </c>
       <c r="B4014" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/29/). Youth sports of Pullman - The Daily Evergreen University Wire, (), . </t>
+          <t>Nuñez, Lauren (2024/02/29/). Jada Mangahas embarks on her final rotation as a Gym Devil University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4015" spans="1:2">
       <c r="A4015" s="0">
-        <v>4479</v>
+        <v>4480</v>
       </c>
       <c r="B4015" s="0" t="inlineStr">
         <is>
-          <t>Nuñez, Lauren (2024/02/29/). Jada Mangahas embarks on her final rotation as a Gym Devil University Wire, (), . </t>
+          <t>Show-Me Institute, Missouri (2024/02/28/). Considering the Four-Day School Week? Pilot It and Evaluate It CE Think Tank Newswire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4016" spans="1:2">
       <c r="A4016" s="0">
-        <v>4480</v>
+        <v>4481</v>
       </c>
       <c r="B4016" s="0" t="inlineStr">
         <is>
-          <t>Show-Me Institute, Missouri (2024/02/28/). Considering the Four-Day School Week? Pilot It and Evaluate It CE Think Tank Newswire, (), . </t>
+          <t> (2024/02/28/). Diary of a Black Girl: Jena Brown University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4017" spans="1:2">
       <c r="A4017" s="0">
-        <v>4481</v>
+        <v>4482</v>
       </c>
       <c r="B4017" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/28/). Diary of a Black Girl: Jena Brown University Wire, (), . </t>
+          <t>Rabieh, Abigail (2024/02/28/). What do academics have to do with mental health anyway? University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4018" spans="1:2">
       <c r="A4018" s="0">
-        <v>4482</v>
+        <v>4483</v>
       </c>
       <c r="B4018" s="0" t="inlineStr">
         <is>
-          <t>Rabieh, Abigail (2024/02/28/). What do academics have to do with mental health anyway? University Wire, (), . </t>
+          <t>Schmitz, Mallory (2024/02/26/). NISG elections: What you need to know – Northern Iowan University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4019" spans="1:2">
       <c r="A4019" s="0">
-        <v>4483</v>
+        <v>4484</v>
       </c>
       <c r="B4019" s="0" t="inlineStr">
         <is>
-          <t>Schmitz, Mallory (2024/02/26/). NISG elections: What you need to know – Northern Iowan University Wire, (), . </t>
+          <t> (2024/02/26/). How do Knox students celebrate Lunar New Year? - The Knox Student University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4020" spans="1:2">
       <c r="A4020" s="0">
-        <v>4484</v>
+        <v>4485</v>
       </c>
       <c r="B4020" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/26/). How do Knox students celebrate Lunar New Year? - The Knox Student University Wire, (), . </t>
+          <t>Kalo, Sonia (2024/02/26/). CUNY not to hold classes on four cultural holidays - The Ticker University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4021" spans="1:2">
       <c r="A4021" s="0">
-        <v>4485</v>
+        <v>4487</v>
       </c>
       <c r="B4021" s="0" t="inlineStr">
         <is>
-          <t>Kalo, Sonia (2024/02/26/). CUNY not to hold classes on four cultural holidays - The Ticker University Wire, (), . </t>
+          <t>Lee, Julianna (2024/02/26/). Princeton should lengthen the semester to reduce burnout University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4022" spans="1:2">
       <c r="A4022" s="0">
-        <v>4487</v>
+        <v>4488</v>
       </c>
       <c r="B4022" s="0" t="inlineStr">
         <is>
-          <t>Lee, Julianna (2024/02/26/). Princeton should lengthen the semester to reduce burnout University Wire, (), . </t>
+          <t> (2024/02/25/). Professors are responsible for improving the culture around group projects – Massachusetts Daily Collegian University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4023" spans="1:2">
       <c r="A4023" s="0">
-        <v>4488</v>
+        <v>4489</v>
       </c>
       <c r="B4023" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/25/). Professors are responsible for improving the culture around group projects – Massachusetts Daily Collegian University Wire, (), . </t>
+          <t>Lesch, Nathan (2024/02/23/). Wednesday classes impede Thanksgiving travel plans – The Observer University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4024" spans="1:2">
       <c r="A4024" s="0">
-        <v>4489</v>
+        <v>4490</v>
       </c>
       <c r="B4024" s="0" t="inlineStr">
         <is>
-          <t>Lesch, Nathan (2024/02/23/). Wednesday classes impede Thanksgiving travel plans – The Observer University Wire, (), . </t>
+          <t> (2024/02/23/). Thwing construction takes hiatus – The Observer University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4025" spans="1:2">
       <c r="A4025" s="0">
-        <v>4490</v>
+        <v>4491</v>
       </c>
       <c r="B4025" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/23/). Thwing construction takes hiatus – The Observer University Wire, (), . </t>
+          <t> (2024/02/23/). Editorial: We are exhausted – The Observer University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4026" spans="1:2">
       <c r="A4026" s="0">
-        <v>4491</v>
+        <v>4492</v>
       </c>
       <c r="B4026" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/23/). Editorial: We are exhausted – The Observer University Wire, (), . </t>
+          <t> (2024/02/23/). The Purr-fect spot in downtown Erie – THE GANNON KNIGHT University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4027" spans="1:2">
       <c r="A4027" s="0">
-        <v>4492</v>
+        <v>4493</v>
       </c>
       <c r="B4027" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/23/). The Purr-fect spot in downtown Erie – THE GANNON KNIGHT University Wire, (), . </t>
+          <t> (2024/02/23/). Coleman: Finals season: difficult but survivable – The Observer University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4028" spans="1:2">
       <c r="A4028" s="0">
-        <v>4493</v>
+        <v>4494</v>
       </c>
       <c r="B4028" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/23/). Coleman: Finals season: difficult but survivable – The Observer University Wire, (), . </t>
+          <t>Kuntzman, Caroline (2024/02/23/). Kuntzman: CWRU and Cleveland Clinic should not host an in-person presidential debate – The Observer University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4029" spans="1:2">
       <c r="A4029" s="0">
-        <v>4494</v>
+        <v>4495</v>
       </c>
       <c r="B4029" s="0" t="inlineStr">
         <is>
-          <t>Kuntzman, Caroline (2024/02/23/). Kuntzman: CWRU and Cleveland Clinic should not host an in-person presidential debate – The Observer University Wire, (), . </t>
+          <t> (2024/02/23/). Kim: Using the summer to get ahead – The Observer University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4030" spans="1:2">
       <c r="A4030" s="0">
-        <v>4495</v>
+        <v>4496</v>
       </c>
       <c r="B4030" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/23/). Kim: Using the summer to get ahead – The Observer University Wire, (), . </t>
+          <t>Shakhnovskaya, Eugenia, Ahluwalia, Lily (2024/02/22/). Are These Winged Creatures a Safety Hazard to the University’s Students? University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4031" spans="1:2">
       <c r="A4031" s="0">
-        <v>4496</v>
+        <v>4497</v>
       </c>
       <c r="B4031" s="0" t="inlineStr">
         <is>
-          <t>Shakhnovskaya, Eugenia, Ahluwalia, Lily (2024/02/22/). Are These Winged Creatures a Safety Hazard to the University’s Students? University Wire, (), . </t>
+          <t> (2024/02/22/). The rise and fall of Extended Wellness Weekend – The Racquet Press University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4032" spans="1:2">
       <c r="A4032" s="0">
-        <v>4497</v>
+        <v>4498</v>
       </c>
       <c r="B4032" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/22/). The rise and fall of Extended Wellness Weekend – The Racquet Press University Wire, (), . </t>
+          <t> (2024/02/22/). A guide to the 2024 Student Government Board election - The Pitt News University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4033" spans="1:2">
       <c r="A4033" s="0">
-        <v>4498</v>
+        <v>4499</v>
       </c>
       <c r="B4033" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/22/). A guide to the 2024 Student Government Board election - The Pitt News University Wire, (), . </t>
+          <t>Buchholz, Jonathan (2024/02/22/). Men's and women's squash has strong showing at championships University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4034" spans="1:2">
       <c r="A4034" s="0">
-        <v>4499</v>
+        <v>4500</v>
       </c>
       <c r="B4034" s="0" t="inlineStr">
         <is>
-          <t>Buchholz, Jonathan (2024/02/22/). Men's and women's squash has strong showing at championships University Wire, (), . </t>
+          <t>Blunt, Tabitha (2024/02/21/). Winter Dance Collection with choreographer Kia Smith and original work by students and faculty University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4035" spans="1:2">
       <c r="A4035" s="0">
-        <v>4500</v>
+        <v>4501</v>
       </c>
       <c r="B4035" s="0" t="inlineStr">
         <is>
-          <t>Blunt, Tabitha (2024/02/21/). Winter Dance Collection with choreographer Kia Smith and original work by students and faculty University Wire, (), . </t>
+          <t> (2024/02/19/). Snow and Ice Greet ATU's Spring Semester University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4036" spans="1:2">
       <c r="A4036" s="0">
-        <v>4501</v>
+        <v>4502</v>
       </c>
       <c r="B4036" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/19/). Snow and Ice Greet ATU's Spring Semester University Wire, (), . </t>
+          <t> (2024/02/16/). How to Apply for On-Campus Jobs University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4037" spans="1:2">
       <c r="A4037" s="0">
-        <v>4502</v>
+        <v>4503</v>
       </c>
       <c r="B4037" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/16/). How to Apply for On-Campus Jobs University Wire, (), . </t>
+          <t> (2024/02/15/). Iowa City schools add five virtual learning days to academic calendar - The Daily Iowan University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4038" spans="1:2">
       <c r="A4038" s="0">
-        <v>4503</v>
+        <v>4504</v>
       </c>
       <c r="B4038" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/15/). Iowa City schools add five virtual learning days to academic calendar - The Daily Iowan University Wire, (), . </t>
+          <t>Millenson-Wilens, Thea (2024/02/15/). Board of Trustees increases operational budget, tuition cost University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4039" spans="1:2">
       <c r="A4039" s="0">
-        <v>4504</v>
+        <v>4505</v>
       </c>
       <c r="B4039" s="0" t="inlineStr">
         <is>
-          <t>Millenson-Wilens, Thea (2024/02/15/). Board of Trustees increases operational budget, tuition cost University Wire, (), . </t>
+          <t> (2024/02/14/). ODEI plans to host a screening of “The Color Purple” on Feb. 15  University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4040" spans="1:2">
       <c r="A4040" s="0">
-        <v>4505</v>
+        <v>4506</v>
       </c>
       <c r="B4040" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/14/). ODEI plans to host a screening of “The Color Purple” on Feb. 15  University Wire, (), . </t>
+          <t>Robinson, Daniel H (2024/02/13/). Philadelphia hopes year-round schooling can catch kids up to grade level – will it make a difference? The Conversation : Education, (), . </t>
         </is>
       </c>
     </row>
     <row r="4041" spans="1:2">
       <c r="A4041" s="0">
-        <v>4506</v>
+        <v>4507</v>
       </c>
       <c r="B4041" s="0" t="inlineStr">
         <is>
-          <t>Robinson, Daniel H (2024/02/13/). Philadelphia hopes year-round schooling can catch kids up to grade level – will it make a difference? The Conversation : Education, (), . </t>
+          <t>Zimmerman, Alex, Zimmer, Amy (2024/02/13/). Chalkbeat: Technical meltdown prevents NYC students from logging onto virtual classes during remote snow day Chalkbeat, (), . </t>
         </is>
       </c>
     </row>
     <row r="4042" spans="1:2">
       <c r="A4042" s="0">
-        <v>4507</v>
+        <v>4508</v>
       </c>
       <c r="B4042" s="0" t="inlineStr">
         <is>
-          <t>Zimmerman, Alex, Zimmer, Amy (2024/02/13/). Chalkbeat: Technical meltdown prevents NYC students from logging onto virtual classes during remote snow day Chalkbeat, (), . </t>
+          <t> (2024/02/11/). Sole candidate for speaker of the student senate aspires to serve all students University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4043" spans="1:2">
       <c r="A4043" s="0">
-        <v>4508</v>
+        <v>4509</v>
       </c>
       <c r="B4043" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/11/). Sole candidate for speaker of the student senate aspires to serve all students University Wire, (), . </t>
+          <t> (2024/02/08/). Church, apartment demolished, make way for Smile Student Living complex University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4044" spans="1:2">
       <c r="A4044" s="0">
-        <v>4509</v>
+        <v>4510</v>
       </c>
       <c r="B4044" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/08/). Church, apartment demolished, make way for Smile Student Living complex University Wire, (), . </t>
+          <t> (2024/02/07/). UWP Provost and Vice Chancellor Candidates – Exponent University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4045" spans="1:2">
       <c r="A4045" s="0">
-        <v>4510</v>
+        <v>4511</v>
       </c>
       <c r="B4045" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/07/). UWP Provost and Vice Chancellor Candidates – Exponent University Wire, (), . </t>
+          <t>Feyerherm, Alicia (2024/02/06/). USD 489 discusses HVAC maintenance, school calendar, KASB policies University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4046" spans="1:2">
       <c r="A4046" s="0">
-        <v>4511</v>
+        <v>4512</v>
       </c>
       <c r="B4046" s="0" t="inlineStr">
         <is>
-          <t>Feyerherm, Alicia (2024/02/06/). USD 489 discusses HVAC maintenance, school calendar, KASB policies University Wire, (), . </t>
+          <t>Clara Harms Noah Harris (2024/02/06/). 'At a breaking point': Durham Public Schools educators, community protest revoked employee raises University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4047" spans="1:2">
       <c r="A4047" s="0">
-        <v>4512</v>
+        <v>4513</v>
       </c>
       <c r="B4047" s="0" t="inlineStr">
         <is>
-          <t>Clara Harms Noah Harris (2024/02/06/). 'At a breaking point': Durham Public Schools educators, community protest revoked employee raises University Wire, (), . </t>
+          <t> (2024/02/05/). Next schedule with shorter passing periods will start next year – The Ring-tum Phi University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4048" spans="1:2">
       <c r="A4048" s="0">
-        <v>4513</v>
+        <v>4514</v>
       </c>
       <c r="B4048" s="0" t="inlineStr">
         <is>
-          <t> (2024/02/05/). Next schedule with shorter passing periods will start next year – The Ring-tum Phi University Wire, (), . </t>
+          <t>Willis, Jack (2024/02/02/). Don’t Shorten Winter Break, Students Say University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4049" spans="1:2">
       <c r="A4049" s="0">
-        <v>4514</v>
+        <v>4515</v>
       </c>
       <c r="B4049" s="0" t="inlineStr">
         <is>
-          <t>Willis, Jack (2024/02/02/). Don’t Shorten Winter Break, Students Say University Wire, (), . </t>
+          <t>Barry, Liv (2024/02/01/). Future of students’ snow days remains undetermined in a digital era University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4050" spans="1:2">
       <c r="A4050" s="0">
-        <v>4515</v>
+        <v>4516</v>
       </c>
       <c r="B4050" s="0" t="inlineStr">
         <is>
-          <t>Barry, Liv (2024/02/01/). Future of students’ snow days remains undetermined in a digital era University Wire, (), . </t>
+          <t>Amin, Reema (2024/02/01/). Chalkbeat: Chicago proposes later start date for 2024-25 school year due to Democratic National Convention Chalkbeat, (), . </t>
         </is>
       </c>
     </row>
     <row r="4051" spans="1:2">
       <c r="A4051" s="0">
-        <v>4516</v>
+        <v>4517</v>
       </c>
       <c r="B4051" s="0" t="inlineStr">
         <is>
-          <t>Amin, Reema (2024/02/01/). Chalkbeat: Chicago proposes later start date for 2024-25 school year due to Democratic National Convention Chalkbeat, (), . </t>
+          <t>Freeman, Laila (2024/01/31/). Veterans strive to make Chapman a destination campus for veteran, military-connected students (Part 1) University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4052" spans="1:2">
       <c r="A4052" s="0">
-        <v>4517</v>
+        <v>4518</v>
       </c>
       <c r="B4052" s="0" t="inlineStr">
         <is>
-          <t>Freeman, Laila (2024/01/31/). Veterans strive to make Chapman a destination campus for veteran, military-connected students (Part 1) University Wire, (), . </t>
+          <t>Syren, Lillian (2024/01/31/). Mock Thesis: Whether Aquinas Should Implement a Four-Day School Week University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4053" spans="1:2">
       <c r="A4053" s="0">
-        <v>4518</v>
+        <v>4519</v>
       </c>
       <c r="B4053" s="0" t="inlineStr">
         <is>
-          <t>Syren, Lillian (2024/01/31/). Mock Thesis: Whether Aquinas Should Implement a Four-Day School Week University Wire, (), . </t>
+          <t> (2024/01/31/). ‘The perfect option’: Students speak on University jobs - The Pitt News University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4054" spans="1:2">
       <c r="A4054" s="0">
-        <v>4519</v>
+        <v>4520</v>
       </c>
       <c r="B4054" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/31/). ‘The perfect option’: Students speak on University jobs - The Pitt News University Wire, (), . </t>
+          <t>Sophia De Lisi Anika Jain (2024/01/30/). Newton teachers' illegal strike persists amid building fines University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4055" spans="1:2">
       <c r="A4055" s="0">
-        <v>4520</v>
+        <v>4521</v>
       </c>
       <c r="B4055" s="0" t="inlineStr">
         <is>
-          <t>Sophia De Lisi Anika Jain (2024/01/30/). Newton teachers' illegal strike persists amid building fines University Wire, (), . </t>
+          <t>Smith, Mackenzie (2024/01/29/). Fall Break - Should it stay or should it go? University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4056" spans="1:2">
       <c r="A4056" s="0">
-        <v>4521</v>
+        <v>4522</v>
       </c>
       <c r="B4056" s="0" t="inlineStr">
         <is>
-          <t>Smith, Mackenzie (2024/01/29/). Fall Break - Should it stay or should it go? University Wire, (), . </t>
+          <t>McKoy, Sarah (2024/01/29/). Students Are Joining the Podcasting Market – The Greyhound University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4057" spans="1:2">
       <c r="A4057" s="0">
-        <v>4522</v>
+        <v>4523</v>
       </c>
       <c r="B4057" s="0" t="inlineStr">
         <is>
-          <t>McKoy, Sarah (2024/01/29/). Students Are Joining the Podcasting Market – The Greyhound University Wire, (), . </t>
+          <t>Hall, Emma (2024/01/29/). Summer courses should be more accessible University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4058" spans="1:2">
       <c r="A4058" s="0">
-        <v>4523</v>
+        <v>4524</v>
       </c>
       <c r="B4058" s="0" t="inlineStr">
         <is>
-          <t>Hall, Emma (2024/01/29/). Summer courses should be more accessible University Wire, (), . </t>
+          <t>Baker, Chloe, Sruli Friedman Chloe Baker, Friedman, Sruli (2024/01/26/). News Brief: Security Fee Introduced and Commencement Delayed a Week University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4059" spans="1:2">
       <c r="A4059" s="0">
-        <v>4524</v>
+        <v>4525</v>
       </c>
       <c r="B4059" s="0" t="inlineStr">
         <is>
-          <t>Baker, Chloe, Sruli Friedman Chloe Baker, Friedman, Sruli (2024/01/26/). News Brief: Security Fee Introduced and Commencement Delayed a Week University Wire, (), . </t>
+          <t>Meier, Alexandra (2024/01/25/). Panhellenic recruitment remains partially virtual – Old Gold &amp; Black University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4060" spans="1:2">
       <c r="A4060" s="0">
-        <v>4525</v>
+        <v>4526</v>
       </c>
       <c r="B4060" s="0" t="inlineStr">
         <is>
-          <t>Meier, Alexandra (2024/01/25/). Panhellenic recruitment remains partially virtual – Old Gold &amp; Black University Wire, (), . </t>
+          <t>Sibbitt, Dylan (2024/01/25/). February break would alleviate undue pressure on students University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4061" spans="1:2">
       <c r="A4061" s="0">
-        <v>4526</v>
+        <v>4527</v>
       </c>
       <c r="B4061" s="0" t="inlineStr">
         <is>
-          <t>Sibbitt, Dylan (2024/01/25/). February break would alleviate undue pressure on students University Wire, (), . </t>
+          <t>Alvarado, Jazmin (2024/01/22/). CFA systemwide strike will begin as planned due to inadequate GSI – The Collegian University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4062" spans="1:2">
       <c r="A4062" s="0">
-        <v>4527</v>
+        <v>4528</v>
       </c>
       <c r="B4062" s="0" t="inlineStr">
         <is>
-          <t>Alvarado, Jazmin (2024/01/22/). CFA systemwide strike will begin as planned due to inadequate GSI – The Collegian University Wire, (), . </t>
+          <t> (2024/01/22/). Durham Public Schools will not take money back from overpaid workers following walkouts University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4063" spans="1:2">
       <c r="A4063" s="0">
-        <v>4528</v>
+        <v>4529</v>
       </c>
       <c r="B4063" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/22/). Durham Public Schools will not take money back from overpaid workers following walkouts University Wire, (), . </t>
+          <t>Schuman, Rebecca (2024/01/19/). The Disposable, Indispensable Faculty Member: If teaching is so easy, why do so many tenured professors take such great pains to avoid it? The Chronicle of Higher Education, (), . </t>
         </is>
       </c>
     </row>
     <row r="4064" spans="1:2">
       <c r="A4064" s="0">
-        <v>4529</v>
+        <v>4530</v>
       </c>
       <c r="B4064" s="0" t="inlineStr">
         <is>
-          <t>Schuman, Rebecca (2024/01/19/). The Disposable, Indispensable Faculty Member: If teaching is so easy, why do so many tenured professors take such great pains to avoid it? The Chronicle of Higher Education, (), . </t>
+          <t>Gavin Meichelbock Kaycie Rippe Reid Sperisen Eric Sican Yuna Choi (2024/01/17/). TV preview: Five upcoming shows to start watching this winter University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4065" spans="1:2">
       <c r="A4065" s="0">
-        <v>4530</v>
+        <v>4531</v>
       </c>
       <c r="B4065" s="0" t="inlineStr">
         <is>
-          <t>Gavin Meichelbock Kaycie Rippe Reid Sperisen Eric Sican Yuna Choi (2024/01/17/). TV preview: Five upcoming shows to start watching this winter University Wire, (), . </t>
+          <t>Sabo, Oliver (2024/01/17/). Temple announces results of Fall scheduling survey University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4066" spans="1:2">
       <c r="A4066" s="0">
-        <v>4531</v>
+        <v>4532</v>
       </c>
       <c r="B4066" s="0" t="inlineStr">
         <is>
-          <t>Sabo, Oliver (2024/01/17/). Temple announces results of Fall scheduling survey University Wire, (), . </t>
+          <t> (2024/01/16/). Staff editorial: The pros and cons of GW's academic calendar - The GW Hatchet University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4067" spans="1:2">
       <c r="A4067" s="0">
-        <v>4532</v>
+        <v>4533</v>
       </c>
       <c r="B4067" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/16/). Staff editorial: The pros and cons of GW's academic calendar - The GW Hatchet University Wire, (), . </t>
+          <t> (2024/01/09/). Copper Country Human Society 50th Anniversary – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4068" spans="1:2">
       <c r="A4068" s="0">
-        <v>4533</v>
+        <v>4534</v>
       </c>
       <c r="B4068" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). Copper Country Human Society 50th Anniversary – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). Winter Carnival – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4069" spans="1:2">
       <c r="A4069" s="0">
-        <v>4534</v>
+        <v>4535</v>
       </c>
       <c r="B4069" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). Winter Carnival – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). New AISC steel sculpture – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4070" spans="1:2">
       <c r="A4070" s="0">
-        <v>4535</v>
+        <v>4536</v>
       </c>
       <c r="B4070" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). New AISC steel sculpture – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). Broomball to begin its next season – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4071" spans="1:2">
       <c r="A4071" s="0">
-        <v>4536</v>
+        <v>4537</v>
       </c>
       <c r="B4071" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). Broomball to begin its next season – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). Huskey Family loses Valued Student – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4072" spans="1:2">
       <c r="A4072" s="0">
-        <v>4537</v>
+        <v>4538</v>
       </c>
       <c r="B4072" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). Huskey Family loses Valued Student – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). AISES raises concerns on cancelled event – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4073" spans="1:2">
       <c r="A4073" s="0">
-        <v>4538</v>
+        <v>4539</v>
       </c>
       <c r="B4073" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). AISES raises concerns on cancelled event – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). Husky Thoughts – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4074" spans="1:2">
       <c r="A4074" s="0">
-        <v>4539</v>
+        <v>4540</v>
       </c>
       <c r="B4074" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). Husky Thoughts – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). Upcoming Events – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4075" spans="1:2">
       <c r="A4075" s="0">
-        <v>4540</v>
+        <v>4541</v>
       </c>
       <c r="B4075" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). Upcoming Events – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). Michigan Tech campus construction continues – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4076" spans="1:2">
       <c r="A4076" s="0">
-        <v>4541</v>
+        <v>4542</v>
       </c>
       <c r="B4076" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). Michigan Tech campus construction continues – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). Mont Ripley updates – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4077" spans="1:2">
       <c r="A4077" s="0">
-        <v>4542</v>
+        <v>4543</v>
       </c>
       <c r="B4077" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). Mont Ripley updates – The Lode University Wire, (), . </t>
+          <t> (2024/01/09/). What’s new with The Lode – The Lode University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4078" spans="1:2">
       <c r="A4078" s="0">
-        <v>4543</v>
+        <v>4544</v>
       </c>
       <c r="B4078" s="0" t="inlineStr">
         <is>
-          <t> (2024/01/09/). What’s new with The Lode – The Lode University Wire, (), . </t>
+          <t>Camp, Andrew Mitchell (2024). The Educator Labor Market in Times of Change: Lessons From the COVID-19 Pandemic ProQuest Dissertations and Theses, (), 152. </t>
         </is>
       </c>
     </row>
     <row r="4079" spans="1:2">
       <c r="A4079" s="0">
-        <v>4544</v>
+        <v>4545</v>
       </c>
       <c r="B4079" s="0" t="inlineStr">
         <is>
-          <t>Camp, Andrew Mitchell (2024). The Educator Labor Market in Times of Change: Lessons From the COVID-19 Pandemic ProQuest Dissertations and Theses, (), 152. </t>
+          <t>Jenkins, Davis, Lahr, Hana, Brock, Thomas (2024). Lessons from Two Major Evaluations of Guided Pathways. Research Brief Community College Research Center, Teachers College, Columbia University, (), . </t>
         </is>
       </c>
     </row>
     <row r="4080" spans="1:2">
       <c r="A4080" s="0">
-        <v>4545</v>
+        <v>4546</v>
       </c>
       <c r="B4080" s="0" t="inlineStr">
         <is>
-          <t>Jenkins, Davis, Lahr, Hana, Brock, Thomas (2024). Lessons from Two Major Evaluations of Guided Pathways. Research Brief Community College Research Center, Teachers College, Columbia University, (), . </t>
+          <t>Zhang, Xiaoxia, Gu, Xiangli, Chu, Tsz Lun, Lee, Joonyoung, Zhang, Tao (2024). Weight Status and Socio-Demographic Disparities in Children's Physical Activity Intensity during Different Segments of the School Day Elementary School Journal, 124(3), 499. https://doi.org/10.1086/728407</t>
         </is>
       </c>
     </row>
     <row r="4081" spans="1:2">
       <c r="A4081" s="0">
-        <v>4546</v>
+        <v>4547</v>
       </c>
       <c r="B4081" s="0" t="inlineStr">
         <is>
-          <t>Zhang, Xiaoxia, Gu, Xiangli, Chu, Tsz Lun, Lee, Joonyoung, Zhang, Tao (2024). Weight Status and Socio-Demographic Disparities in Children's Physical Activity Intensity during Different Segments of the School Day Elementary School Journal, 124(3), 499. https://doi.org/10.1086/728407</t>
+          <t>Zoromski, Keith, Sasso, Pietro A (2024). Transactional and Stopgap Relationships between Community College Department Chairs and Their Adjuncts Community College Review, 52(2), 210. https://doi.org/10.1177/00915521231218239</t>
         </is>
       </c>
     </row>
     <row r="4082" spans="1:2">
       <c r="A4082" s="0">
-        <v>4547</v>
+        <v>4548</v>
       </c>
       <c r="B4082" s="0" t="inlineStr">
         <is>
-          <t>Zoromski, Keith, Sasso, Pietro A (2024). Transactional and Stopgap Relationships between Community College Department Chairs and Their Adjuncts Community College Review, 52(2), 210. https://doi.org/10.1177/00915521231218239</t>
+          <t>Jones, Daniel A (2024). Views on Modifying the Traditional School Calendar for a Post-COVID World: Could a Balanced Calendar Model Mitigate COVID-19 Slide? Journal of Education, 204(1), 230. https://doi.org/10.1177/00220574221112626</t>
         </is>
       </c>
     </row>
     <row r="4083" spans="1:2">
       <c r="A4083" s="0">
-        <v>4548</v>
+        <v>4549</v>
       </c>
       <c r="B4083" s="0" t="inlineStr">
         <is>
-          <t>Jones, Daniel A (2024). Views on Modifying the Traditional School Calendar for a Post-COVID World: Could a Balanced Calendar Model Mitigate COVID-19 Slide? Journal of Education, 204(1), 230. https://doi.org/10.1177/00220574221112626</t>
+          <t>Kottenstette, Bill, Paga, Paola (2024). 2022-23 Innovation Schools Annual Report Colorado Department of Education, (), . </t>
         </is>
       </c>
     </row>
     <row r="4084" spans="1:2">
       <c r="A4084" s="0">
-        <v>4549</v>
+        <v>4550</v>
       </c>
       <c r="B4084" s="0" t="inlineStr">
         <is>
-          <t>Kottenstette, Bill, Paga, Paola (2024). 2022-23 Innovation Schools Annual Report Colorado Department of Education, (), . </t>
+          <t>Rafael da Silva Fernandes, Rosana Maria do Nascimento Luz, Jaqueline Matias da Silva, de Andrade, Dalton Francisco (2024). Analysis of the effects of perceived quality differences between adequacy for emergency remote education and return to traditional in-person education Quality Assurance in Education, 32(1), 141. https://doi.org/10.1108/QAE-01-2023-0005</t>
         </is>
       </c>
     </row>
     <row r="4085" spans="1:2">
       <c r="A4085" s="0">
-        <v>4550</v>
+        <v>4551</v>
       </c>
       <c r="B4085" s="0" t="inlineStr">
         <is>
-          <t>Rafael da Silva Fernandes, Rosana Maria do Nascimento Luz, Jaqueline Matias da Silva, de Andrade, Dalton Francisco (2024). Analysis of the effects of perceived quality differences between adequacy for emergency remote education and return to traditional in-person education Quality Assurance in Education, 32(1), 141. https://doi.org/10.1108/QAE-01-2023-0005</t>
+          <t>DeWitt, Ben (2023/12/21/). Prosecutors seek summer trial date in Kohberger case  University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4086" spans="1:2">
       <c r="A4086" s="0">
-        <v>4551</v>
+        <v>4552</v>
       </c>
       <c r="B4086" s="0" t="inlineStr">
         <is>
-          <t>DeWitt, Ben (2023/12/21/). Prosecutors seek summer trial date in Kohberger case  University Wire, (), . </t>
+          <t>Kelleher, Maureen (2023/12/20/). FutureEd: Three Keys to Successful High-Dosage Tutoring FutureEd, (), . </t>
         </is>
       </c>
     </row>
     <row r="4087" spans="1:2">
       <c r="A4087" s="0">
-        <v>4552</v>
+        <v>4553</v>
       </c>
       <c r="B4087" s="0" t="inlineStr">
         <is>
-          <t>Kelleher, Maureen (2023/12/20/). FutureEd: Three Keys to Successful High-Dosage Tutoring FutureEd, (), . </t>
+          <t>Fong-Isariyawongse, Joanna (2023/12/18/). Students could get more sleep and learn better if school started a little later The Conversation : Education, (), . </t>
         </is>
       </c>
     </row>
     <row r="4088" spans="1:2">
       <c r="A4088" s="0">
-        <v>4553</v>
+        <v>4555</v>
       </c>
       <c r="B4088" s="0" t="inlineStr">
         <is>
-          <t>Fong-Isariyawongse, Joanna (2023/12/18/). Students could get more sleep and learn better if school started a little later The Conversation : Education, (), . </t>
+          <t> (2023/12/16/). Style and trends to expect in spring 2024 University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4089" spans="1:2">
       <c r="A4089" s="0">
-        <v>4555</v>
+        <v>4556</v>
       </c>
       <c r="B4089" s="0" t="inlineStr">
         <is>
-          <t> (2023/12/16/). Style and trends to expect in spring 2024 University Wire, (), . </t>
+          <t>Mack, Ryan (2023/12/14/). How Temple is deciding the Fall 2024 academic calendar University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4090" spans="1:2">
       <c r="A4090" s="0">
-        <v>4556</v>
+        <v>4557</v>
       </c>
       <c r="B4090" s="0" t="inlineStr">
         <is>
-          <t>Mack, Ryan (2023/12/14/). How Temple is deciding the Fall 2024 academic calendar University Wire, (), . </t>
+          <t>Seals, Hana (2023/12/14/). Cheering for change - The Oak Leaf University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4091" spans="1:2">
       <c r="A4091" s="0">
-        <v>4557</v>
+        <v>4558</v>
       </c>
       <c r="B4091" s="0" t="inlineStr">
         <is>
-          <t>Seals, Hana (2023/12/14/). Cheering for change - The Oak Leaf University Wire, (), . </t>
+          <t>Rosas, Luna (2023/12/13/). Dyani White Hawk presents lecture on advocating for Native American women through her art as part of MFA series University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4092" spans="1:2">
       <c r="A4092" s="0">
-        <v>4558</v>
+        <v>4559</v>
       </c>
       <c r="B4092" s="0" t="inlineStr">
         <is>
-          <t>Rosas, Luna (2023/12/13/). Dyani White Hawk presents lecture on advocating for Native American women through her art as part of MFA series University Wire, (), . </t>
+          <t>Victoria Davies Louisa Gheorghita (2023/12/13/). International students highlight challenges with flying home after finals period University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4093" spans="1:2">
       <c r="A4093" s="0">
-        <v>4559</v>
+        <v>4560</v>
       </c>
       <c r="B4093" s="0" t="inlineStr">
         <is>
-          <t>Victoria Davies Louisa Gheorghita (2023/12/13/). International students highlight challenges with flying home after finals period University Wire, (), . </t>
+          <t> (2023/12/12/). Game on! CPP students showcase esports skills in FIFA tournament University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4094" spans="1:2">
       <c r="A4094" s="0">
-        <v>4560</v>
+        <v>4561</v>
       </c>
       <c r="B4094" s="0" t="inlineStr">
         <is>
-          <t> (2023/12/12/). Game on! CPP students showcase esports skills in FIFA tournament University Wire, (), . </t>
+          <t> (2023/12/08/). This Week in Senate University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4095" spans="1:2">
       <c r="A4095" s="0">
-        <v>4561</v>
+        <v>4562</v>
       </c>
       <c r="B4095" s="0" t="inlineStr">
         <is>
-          <t> (2023/12/08/). This Week in Senate University Wire, (), . </t>
+          <t>Rachel Mintz Astrid Code Eilene Koo Joshua Nicholson (2023/12/06/). Student Life VP Martino Harmon discusses student activism, AI in exclusive interview University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4096" spans="1:2">
       <c r="A4096" s="0">
-        <v>4562</v>
+        <v>4563</v>
       </c>
       <c r="B4096" s="0" t="inlineStr">
         <is>
-          <t>Rachel Mintz Astrid Code Eilene Koo Joshua Nicholson (2023/12/06/). Student Life VP Martino Harmon discusses student activism, AI in exclusive interview University Wire, (), . </t>
+          <t> (2023/12/06/). CCCA Fall Research Showcase highlights faculty and student projects University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4097" spans="1:2">
       <c r="A4097" s="0">
-        <v>4563</v>
+        <v>4564</v>
       </c>
       <c r="B4097" s="0" t="inlineStr">
         <is>
-          <t> (2023/12/06/). CCCA Fall Research Showcase highlights faculty and student projects University Wire, (), . </t>
+          <t>Hope, Nathan (2023/12/06/). Hootie Days in discussion to make return University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4098" spans="1:2">
       <c r="A4098" s="0">
-        <v>4564</v>
+        <v>4565</v>
       </c>
       <c r="B4098" s="0" t="inlineStr">
         <is>
-          <t>Hope, Nathan (2023/12/06/). Hootie Days in discussion to make return University Wire, (), . </t>
+          <t> (2023/12/05/). Taking a breather – The Orion University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4099" spans="1:2">
       <c r="A4099" s="0">
-        <v>4565</v>
+        <v>4566</v>
       </c>
       <c r="B4099" s="0" t="inlineStr">
         <is>
-          <t> (2023/12/05/). Taking a breather – The Orion University Wire, (), . </t>
+          <t> (2023/12/04/). FSU surveying students on policy such as Bright Futures expansion, Narcan in dorm halls University Wire, (), . </t>
         </is>
       </c>
     </row>
     <row r="4100" spans="1:2">
       <c r="A4100" s="0">
-        <v>4566</v>
+        <v>4567</v>
       </c>
       <c r="B4100" s="0" t="inlineStr">
         <is>
-          <t> (2023/12/04/). FSU surveying students on policy such as Bright Futures expansion, Narcan in dorm halls University Wire, (), . </t>
+          <t>Jeruszka-Bielak, Marta, Górnicka, Magdalena (2024). Healthy and sustainable school meals - proposal for a new quality index SMI-LE. Annals of agricultural and environmental medicine : AAEM, 31(1), 57. 10.26444/aaem/171610</t>
         </is>
       </c>
     </row>
     <row r="4101" spans="1:2">
       <c r="A4101" s="0">
-        <v>4567</v>
+        <v>4568</v>
       </c>
       <c r="B4101" s="0" t="inlineStr">
         <is>
-          <t>Jeruszka-Bielak, Marta, Górnicka, Magdalena (2024). Healthy and sustainable school meals - proposal for a new quality index SMI-LE. Annals of agricultural and environmental medicine : AAEM, 31(1), 57. 10.26444/aaem/171610</t>
+          <t>Steuber, Taylor D., Trujillo, Daniel, McCoy, Emily K., Pinner, Nathan A., Hornsby, Lori, Andrus, Miranda R., Kleppinger, Erika L., Eiland, Lea S. (2024). Evaluation of Student Academic Performance After Curricular Content Reduction. American journal of pharmaceutical education, 88(7), 100721. 10.1016/j.ajpe.2024.100721</t>
         </is>
       </c>
     </row>
     <row r="4102" spans="1:2">
       <c r="A4102" s="0">
-        <v>4568</v>
+        <v>4569</v>
       </c>
       <c r="B4102" s="0" t="inlineStr">
         <is>
-          <t>Steuber, Taylor D., Trujillo, Daniel, McCoy, Emily K., Pinner, Nathan A., Hornsby, Lori, Andrus, Miranda R., Kleppinger, Erika L., Eiland, Lea S. (2024). Evaluation of Student Academic Performance After Curricular Content Reduction. American journal of pharmaceutical education, 88(7), 100721. 10.1016/j.ajpe.2024.100721</t>
+          <t>Togha, Mansoureh, Rafiee, Pegah, Haghdoost, Faraidoon, Rafie, Shahram, Paknejad, Seyed Mohammad Hasan, Amouian, Sepideh, Şaşmaz, Tayyar, Kale, Derya, Uluduz, Derya, Steiner, Timothy J. (2024). The burdens attributable to primary headache disorders in children and adolescents in Iran: estimates from a schools-based study. The journal of headache and pain, 25(1), 86. 10.1186/s10194-024-01789-0</t>
         </is>
       </c>
     </row>
     <row r="4103" spans="1:2">
       <c r="A4103" s="0">
-        <v>4569</v>
+        <v>4570</v>
       </c>
       <c r="B4103" s="0" t="inlineStr">
         <is>
-          <t>Togha, Mansoureh, Rafiee, Pegah, Haghdoost, Faraidoon, Rafie, Shahram, Paknejad, Seyed Mohammad Hasan, Amouian, Sepideh, Şaşmaz, Tayyar, Kale, Derya, Uluduz, Derya, Steiner, Timothy J. (2024). The burdens attributable to primary headache disorders in children and adolescents in Iran: estimates from a schools-based study. The journal of headache and pain, 25(1), 86. 10.1186/s10194-024-01789-0</t>
+          <t>Morton, Emily (2024). Can four equal five? Essays on the four-day school week. , 85(6-B), No. </t>
         </is>
       </c>
     </row>
     <row r="4104" spans="1:2">
       <c r="A4104" s="0">
-        <v>4570</v>
+        <v>4576</v>
       </c>
       <c r="B4104" s="0" t="inlineStr">
         <is>
-          <t>Morton, Emily (2024). Can four equal five? Essays on the four-day school week. , 85(6-B), No. </t>
+          <t>Edney, Sarah, Goh, Claire Marie, Chua, Xin Hui, Low, Alicia, Chia, Janelle, Koek, Daphne S., Cheong, Karen, van Dam, Rob, Tan, Chuen Seng, Müller-Riemenschneider, Falk (2023). Evaluating the effects of rewards and schedule length on response rates to ecological momentary assessment surveys: Randomized controlled trials. Journal of Medical Internet Research, 25(), . 10.2196/45764</t>
         </is>
       </c>
     </row>
     <row r="4105" spans="1:2">
       <c r="A4105" s="0">
-        <v>4576</v>
+        <v>4578</v>
       </c>
       <c r="B4105" s="0" t="inlineStr">
         <is>
-          <t>Edney, Sarah, Goh, Claire Marie, Chua, Xin Hui, Low, Alicia, Chia, Janelle, Koek, Daphne S., Cheong, Karen, van Dam, Rob, Tan, Chuen Seng, Müller-Riemenschneider, Falk (2023). Evaluating the effects of rewards and schedule length on response rates to ecological momentary assessment surveys: Randomized controlled trials. Journal of Medical Internet Research, 25(), . 10.2196/45764</t>
+          <t>Andrew M. Camp, Taylor Wilson, Yujia Liu, J. Cameron Anglum, Anita Manion, &amp; Tuan Nguyen (2024). Teacher Retention and the Four-Day School Week in Missouri PRiME Center | St. Louis University, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4106" spans="1:2">
+      <c r="A4106" s="0">
+        <v>4579</v>
+      </c>
+      <c r="B4106" s="0" t="inlineStr">
+        <is>
+          <t>Ainsworth, Aaron J., Penner, Emily K., Liu, Yujia (2024). Less is More? The Causal Effect of Four-Day School Weeks on Employee , (), . 10.26300/QGTJ-MJ51</t>
+        </is>
+      </c>
+    </row>
+    <row r="4107" spans="1:2">
+      <c r="A4107" s="0">
+        <v>4580</v>
+      </c>
+      <c r="B4107" s="0" t="inlineStr">
+        <is>
+          <t>Gottlieb, Alan , Lagana, Maya,  &amp; Schoales, Van  (#year#). Doing less with less: How a four-day school week a_x000E_ects  student learning and the teacher workforce. , (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4108" spans="1:2">
+      <c r="A4108" s="0">
+        <v>4581</v>
+      </c>
+      <c r="B4108" s="0" t="inlineStr">
+        <is>
+          <t>Emily Morton &amp; Emma Dewil (2024). Impacts of Four-Day School Weeks on Teacher Recruitment and Retention and Student  Attendance: Evidence from Colorado CALDER Working Paper No. 307-0924, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4109" spans="1:2">
+      <c r="A4109" s="0">
+        <v>4582</v>
+      </c>
+      <c r="B4109" s="0" t="inlineStr">
+        <is>
+          <t>Ramshini, E, Shabani, M (2024). Cannabinoid receptor type 1 agonist disrupts methamphetamine-induced conditioned place preference in adolescent male rats. Neuroscience letters, 844(), 138033. 10.1016/j.neulet.2024.138033</t>
+        </is>
+      </c>
+    </row>
+    <row r="4110" spans="1:2">
+      <c r="A4110" s="0">
+        <v>4583</v>
+      </c>
+      <c r="B4110" s="0" t="inlineStr">
+        <is>
+          <t>Steuber, TD, Trujillo, D, McCoy, EK, Pinner, NA, Hornsby, L, Andrus, MR, Kleppinger, EL, Eiland, LS (2024). Evaluation of Student Academic Performance After Curricular Content Reduction. American journal of pharmaceutical education, 88(7), 100721. 10.1016/j.ajpe.2024.100721</t>
+        </is>
+      </c>
+    </row>
+    <row r="4111" spans="1:2">
+      <c r="A4111" s="0">
+        <v>4584</v>
+      </c>
+      <c r="B4111" s="0" t="inlineStr">
+        <is>
+          <t>Thomas, Kirsten (2024/11/21/). OPINION: Chill out with your fitness goals – The Daily Wildcat University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4112" spans="1:2">
+      <c r="A4112" s="0">
+        <v>4585</v>
+      </c>
+      <c r="B4112" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/21/). How did De Anza vote? - La Voz News University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4113" spans="1:2">
+      <c r="A4113" s="0">
+        <v>4586</v>
+      </c>
+      <c r="B4113" s="0" t="inlineStr">
+        <is>
+          <t>Gallegos, Alex (2024/11/18/). The one thing every college student should do for success University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4114" spans="1:2">
+      <c r="A4114" s="0">
+        <v>4587</v>
+      </c>
+      <c r="B4114" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/18/). Students race toward Thanksgiving break as fall burnout reaches peak – THE CHANTICLEER University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4115" spans="1:2">
+      <c r="A4115" s="0">
+        <v>4588</v>
+      </c>
+      <c r="B4115" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/16/). Why a Four-Day Work Week is Beneficial University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4116" spans="1:2">
+      <c r="A4116" s="0">
+        <v>4589</v>
+      </c>
+      <c r="B4116" s="0" t="inlineStr">
+        <is>
+          <t>Polovina, Brenna (2024/11/15/). MCCSC board members plan to address unfinished work in new term - Indiana Daily Student University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4117" spans="1:2">
+      <c r="A4117" s="0">
+        <v>4590</v>
+      </c>
+      <c r="B4117" s="0" t="inlineStr">
+        <is>
+          <t>Vezmar, Evan (2024/11/14/). What the approved ballot initiatives mean for Medford, Somerville University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4118" spans="1:2">
+      <c r="A4118" s="0">
+        <v>4591</v>
+      </c>
+      <c r="B4118" s="0" t="inlineStr">
+        <is>
+          <t>Bereny, Annika (2024/11/13/). TAA launches bioscience graduate worker campaign University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4119" spans="1:2">
+      <c r="A4119" s="0">
+        <v>4592</v>
+      </c>
+      <c r="B4119" s="0" t="inlineStr">
+        <is>
+          <t>Bereny, Annika (2024/11/13/). TAA launches bioscience graduate worker campaign University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4120" spans="1:2">
+      <c r="A4120" s="0">
+        <v>4593</v>
+      </c>
+      <c r="B4120" s="0" t="inlineStr">
+        <is>
+          <t>Bartlett, Parker (2024/11/13/). The election day dilemma: Students weigh in on if classes should be held on the day University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4121" spans="1:2">
+      <c r="A4121" s="0">
+        <v>4594</v>
+      </c>
+      <c r="B4121" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/12/). Letter to the Editor: UVM should have classes off for federal elections – The Vermont Cynic University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4122" spans="1:2">
+      <c r="A4122" s="0">
+        <v>4595</v>
+      </c>
+      <c r="B4122" s="0" t="inlineStr">
+        <is>
+          <t>Tolbert, Noah (2024/11/11/). Quarter Muncher: Persona 4 - The Spectator University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4123" spans="1:2">
+      <c r="A4123" s="0">
+        <v>4596</v>
+      </c>
+      <c r="B4123" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/10/). Is it Columbus Day or Indigenous Peoples Day? Students speak on the second Monday of October tradition University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4124" spans="1:2">
+      <c r="A4124" s="0">
+        <v>4597</v>
+      </c>
+      <c r="B4124" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/09/). CSU Esports Team exercises dedication, teamwork in video game competitions – The Rocky Mountain Collegian University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4125" spans="1:2">
+      <c r="A4125" s="0">
+        <v>4598</v>
+      </c>
+      <c r="B4125" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/07/). Slime time on campus: An unforgettable bash University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4126" spans="1:2">
+      <c r="A4126" s="0">
+        <v>4599</v>
+      </c>
+      <c r="B4126" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/06/). Rowan students consider women’s rights and healthcare when casting their ballots early – The Whit University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4127" spans="1:2">
+      <c r="A4127" s="0">
+        <v>4600</v>
+      </c>
+      <c r="B4127" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/06/). Clocking out: Daylight saving time’s impact on students University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4128" spans="1:2">
+      <c r="A4128" s="0">
+        <v>4601</v>
+      </c>
+      <c r="B4128" s="0" t="inlineStr">
+        <is>
+          <t>Marblestone, Chloe (2024/11/05/). Surviving Your First Semester - The Ionian University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4129" spans="1:2">
+      <c r="A4129" s="0">
+        <v>4602</v>
+      </c>
+      <c r="B4129" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/05/). COLUMN | Auburn's unique pace in a fast moving world University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4130" spans="1:2">
+      <c r="A4130" s="0">
+        <v>4603</v>
+      </c>
+      <c r="B4130" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/04/). Why isn't Election Day an academic holiday? University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4131" spans="1:2">
+      <c r="A4131" s="0">
+        <v>4604</v>
+      </c>
+      <c r="B4131" s="0" t="inlineStr">
+        <is>
+          <t>Bickley, Ryland (2024/11/04/). LBCC Winter Term Priority Registration Opens Nov. 12 University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4132" spans="1:2">
+      <c r="A4132" s="0">
+        <v>4605</v>
+      </c>
+      <c r="B4132" s="0" t="inlineStr">
+        <is>
+          <t>Limehouse, Jonathan (2024/11/04/). Are schools closed on Election Day? Here's what to know before polls open University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4133" spans="1:2">
+      <c r="A4133" s="0">
+        <v>4606</v>
+      </c>
+      <c r="B4133" s="0" t="inlineStr">
+        <is>
+          <t>Dawkins-Maldonado, Alexis (2024/11/04/). A canon event: Registering for classes at the university - The Charger Bulletin University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4134" spans="1:2">
+      <c r="A4134" s="0">
+        <v>4607</v>
+      </c>
+      <c r="B4134" s="0" t="inlineStr">
+        <is>
+          <t> (2024/11/02/). 'Unless you've been through it, you can't understand': Helene recovery continues in NC University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4135" spans="1:2">
+      <c r="A4135" s="0">
+        <v>4608</v>
+      </c>
+      <c r="B4135" s="0" t="inlineStr">
+        <is>
+          <t>Zak, Yehuda Ayala, Baron-Epel Orna (2024/11//). Factors contributing to the development of health-promoting schools, applying Fullan’s triple change model – A qualitative study The Health Education Journal, 83(7), 759. https://doi.org/10.1177/00178969241279284</t>
+        </is>
+      </c>
+    </row>
+    <row r="4136" spans="1:2">
+      <c r="A4136" s="0">
+        <v>4609</v>
+      </c>
+      <c r="B4136" s="0" t="inlineStr">
+        <is>
+          <t>Zimmer, Amy, Zimmerman, Alex (2024/10/30/). Chalkbeat: NYC school calendar update: Monday, Dec. 23 will now be a day off Chalkbeat, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4137" spans="1:2">
+      <c r="A4137" s="0">
+        <v>4610</v>
+      </c>
+      <c r="B4137" s="0" t="inlineStr">
+        <is>
+          <t> (2024/10/30/). COLUMN: We deserve Election Day off University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4138" spans="1:2">
+      <c r="A4138" s="0">
+        <v>4611</v>
+      </c>
+      <c r="B4138" s="0" t="inlineStr">
+        <is>
+          <t>Balas, Lydia (2024/10/30/). Is Fall Break Beneficial? – The Informer University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4139" spans="1:2">
+      <c r="A4139" s="0">
+        <v>4612</v>
+      </c>
+      <c r="B4139" s="0" t="inlineStr">
+        <is>
+          <t>Wallace, Ethan (2024/10/26/). NCAC shake-up continues with addition of Wash U football University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4140" spans="1:2">
+      <c r="A4140" s="0">
+        <v>4613</v>
+      </c>
+      <c r="B4140" s="0" t="inlineStr">
+        <is>
+          <t>Bower, Bianca (2024/10/22/). My Experience as a Dual Enrollment Student at GRCC University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4141" spans="1:2">
+      <c r="A4141" s="0">
+        <v>4614</v>
+      </c>
+      <c r="B4141" s="0" t="inlineStr">
+        <is>
+          <t> (2024/10/21/). Dallas College adds new holidays to academic calendar – Richland Student Media University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4142" spans="1:2">
+      <c r="A4142" s="0">
+        <v>4615</v>
+      </c>
+      <c r="B4142" s="0" t="inlineStr">
+        <is>
+          <t> (2024/10/20/). The University of Tampa Announces Saturday Classes – The Minaret University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4143" spans="1:2">
+      <c r="A4143" s="0">
+        <v>4616</v>
+      </c>
+      <c r="B4143" s="0" t="inlineStr">
+        <is>
+          <t>Franjola, Sacha (2024/10/17/). Archives: Family Weekend came from humble beginnings  University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4144" spans="1:2">
+      <c r="A4144" s="0">
+        <v>4617</v>
+      </c>
+      <c r="B4144" s="0" t="inlineStr">
+        <is>
+          <t>Hobbs, Scott (2024/10/15/). UAA needs more Alaska Native representation University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4145" spans="1:2">
+      <c r="A4145" s="0">
+        <v>4618</v>
+      </c>
+      <c r="B4145" s="0" t="inlineStr">
+        <is>
+          <t>Hopp, Peyton (2024/10/14/). A focus on student athletes academics - The DePaulia University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4146" spans="1:2">
+      <c r="A4146" s="0">
+        <v>4619</v>
+      </c>
+      <c r="B4146" s="0" t="inlineStr">
+        <is>
+          <t>Kozina, Emma (2024/10/12/). Fall-themed games, shows, movies to satisfy every festive craving - The Badger Herald University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4147" spans="1:2">
+      <c r="A4147" s="0">
+        <v>4620</v>
+      </c>
+      <c r="B4147" s="0" t="inlineStr">
+        <is>
+          <t>Moore, Tony (2024/10/11/). Redefining Success University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4148" spans="1:2">
+      <c r="A4148" s="0">
+        <v>4621</v>
+      </c>
+      <c r="B4148" s="0" t="inlineStr">
+        <is>
+          <t>Heller, Madison (2024/10/11/). Navigating fall cultural holidays and accommodations University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4149" spans="1:2">
+      <c r="A4149" s="0">
+        <v>4622</v>
+      </c>
+      <c r="B4149" s="0" t="inlineStr">
+        <is>
+          <t> (2024/10/10/). What happened at Tuesday’s SA Congress meeting University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4150" spans="1:2">
+      <c r="A4150" s="0">
+        <v>4623</v>
+      </c>
+      <c r="B4150" s="0" t="inlineStr">
+        <is>
+          <t>FARNAN, BROOKLYN (2024/10/09/). Northwest celebrates LGBTQ+ History Month, multiple events held to educate students University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4151" spans="1:2">
+      <c r="A4151" s="0">
+        <v>4624</v>
+      </c>
+      <c r="B4151" s="0" t="inlineStr">
+        <is>
+          <t> (2024/10/08/). York Theatre Celebrates 100th Anniversary University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4152" spans="1:2">
+      <c r="A4152" s="0">
+        <v>4625</v>
+      </c>
+      <c r="B4152" s="0" t="inlineStr">
+        <is>
+          <t> (2024/10/07/). Cole Benzmiller: The baseball player and former yell leader - The Washburn Review University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4153" spans="1:2">
+      <c r="A4153" s="0">
+        <v>4626</v>
+      </c>
+      <c r="B4153" s="0" t="inlineStr">
+        <is>
+          <t>Chandler, Chloe (2024/10/07/). Women's Services and Resources, others offer resources to BYU student parents University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4154" spans="1:2">
+      <c r="A4154" s="0">
+        <v>4627</v>
+      </c>
+      <c r="B4154" s="0" t="inlineStr">
+        <is>
+          <t> (2024/10/02/). Mandatory earthquake drill could affect scheduled meeting times with students - El Camino College The Union University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4155" spans="1:2">
+      <c r="A4155" s="0">
+        <v>4628</v>
+      </c>
+      <c r="B4155" s="0" t="inlineStr">
+        <is>
+          <t>Russell, Jillian (2024/10/02/). New job blues: working students face learning curve in Oxford University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4156" spans="1:2">
+      <c r="A4156" s="0">
+        <v>4629</v>
+      </c>
+      <c r="B4156" s="0" t="inlineStr">
+        <is>
+          <t>Berthelon, Matias, Kruger, Diana, Lauer, Catalina, Tiberti, Luca, Zamora, Carlos (2024/10//). Longer school schedules, childcare and the quality of mothers’ employment Economic Policy, 39(120), 817. https://doi.org/10.1093/epolic/eiae037</t>
+        </is>
+      </c>
+    </row>
+    <row r="4157" spans="1:2">
+      <c r="A4157" s="0">
+        <v>4630</v>
+      </c>
+      <c r="B4157" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/25/). Faces of Mason: Chadwick Edralin University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4158" spans="1:2">
+      <c r="A4158" s="0">
+        <v>4631</v>
+      </c>
+      <c r="B4158" s="0" t="inlineStr">
+        <is>
+          <t>Archer, Bella (2024/09/25/). The Hidden Costs of Travel Disruption University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4159" spans="1:2">
+      <c r="A4159" s="0">
+        <v>4632</v>
+      </c>
+      <c r="B4159" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/24/). Kelsey aces latest milestone in volleyball's dominating start - The Suffolk Journal University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4160" spans="1:2">
+      <c r="A4160" s="0">
+        <v>4633</v>
+      </c>
+      <c r="B4160" s="0" t="inlineStr">
+        <is>
+          <t>Show-Me Institute, Missouri (2024/09/20/). The Four-Day School Week Continues to Grow in Missouri CE Think Tank Newswire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4161" spans="1:2">
+      <c r="A4161" s="0">
+        <v>4634</v>
+      </c>
+      <c r="B4161" s="0" t="inlineStr">
+        <is>
+          <t>Gaffney, Emmett (2024/09/19/). UW-Madison should start school earlier, here's why University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4162" spans="1:2">
+      <c r="A4162" s="0">
+        <v>4635</v>
+      </c>
+      <c r="B4162" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/19/). Proposed calendar change won't take effect in upcoming school year - El Camino College The Union University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4163" spans="1:2">
+      <c r="A4163" s="0">
+        <v>4636</v>
+      </c>
+      <c r="B4163" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/19/). Schedule leaves no time to breathe after turkey dinner University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4164" spans="1:2">
+      <c r="A4164" s="0">
+        <v>4637</v>
+      </c>
+      <c r="B4164" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/19/). How to Choose the Right Level of Care for Your Mental Health Needs University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4165" spans="1:2">
+      <c r="A4165" s="0">
+        <v>4638</v>
+      </c>
+      <c r="B4165" s="0" t="inlineStr">
+        <is>
+          <t>Gaffney, Emmett (2024/09/19/). UW-Madison should start school earlier, here's why University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4166" spans="1:2">
+      <c r="A4166" s="0">
+        <v>4639</v>
+      </c>
+      <c r="B4166" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/19/). Sun Devil side hustles: Passion pays the bills University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4167" spans="1:2">
+      <c r="A4167" s="0">
+        <v>4640</v>
+      </c>
+      <c r="B4167" s="0" t="inlineStr">
+        <is>
+          <t>Sena Chang Eojin Park (2024/09/18/). University released final exam schedule early, allowing earlier travel booking University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4168" spans="1:2">
+      <c r="A4168" s="0">
+        <v>4641</v>
+      </c>
+      <c r="B4168" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/18/). ListenUP: A Healthy Start – The Villanovan University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4169" spans="1:2">
+      <c r="A4169" s="0">
+        <v>4642</v>
+      </c>
+      <c r="B4169" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/15/). Are you smarter than a fifth grader? University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4170" spans="1:2">
+      <c r="A4170" s="0">
+        <v>4643</v>
+      </c>
+      <c r="B4170" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/14/). US seizes 10-6 lead over Europe after day two of Solheim Cup University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4171" spans="1:2">
+      <c r="A4171" s="0">
+        <v>4644</v>
+      </c>
+      <c r="B4171" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/13/). OU Board of Regents approves employee health insurance changes, dean search committees University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4172" spans="1:2">
+      <c r="A4172" s="0">
+        <v>4645</v>
+      </c>
+      <c r="B4172" s="0" t="inlineStr">
+        <is>
+          <t>Rode, Erin (2024/09/11/). Chalkbeat: 109 degrees on the first day of school? In some districts, extreme heat is changing the school calendar. Chalkbeat, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4173" spans="1:2">
+      <c r="A4173" s="0">
+        <v>4646</v>
+      </c>
+      <c r="B4173" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/10/). Know Your Athlete: Caroline Crossley - The Tribune University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4174" spans="1:2">
+      <c r="A4174" s="0">
+        <v>4647</v>
+      </c>
+      <c r="B4174" s="0" t="inlineStr">
+        <is>
+          <t>Jimenez, Bryan (2024/09/09/). Following CSU policy, CSUF tightens protest rules | News | dailytitan.com University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4175" spans="1:2">
+      <c r="A4175" s="0">
+        <v>4648</v>
+      </c>
+      <c r="B4175" s="0" t="inlineStr">
+        <is>
+          <t>Jimenez, Kayla (2024/09/08/). Students are sweating through class without air conditioning. Districts are facing the heat. University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4176" spans="1:2">
+      <c r="A4176" s="0">
+        <v>4649</v>
+      </c>
+      <c r="B4176" s="0" t="inlineStr">
+        <is>
+          <t>Kearney, Grace (2024/09/07/). Managing a School-Life Balance University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4177" spans="1:2">
+      <c r="A4177" s="0">
+        <v>4650</v>
+      </c>
+      <c r="B4177" s="0" t="inlineStr">
+        <is>
+          <t>Andrews, Elijah (2024/09/06/). Stingers lack status updates University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4178" spans="1:2">
+      <c r="A4178" s="0">
+        <v>4651</v>
+      </c>
+      <c r="B4178" s="0" t="inlineStr">
+        <is>
+          <t>Shackelford, Landon, The Breeze (2024/09/05/). JMU partners with new laundry service | News | breezejmu.org University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4179" spans="1:2">
+      <c r="A4179" s="0">
+        <v>4652</v>
+      </c>
+      <c r="B4179" s="0" t="inlineStr">
+        <is>
+          <t> (2024/09/05/). Agenda Hero Launches New AI-Powered 2024-25 Academic Calendar Directory University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4180" spans="1:2">
+      <c r="A4180" s="0">
+        <v>4654</v>
+      </c>
+      <c r="B4180" s="0" t="inlineStr">
+        <is>
+          <t>Farquharson, Michael (2024/09/04/). Farquharson: The Class Withdrawal System Needs Reform - The Dartmouth University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4181" spans="1:2">
+      <c r="A4181" s="0">
+        <v>4655</v>
+      </c>
+      <c r="B4181" s="0" t="inlineStr">
+        <is>
+          <t>Skiba, Katarzyna (2024/09/03/). The "Four-Day School Week" Experiments Are Multiplying Around The World Worldcrunch, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4182" spans="1:2">
+      <c r="A4182" s="0">
+        <v>4656</v>
+      </c>
+      <c r="B4182" s="0" t="inlineStr">
+        <is>
+          <t>Brooker, Jena, BridgeDetroit, Worth, Katie, Climate Central (2024/08/31/). Chalkbeat: More Detroit school closures expected with extreme heat Chalkbeat, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4183" spans="1:2">
+      <c r="A4183" s="0">
+        <v>4657</v>
+      </c>
+      <c r="B4183" s="0" t="inlineStr">
+        <is>
+          <t>Carrera, Catherine (2024/08/27/). Chalkbeat: Newark charters kick off 2024-25 school year with larger tutoring fleet, focus on academic recovery Chalkbeat, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4184" spans="1:2">
+      <c r="A4184" s="0">
+        <v>4658</v>
+      </c>
+      <c r="B4184" s="0" t="inlineStr">
+        <is>
+          <t> (2024/08/27/). “We’re Still Here”: UConnDivest holds first Gaza solidarity conference of the academic year  | The Daily Campus University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4185" spans="1:2">
+      <c r="A4185" s="0">
+        <v>4659</v>
+      </c>
+      <c r="B4185" s="0" t="inlineStr">
+        <is>
+          <t>Evans, Libby (2024/08/22/). Sororities prepare for an exciting, more relaxed recruitment University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4186" spans="1:2">
+      <c r="A4186" s="0">
+        <v>4660</v>
+      </c>
+      <c r="B4186" s="0" t="inlineStr">
+        <is>
+          <t>DeLetter, Emily (2024/08/20/). When is the first day of fall? What to know about the start of the autumnal season University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4187" spans="1:2">
+      <c r="A4187" s="0">
+        <v>4661</v>
+      </c>
+      <c r="B4187" s="0" t="inlineStr">
+        <is>
+          <t>Kiviat, Matthew (2024/08/18/). BREAKING: Cornell Workers to Strike After Failed Negotiations with the University University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4188" spans="1:2">
+      <c r="A4188" s="0">
+        <v>4662</v>
+      </c>
+      <c r="B4188" s="0" t="inlineStr">
+        <is>
+          <t>Kiviat, Matthew (2024/08/16/). 'When We Fight, We Win': Cornell's UAW Chapter Rallies Following Successful Strike Authorization Vote University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4189" spans="1:2">
+      <c r="A4189" s="0">
+        <v>4663</v>
+      </c>
+      <c r="B4189" s="0" t="inlineStr">
+        <is>
+          <t> (2024/08/15/). Is it worth working part-time as a student? | Blog | dailycal.org University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4190" spans="1:2">
+      <c r="A4190" s="0">
+        <v>4664</v>
+      </c>
+      <c r="B4190" s="0" t="inlineStr">
+        <is>
+          <t>Mueller, Joe (2024/08/14/). Report: Colorado must review academic, overall performance of 4-day school week CE Think Tank Newswire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4191" spans="1:2">
+      <c r="A4191" s="0">
+        <v>4665</v>
+      </c>
+      <c r="B4191" s="0" t="inlineStr">
+        <is>
+          <t>Schimke, Ann (2024/08/13/). Chalkbeat: More guardrails for Colorado districts that want 4-day weeks, report urges Chalkbeat, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4192" spans="1:2">
+      <c r="A4192" s="0">
+        <v>4666</v>
+      </c>
+      <c r="B4192" s="0" t="inlineStr">
+        <is>
+          <t>Eames, Austin (2024/08/12/). Get in the Game with Intramural Sports - Daily Chronicle University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4193" spans="1:2">
+      <c r="A4193" s="0">
+        <v>4667</v>
+      </c>
+      <c r="B4193" s="0" t="inlineStr">
+        <is>
+          <t> (2024/08/09/). Everything you Need to Know about Securing an On-Campus Job - The Daily Aztec University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4194" spans="1:2">
+      <c r="A4194" s="0">
+        <v>4668</v>
+      </c>
+      <c r="B4194" s="0" t="inlineStr">
+        <is>
+          <t> (2024/08/09/). Idaho juvenile corrections students thrive with LC State - Campus News | Lewis-Clark State user--solid open-close-angle arrow-right--line arrow-right--line arrow-right--line arrow-right--line arrow-right--line arrow-right--line arrow-right--line arrow-rig University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4195" spans="1:2">
+      <c r="A4195" s="0">
+        <v>4669</v>
+      </c>
+      <c r="B4195" s="0" t="inlineStr">
+        <is>
+          <t>Saclarides, Evthokia, Munson, Jen (2024/08//). Forces that shape coaches' classroom access The Learning Professional, 45(4), 68. </t>
+        </is>
+      </c>
+    </row>
+    <row r="4196" spans="1:2">
+      <c r="A4196" s="0">
+        <v>4670</v>
+      </c>
+      <c r="B4196" s="0" t="inlineStr">
+        <is>
+          <t>Bertrando, Marc S (2024/08//). Scheduling 3.0: Our Playbook on Delaying School Start Times School Administrator, 81(8), 32. </t>
+        </is>
+      </c>
+    </row>
+    <row r="4197" spans="1:2">
+      <c r="A4197" s="0">
+        <v>4671</v>
+      </c>
+      <c r="B4197" s="0" t="inlineStr">
+        <is>
+          <t>Littman, Ava (2024/08/01/). A glimpse into OIT's emergency response to the CrowdStrike outage University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4198" spans="1:2">
+      <c r="A4198" s="0">
+        <v>4672</v>
+      </c>
+      <c r="B4198" s="0" t="inlineStr">
+        <is>
+          <t>Kristin O'Donnell Tubb (2024/08//). Ace Author Visits: Tips To Get The Most Of Events School Library Journal, 70(8), 17. </t>
+        </is>
+      </c>
+    </row>
+    <row r="4199" spans="1:2">
+      <c r="A4199" s="0">
+        <v>4673</v>
+      </c>
+      <c r="B4199" s="0" t="inlineStr">
+        <is>
+          <t>Mary Walrath-Holdridge Kinsey Crowley (2024/07/29/). Sliding out of summer: Many US schools are underway as others have weeks of vacation left University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4200" spans="1:2">
+      <c r="A4200" s="0">
+        <v>4674</v>
+      </c>
+      <c r="B4200" s="0" t="inlineStr">
+        <is>
+          <t> (2024/07/24/). OU faculty contract negotiations: Workload, salary increase and special lecturer status – The Oakland Post University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4201" spans="1:2">
+      <c r="A4201" s="0">
+        <v>4675</v>
+      </c>
+      <c r="B4201" s="0" t="inlineStr">
+        <is>
+          <t>Jefferson, Angel (2024/07/22/). UTA apps help navigate campus resources, events University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4202" spans="1:2">
+      <c r="A4202" s="0">
+        <v>4676</v>
+      </c>
+      <c r="B4202" s="0" t="inlineStr">
+        <is>
+          <t>Jefferson, Angel (2024/07/22/). UTA apps make Maverick lives easier University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4203" spans="1:2">
+      <c r="A4203" s="0">
+        <v>4677</v>
+      </c>
+      <c r="B4203" s="0" t="inlineStr">
+        <is>
+          <t> (2024/07/08/). When will Tallahassee change its school start times? University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4204" spans="1:2">
+      <c r="A4204" s="0">
+        <v>4679</v>
+      </c>
+      <c r="B4204" s="0" t="inlineStr">
+        <is>
+          <t>Hall, Sarah Lindenfeld (2024/07//). Embracing the Four-Day School Week School Administrator, 81(7), 78. </t>
+        </is>
+      </c>
+    </row>
+    <row r="4205" spans="1:2">
+      <c r="A4205" s="0">
+        <v>4680</v>
+      </c>
+      <c r="B4205" s="0" t="inlineStr">
+        <is>
+          <t>Patterson, Paula (2024/07//). Why We Transitioned to a Four-Day Week School Administrator, 81(7), 81. </t>
+        </is>
+      </c>
+    </row>
+    <row r="4206" spans="1:2">
+      <c r="A4206" s="0">
+        <v>4681</v>
+      </c>
+      <c r="B4206" s="0" t="inlineStr">
+        <is>
+          <t>Smith, Wendy K, Noonan, Kieren M (2024/07//). Embracing Both/And Thinking and Actions School Administrator, 81(7), 20. </t>
+        </is>
+      </c>
+    </row>
+    <row r="4207" spans="1:2">
+      <c r="A4207" s="0">
+        <v>4682</v>
+      </c>
+      <c r="B4207" s="0" t="inlineStr">
+        <is>
+          <t>Bernstein, Karen, Hageman, Joseph R (2024/07//). Advice on Establishing Healthy Cell Phone Routines for Teenagers Pediatric Annals, 53(7), e239. https://doi.org/10.3928/19382359-20240529-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="4208" spans="1:2">
+      <c r="A4208" s="0">
+        <v>4684</v>
+      </c>
+      <c r="B4208" s="0" t="inlineStr">
+        <is>
+          <t>Hurtado, Kaitlin (2024/06/27/). How Your Babysitter Can Help Develop Your Kids' Summer Routine University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4209" spans="1:2">
+      <c r="A4209" s="0">
+        <v>4685</v>
+      </c>
+      <c r="B4209" s="0" t="inlineStr">
+        <is>
+          <t> (2024/06/26/). Her Own Place in the Sun University Wire, (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4210" spans="1:2">
+      <c r="A4210" s="0">
+        <v>4687</v>
+      </c>
+      <c r="B4210" s="0" t="inlineStr">
+        <is>
+          <t>Niceley, Shannon L. (2025). Factors that influence student learning during a week-long zoo education program. , 86(2-A), No Pagination Specified. </t>
+        </is>
+      </c>
+    </row>
+    <row r="4211" spans="1:2">
+      <c r="A4211" s="0">
+        <v>4690</v>
+      </c>
+      <c r="B4211" s="0" t="inlineStr">
+        <is>
+          <t>James V. Shuls (2023). Five for me: A survey of Missourians regarding the four-day school week , (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4212" spans="1:2">
+      <c r="A4212" s="0">
+        <v>4691</v>
+      </c>
+      <c r="B4212" s="0" t="inlineStr">
+        <is>
+          <t>Avery Frank and James V. Shuls (2024). Longer days and fewer total hours: examining the four-day school week in Missouri , (), . </t>
+        </is>
+      </c>
+    </row>
+    <row r="4213" spans="1:2">
+      <c r="A4213" s="0">
+        <v>4692</v>
+      </c>
+      <c r="B4213" s="0" t="inlineStr">
+        <is>
+          <t>Avery Frank and James V. Shuls (2023). Evidence based? A systematic literature review of the four-day school week , (), . </t>
         </is>
       </c>
     </row>

</xml_diff>